<commit_message>
Programa de auditoria actualizado segun cambios recomendados
</commit_message>
<xml_diff>
--- a/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
+++ b/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATIAS\Desktop\ESPE\Septimo_Semestre\Quality Assurance\Repo\2563_G3_ACSW\02_Proyecto\09. Programa de Auditoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9985E078-8065-48B2-AA51-F7F8986D564F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{396B89BC-956B-44FD-B2C7-B8E74777C281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. PROGRAMA" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t>Fecha de Emisión:</t>
   </si>
@@ -227,74 +227,10 @@
     <t>ISO-ICE-IEEE-29119-5</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Identifying Keywords:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Is a pivotal task in Keyword-Driven Testing as the contents, granularity and structure of the keywords can impact the way keyword test cases are defined. It is important to name keywords in a way that appears natural to the people who will be working with them.</t>
-    </r>
-  </si>
-  <si>
     <t>6.2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Composing test cases:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Keyword test cases can be created from previously defined keywords and documented using tables or databases. These cases typically use keywords from a single layer, allowing different testers to design different layers.</t>
-    </r>
-  </si>
-  <si>
     <t>6.3</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Keywords and data-driven testing:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Keyword testing with separate parameters allows reusing action sequences with different data, stored in tables or databases, thus creating new tests</t>
-    </r>
   </si>
   <si>
     <t>6.4</t>
@@ -472,13 +408,6 @@
     <t>METODOS: Observación directa, entrevistas con el equipo auditado y verificación de documentación relevante.</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Identifying keywords
-Composing test cases
-Keywords and data-driven testing
-Modularity and refactoring </t>
-  </si>
-  <si>
     <t>Seguimiento de avances
 Evaluación y revisión de la información recopilada
 Análisis de resultados preliminares
@@ -504,33 +433,6 @@
   </si>
   <si>
     <t>Cristopher Zambrano</t>
-  </si>
-  <si>
-    <t>Ricardo Lazo</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Modularity and refactoring :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Modularity in Keyword-Driven Testing is used to improve the longevity of the test cases. However, with the 
-passage of time, changes in the test item, new test cases or new people on the team can all lead to 
-maintenance issues.</t>
-    </r>
   </si>
   <si>
     <t>6.5</t>
@@ -569,6 +471,101 @@
 6.5: Modularidad y refactorización ("Modularity and Refactoring").
 Además, se realizarán reuniones con el equipo auditado para validar el cumplimiento de los objetivos establecidos y garantizar un cierre eficiente del proceso de auditoría.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Identifying Keywords(6.2):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Is a pivotal task in Keyword-Driven Testing as the contents, granularity and structure of the keywords can impact the way keyword test cases are defined. It is important to name keywords in a way that appears natural to the people who will be working with them.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Composing test cases(6.3):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Keyword test cases can be created from previously defined keywords and documented using tables or databases. These cases typically use keywords from a single layer, allowing different testers to design different layers.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Keywords and data-driven testing(6.4):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Keyword testing with separate parameters allows reusing action sequences with different data, stored in tables or databases, thus creating new tests</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Modularity and refactoring(6.5) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Modularity in Keyword-Driven Testing is used to improve the longevity of the test cases. However, with the 
+passage of time, changes in the test item, new test cases or new people on the team can all lead to 
+maintenance issues.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+6.2 Identifying keywords
+6.3 Composing test cases
+6.4 Keywords and data-driven testing
+6.5 Modularity and refactoring </t>
   </si>
 </sst>
 </file>
@@ -1527,9 +1524,6 @@
     <xf numFmtId="0" fontId="28" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1566,29 +1560,90 @@
     <xf numFmtId="167" fontId="39" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1596,18 +1651,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1624,62 +1669,14 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1957,8 +1954,8 @@
   </sheetPr>
   <dimension ref="A1:AW994"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:AB8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E11" zoomScale="64" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24:AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -1991,12 +1988,12 @@
     </row>
     <row r="2" spans="1:48" ht="42.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="136"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="137"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="118"/>
       <c r="H2" s="101"/>
       <c r="I2" s="101"/>
       <c r="J2" s="101"/>
@@ -2007,18 +2004,18 @@
       <c r="O2" s="101"/>
       <c r="P2" s="101"/>
       <c r="Q2" s="102"/>
-      <c r="R2" s="134" t="s">
+      <c r="R2" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="138"/>
-      <c r="T2" s="138"/>
-      <c r="U2" s="138"/>
-      <c r="V2" s="138"/>
+      <c r="S2" s="120"/>
+      <c r="T2" s="120"/>
+      <c r="U2" s="120"/>
+      <c r="V2" s="120"/>
       <c r="W2" s="101"/>
       <c r="X2" s="101"/>
       <c r="Y2" s="102"/>
-      <c r="Z2" s="134" t="s">
-        <v>55</v>
+      <c r="Z2" s="119" t="s">
+        <v>52</v>
       </c>
       <c r="AA2" s="101"/>
       <c r="AB2" s="102"/>
@@ -2045,12 +2042,12 @@
     </row>
     <row r="3" spans="1:48" ht="48.75" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="114"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="139"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="121"/>
       <c r="H3" s="101"/>
       <c r="I3" s="101"/>
       <c r="J3" s="101"/>
@@ -2061,18 +2058,18 @@
       <c r="O3" s="101"/>
       <c r="P3" s="101"/>
       <c r="Q3" s="102"/>
-      <c r="R3" s="132" t="s">
+      <c r="R3" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="133"/>
-      <c r="T3" s="133"/>
-      <c r="U3" s="133"/>
-      <c r="V3" s="133"/>
+      <c r="S3" s="123"/>
+      <c r="T3" s="123"/>
+      <c r="U3" s="123"/>
+      <c r="V3" s="123"/>
       <c r="W3" s="101"/>
       <c r="X3" s="101"/>
       <c r="Y3" s="102"/>
-      <c r="Z3" s="134" t="s">
-        <v>55</v>
+      <c r="Z3" s="119" t="s">
+        <v>52</v>
       </c>
       <c r="AA3" s="101"/>
       <c r="AB3" s="102"/>
@@ -2099,14 +2096,14 @@
     </row>
     <row r="4" spans="1:48" ht="21" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="124" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="101"/>
       <c r="D4" s="101"/>
       <c r="E4" s="101"/>
       <c r="F4" s="102"/>
-      <c r="G4" s="131"/>
+      <c r="G4" s="125"/>
       <c r="H4" s="101"/>
       <c r="I4" s="101"/>
       <c r="J4" s="101"/>
@@ -2117,17 +2114,17 @@
       <c r="O4" s="101"/>
       <c r="P4" s="101"/>
       <c r="Q4" s="102"/>
-      <c r="R4" s="132" t="s">
-        <v>88</v>
+      <c r="R4" s="122" t="s">
+        <v>82</v>
       </c>
-      <c r="S4" s="133"/>
-      <c r="T4" s="133"/>
-      <c r="U4" s="133"/>
-      <c r="V4" s="133"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
       <c r="W4" s="101"/>
       <c r="X4" s="101"/>
       <c r="Y4" s="102"/>
-      <c r="Z4" s="134" t="s">
+      <c r="Z4" s="119" t="s">
         <v>3</v>
       </c>
       <c r="AA4" s="101"/>
@@ -2204,35 +2201,35 @@
       <c r="AV5" s="2"/>
     </row>
     <row r="6" spans="1:48" ht="50.25" customHeight="1">
-      <c r="B6" s="135" t="s">
-        <v>69</v>
+      <c r="B6" s="126" t="s">
+        <v>66</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="108"/>
-      <c r="R6" s="108"/>
-      <c r="S6" s="108"/>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="108"/>
-      <c r="X6" s="108"/>
-      <c r="Y6" s="108"/>
-      <c r="Z6" s="108"/>
-      <c r="AA6" s="108"/>
-      <c r="AB6" s="108"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="99"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="99"/>
+      <c r="S6" s="99"/>
+      <c r="T6" s="99"/>
+      <c r="U6" s="99"/>
+      <c r="V6" s="99"/>
+      <c r="W6" s="99"/>
+      <c r="X6" s="99"/>
+      <c r="Y6" s="99"/>
+      <c r="Z6" s="99"/>
+      <c r="AA6" s="99"/>
+      <c r="AB6" s="99"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="6"/>
@@ -2249,35 +2246,35 @@
       <c r="AP6" s="7"/>
     </row>
     <row r="7" spans="1:48" ht="198" customHeight="1">
-      <c r="B7" s="107" t="s">
-        <v>89</v>
+      <c r="B7" s="133" t="s">
+        <v>83</v>
       </c>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="108"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="108"/>
-      <c r="O7" s="108"/>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="108"/>
-      <c r="R7" s="108"/>
-      <c r="S7" s="108"/>
-      <c r="T7" s="108"/>
-      <c r="U7" s="108"/>
-      <c r="V7" s="108"/>
-      <c r="W7" s="108"/>
-      <c r="X7" s="108"/>
-      <c r="Y7" s="108"/>
-      <c r="Z7" s="108"/>
-      <c r="AA7" s="108"/>
-      <c r="AB7" s="108"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="99"/>
+      <c r="N7" s="99"/>
+      <c r="O7" s="99"/>
+      <c r="P7" s="99"/>
+      <c r="Q7" s="99"/>
+      <c r="R7" s="99"/>
+      <c r="S7" s="99"/>
+      <c r="T7" s="99"/>
+      <c r="U7" s="99"/>
+      <c r="V7" s="99"/>
+      <c r="W7" s="99"/>
+      <c r="X7" s="99"/>
+      <c r="Y7" s="99"/>
+      <c r="Z7" s="99"/>
+      <c r="AA7" s="99"/>
+      <c r="AB7" s="99"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
       <c r="AE7" s="6"/>
@@ -2294,35 +2291,35 @@
       <c r="AP7" s="7"/>
     </row>
     <row r="8" spans="1:48" ht="51" customHeight="1">
-      <c r="B8" s="129" t="s">
-        <v>68</v>
+      <c r="B8" s="134" t="s">
+        <v>65</v>
       </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="108"/>
-      <c r="K8" s="108"/>
-      <c r="L8" s="108"/>
-      <c r="M8" s="108"/>
-      <c r="N8" s="108"/>
-      <c r="O8" s="108"/>
-      <c r="P8" s="108"/>
-      <c r="Q8" s="108"/>
-      <c r="R8" s="108"/>
-      <c r="S8" s="108"/>
-      <c r="T8" s="108"/>
-      <c r="U8" s="108"/>
-      <c r="V8" s="108"/>
-      <c r="W8" s="108"/>
-      <c r="X8" s="108"/>
-      <c r="Y8" s="108"/>
-      <c r="Z8" s="108"/>
-      <c r="AA8" s="108"/>
-      <c r="AB8" s="108"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="99"/>
+      <c r="N8" s="99"/>
+      <c r="O8" s="99"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="99"/>
+      <c r="R8" s="99"/>
+      <c r="S8" s="99"/>
+      <c r="T8" s="99"/>
+      <c r="U8" s="99"/>
+      <c r="V8" s="99"/>
+      <c r="W8" s="99"/>
+      <c r="X8" s="99"/>
+      <c r="Y8" s="99"/>
+      <c r="Z8" s="99"/>
+      <c r="AA8" s="99"/>
+      <c r="AB8" s="99"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="6"/>
@@ -2382,35 +2379,35 @@
       <c r="AP9" s="7"/>
     </row>
     <row r="10" spans="1:48" ht="20.25" customHeight="1">
-      <c r="B10" s="129" t="s">
-        <v>56</v>
+      <c r="B10" s="134" t="s">
+        <v>53</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="108"/>
-      <c r="K10" s="108"/>
-      <c r="L10" s="108"/>
-      <c r="M10" s="108"/>
-      <c r="N10" s="108"/>
-      <c r="O10" s="108"/>
-      <c r="P10" s="108"/>
-      <c r="Q10" s="108"/>
-      <c r="R10" s="108"/>
-      <c r="S10" s="108"/>
-      <c r="T10" s="108"/>
-      <c r="U10" s="108"/>
-      <c r="V10" s="108"/>
-      <c r="W10" s="108"/>
-      <c r="X10" s="108"/>
-      <c r="Y10" s="108"/>
-      <c r="Z10" s="108"/>
-      <c r="AA10" s="108"/>
-      <c r="AB10" s="108"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="99"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="99"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="99"/>
+      <c r="N10" s="99"/>
+      <c r="O10" s="99"/>
+      <c r="P10" s="99"/>
+      <c r="Q10" s="99"/>
+      <c r="R10" s="99"/>
+      <c r="S10" s="99"/>
+      <c r="T10" s="99"/>
+      <c r="U10" s="99"/>
+      <c r="V10" s="99"/>
+      <c r="W10" s="99"/>
+      <c r="X10" s="99"/>
+      <c r="Y10" s="99"/>
+      <c r="Z10" s="99"/>
+      <c r="AA10" s="99"/>
+      <c r="AB10" s="99"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="6"/>
@@ -2428,35 +2425,35 @@
     </row>
     <row r="11" spans="1:48" ht="60" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="107" t="s">
-        <v>70</v>
+      <c r="B11" s="133" t="s">
+        <v>67</v>
       </c>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="108"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="108"/>
-      <c r="L11" s="108"/>
-      <c r="M11" s="108"/>
-      <c r="N11" s="108"/>
-      <c r="O11" s="108"/>
-      <c r="P11" s="108"/>
-      <c r="Q11" s="108"/>
-      <c r="R11" s="108"/>
-      <c r="S11" s="108"/>
-      <c r="T11" s="108"/>
-      <c r="U11" s="108"/>
-      <c r="V11" s="108"/>
-      <c r="W11" s="108"/>
-      <c r="X11" s="108"/>
-      <c r="Y11" s="108"/>
-      <c r="Z11" s="108"/>
-      <c r="AA11" s="108"/>
-      <c r="AB11" s="108"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="99"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="99"/>
+      <c r="M11" s="99"/>
+      <c r="N11" s="99"/>
+      <c r="O11" s="99"/>
+      <c r="P11" s="99"/>
+      <c r="Q11" s="99"/>
+      <c r="R11" s="99"/>
+      <c r="S11" s="99"/>
+      <c r="T11" s="99"/>
+      <c r="U11" s="99"/>
+      <c r="V11" s="99"/>
+      <c r="W11" s="99"/>
+      <c r="X11" s="99"/>
+      <c r="Y11" s="99"/>
+      <c r="Z11" s="99"/>
+      <c r="AA11" s="99"/>
+      <c r="AB11" s="99"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="9"/>
       <c r="AE11" s="9"/>
@@ -2479,35 +2476,35 @@
       <c r="AV11" s="8"/>
     </row>
     <row r="12" spans="1:48" ht="53.25" customHeight="1">
-      <c r="B12" s="107" t="s">
-        <v>71</v>
+      <c r="B12" s="133" t="s">
+        <v>68</v>
       </c>
-      <c r="C12" s="108"/>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="108"/>
-      <c r="K12" s="108"/>
-      <c r="L12" s="108"/>
-      <c r="M12" s="108"/>
-      <c r="N12" s="108"/>
-      <c r="O12" s="108"/>
-      <c r="P12" s="108"/>
-      <c r="Q12" s="108"/>
-      <c r="R12" s="108"/>
-      <c r="S12" s="108"/>
-      <c r="T12" s="108"/>
-      <c r="U12" s="108"/>
-      <c r="V12" s="108"/>
-      <c r="W12" s="108"/>
-      <c r="X12" s="108"/>
-      <c r="Y12" s="108"/>
-      <c r="Z12" s="108"/>
-      <c r="AA12" s="108"/>
-      <c r="AB12" s="108"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="99"/>
+      <c r="F12" s="99"/>
+      <c r="G12" s="99"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="99"/>
+      <c r="J12" s="99"/>
+      <c r="K12" s="99"/>
+      <c r="L12" s="99"/>
+      <c r="M12" s="99"/>
+      <c r="N12" s="99"/>
+      <c r="O12" s="99"/>
+      <c r="P12" s="99"/>
+      <c r="Q12" s="99"/>
+      <c r="R12" s="99"/>
+      <c r="S12" s="99"/>
+      <c r="T12" s="99"/>
+      <c r="U12" s="99"/>
+      <c r="V12" s="99"/>
+      <c r="W12" s="99"/>
+      <c r="X12" s="99"/>
+      <c r="Y12" s="99"/>
+      <c r="Z12" s="99"/>
+      <c r="AA12" s="99"/>
+      <c r="AB12" s="99"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
@@ -2524,35 +2521,35 @@
       <c r="AP12" s="7"/>
     </row>
     <row r="13" spans="1:48" ht="39.75" customHeight="1">
-      <c r="B13" s="107" t="s">
-        <v>72</v>
+      <c r="B13" s="133" t="s">
+        <v>69</v>
       </c>
-      <c r="C13" s="108"/>
-      <c r="D13" s="108"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="108"/>
-      <c r="G13" s="108"/>
-      <c r="H13" s="108"/>
-      <c r="I13" s="108"/>
-      <c r="J13" s="108"/>
-      <c r="K13" s="108"/>
-      <c r="L13" s="108"/>
-      <c r="M13" s="108"/>
-      <c r="N13" s="108"/>
-      <c r="O13" s="108"/>
-      <c r="P13" s="108"/>
-      <c r="Q13" s="108"/>
-      <c r="R13" s="108"/>
-      <c r="S13" s="108"/>
-      <c r="T13" s="108"/>
-      <c r="U13" s="108"/>
-      <c r="V13" s="108"/>
-      <c r="W13" s="108"/>
-      <c r="X13" s="108"/>
-      <c r="Y13" s="108"/>
-      <c r="Z13" s="108"/>
-      <c r="AA13" s="108"/>
-      <c r="AB13" s="108"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="99"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="99"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="99"/>
+      <c r="O13" s="99"/>
+      <c r="P13" s="99"/>
+      <c r="Q13" s="99"/>
+      <c r="R13" s="99"/>
+      <c r="S13" s="99"/>
+      <c r="T13" s="99"/>
+      <c r="U13" s="99"/>
+      <c r="V13" s="99"/>
+      <c r="W13" s="99"/>
+      <c r="X13" s="99"/>
+      <c r="Y13" s="99"/>
+      <c r="Z13" s="99"/>
+      <c r="AA13" s="99"/>
+      <c r="AB13" s="99"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
@@ -2612,35 +2609,35 @@
       <c r="AP14" s="7"/>
     </row>
     <row r="15" spans="1:48" ht="99.75" customHeight="1">
-      <c r="B15" s="109" t="s">
-        <v>73</v>
+      <c r="B15" s="135" t="s">
+        <v>70</v>
       </c>
-      <c r="C15" s="108"/>
-      <c r="D15" s="108"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="108"/>
-      <c r="K15" s="108"/>
-      <c r="L15" s="108"/>
-      <c r="M15" s="108"/>
-      <c r="N15" s="108"/>
-      <c r="O15" s="108"/>
-      <c r="P15" s="108"/>
-      <c r="Q15" s="108"/>
-      <c r="R15" s="108"/>
-      <c r="S15" s="108"/>
-      <c r="T15" s="108"/>
-      <c r="U15" s="108"/>
-      <c r="V15" s="108"/>
-      <c r="W15" s="108"/>
-      <c r="X15" s="108"/>
-      <c r="Y15" s="108"/>
-      <c r="Z15" s="108"/>
-      <c r="AA15" s="108"/>
-      <c r="AB15" s="108"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="99"/>
+      <c r="P15" s="99"/>
+      <c r="Q15" s="99"/>
+      <c r="R15" s="99"/>
+      <c r="S15" s="99"/>
+      <c r="T15" s="99"/>
+      <c r="U15" s="99"/>
+      <c r="V15" s="99"/>
+      <c r="W15" s="99"/>
+      <c r="X15" s="99"/>
+      <c r="Y15" s="99"/>
+      <c r="Z15" s="99"/>
+      <c r="AA15" s="99"/>
+      <c r="AB15" s="99"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="6"/>
@@ -2658,35 +2655,35 @@
     </row>
     <row r="16" spans="1:48" ht="24.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="110" t="s">
-        <v>74</v>
+      <c r="B16" s="136" t="s">
+        <v>71</v>
       </c>
-      <c r="C16" s="108"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="108"/>
-      <c r="G16" s="108"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
-      <c r="K16" s="108"/>
-      <c r="L16" s="108"/>
-      <c r="M16" s="108"/>
-      <c r="N16" s="108"/>
-      <c r="O16" s="108"/>
-      <c r="P16" s="108"/>
-      <c r="Q16" s="108"/>
-      <c r="R16" s="108"/>
-      <c r="S16" s="108"/>
-      <c r="T16" s="108"/>
-      <c r="U16" s="108"/>
-      <c r="V16" s="108"/>
-      <c r="W16" s="108"/>
-      <c r="X16" s="108"/>
-      <c r="Y16" s="108"/>
-      <c r="Z16" s="108"/>
-      <c r="AA16" s="108"/>
-      <c r="AB16" s="108"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="99"/>
+      <c r="H16" s="99"/>
+      <c r="I16" s="99"/>
+      <c r="J16" s="99"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="99"/>
+      <c r="M16" s="99"/>
+      <c r="N16" s="99"/>
+      <c r="O16" s="99"/>
+      <c r="P16" s="99"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="99"/>
+      <c r="S16" s="99"/>
+      <c r="T16" s="99"/>
+      <c r="U16" s="99"/>
+      <c r="V16" s="99"/>
+      <c r="W16" s="99"/>
+      <c r="X16" s="99"/>
+      <c r="Y16" s="99"/>
+      <c r="Z16" s="99"/>
+      <c r="AA16" s="99"/>
+      <c r="AB16" s="99"/>
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
@@ -2709,35 +2706,35 @@
       <c r="AV16" s="2"/>
     </row>
     <row r="17" spans="1:49" ht="24.75" customHeight="1">
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="108"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="108"/>
-      <c r="J17" s="108"/>
-      <c r="K17" s="108"/>
-      <c r="L17" s="108"/>
-      <c r="M17" s="108"/>
-      <c r="N17" s="108"/>
-      <c r="O17" s="108"/>
-      <c r="P17" s="108"/>
-      <c r="Q17" s="108"/>
-      <c r="R17" s="108"/>
-      <c r="S17" s="108"/>
-      <c r="T17" s="108"/>
-      <c r="U17" s="108"/>
-      <c r="V17" s="108"/>
-      <c r="W17" s="108"/>
-      <c r="X17" s="108"/>
-      <c r="Y17" s="108"/>
-      <c r="Z17" s="108"/>
-      <c r="AA17" s="108"/>
-      <c r="AB17" s="108"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
+      <c r="G17" s="99"/>
+      <c r="H17" s="99"/>
+      <c r="I17" s="99"/>
+      <c r="J17" s="99"/>
+      <c r="K17" s="99"/>
+      <c r="L17" s="99"/>
+      <c r="M17" s="99"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="99"/>
+      <c r="P17" s="99"/>
+      <c r="Q17" s="99"/>
+      <c r="R17" s="99"/>
+      <c r="S17" s="99"/>
+      <c r="T17" s="99"/>
+      <c r="U17" s="99"/>
+      <c r="V17" s="99"/>
+      <c r="W17" s="99"/>
+      <c r="X17" s="99"/>
+      <c r="Y17" s="99"/>
+      <c r="Z17" s="99"/>
+      <c r="AA17" s="99"/>
+      <c r="AB17" s="99"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="6"/>
@@ -2754,33 +2751,33 @@
       <c r="AP17" s="7"/>
     </row>
     <row r="18" spans="1:49" ht="6.75" customHeight="1">
-      <c r="B18" s="109"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="108"/>
-      <c r="K18" s="108"/>
-      <c r="L18" s="108"/>
-      <c r="M18" s="108"/>
-      <c r="N18" s="108"/>
-      <c r="O18" s="108"/>
-      <c r="P18" s="108"/>
-      <c r="Q18" s="108"/>
-      <c r="R18" s="108"/>
-      <c r="S18" s="108"/>
-      <c r="T18" s="108"/>
-      <c r="U18" s="108"/>
-      <c r="V18" s="108"/>
-      <c r="W18" s="108"/>
-      <c r="X18" s="108"/>
-      <c r="Y18" s="108"/>
-      <c r="Z18" s="108"/>
-      <c r="AA18" s="108"/>
-      <c r="AB18" s="108"/>
+      <c r="B18" s="135"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="99"/>
+      <c r="G18" s="99"/>
+      <c r="H18" s="99"/>
+      <c r="I18" s="99"/>
+      <c r="J18" s="99"/>
+      <c r="K18" s="99"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="99"/>
+      <c r="N18" s="99"/>
+      <c r="O18" s="99"/>
+      <c r="P18" s="99"/>
+      <c r="Q18" s="99"/>
+      <c r="R18" s="99"/>
+      <c r="S18" s="99"/>
+      <c r="T18" s="99"/>
+      <c r="U18" s="99"/>
+      <c r="V18" s="99"/>
+      <c r="W18" s="99"/>
+      <c r="X18" s="99"/>
+      <c r="Y18" s="99"/>
+      <c r="Z18" s="99"/>
+      <c r="AA18" s="99"/>
+      <c r="AB18" s="99"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
@@ -2796,47 +2793,47 @@
       <c r="AO18" s="6"/>
       <c r="AP18" s="7"/>
     </row>
-    <row r="19" spans="1:49" ht="10.5" customHeight="1">
+    <row r="19" spans="1:49" ht="36.75" customHeight="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="139" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="124" t="s">
+      <c r="C19" s="142" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="112"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="125" t="s">
+      <c r="D19" s="128"/>
+      <c r="E19" s="129"/>
+      <c r="F19" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="111" t="s">
-        <v>57</v>
+      <c r="G19" s="127" t="s">
+        <v>54</v>
       </c>
-      <c r="H19" s="112"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="112"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="112"/>
-      <c r="M19" s="112"/>
-      <c r="N19" s="113"/>
-      <c r="O19" s="111" t="s">
-        <v>58</v>
+      <c r="H19" s="128"/>
+      <c r="I19" s="128"/>
+      <c r="J19" s="128"/>
+      <c r="K19" s="128"/>
+      <c r="L19" s="128"/>
+      <c r="M19" s="128"/>
+      <c r="N19" s="129"/>
+      <c r="O19" s="127" t="s">
+        <v>55</v>
       </c>
-      <c r="P19" s="112"/>
-      <c r="Q19" s="112"/>
-      <c r="R19" s="112"/>
-      <c r="S19" s="112"/>
-      <c r="T19" s="112"/>
-      <c r="U19" s="112"/>
-      <c r="V19" s="112"/>
-      <c r="W19" s="113"/>
-      <c r="X19" s="117" t="s">
+      <c r="P19" s="128"/>
+      <c r="Q19" s="128"/>
+      <c r="R19" s="128"/>
+      <c r="S19" s="128"/>
+      <c r="T19" s="128"/>
+      <c r="U19" s="128"/>
+      <c r="V19" s="128"/>
+      <c r="W19" s="129"/>
+      <c r="X19" s="137" t="s">
         <v>8</v>
       </c>
-      <c r="Y19" s="112"/>
-      <c r="Z19" s="112"/>
-      <c r="AA19" s="113"/>
-      <c r="AB19" s="85" t="s">
+      <c r="Y19" s="128"/>
+      <c r="Z19" s="128"/>
+      <c r="AA19" s="129"/>
+      <c r="AB19" s="84" t="s">
         <v>9</v>
       </c>
       <c r="AC19" s="14"/>
@@ -2862,33 +2859,33 @@
     </row>
     <row r="20" spans="1:49" ht="10.5" customHeight="1">
       <c r="A20" s="14"/>
-      <c r="B20" s="122"/>
-      <c r="C20" s="118"/>
-      <c r="D20" s="108"/>
-      <c r="E20" s="119"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="114"/>
-      <c r="H20" s="115"/>
-      <c r="I20" s="115"/>
-      <c r="J20" s="115"/>
-      <c r="K20" s="115"/>
-      <c r="L20" s="115"/>
-      <c r="M20" s="115"/>
-      <c r="N20" s="116"/>
-      <c r="O20" s="118"/>
-      <c r="P20" s="128"/>
-      <c r="Q20" s="128"/>
-      <c r="R20" s="128"/>
-      <c r="S20" s="128"/>
-      <c r="T20" s="128"/>
-      <c r="U20" s="128"/>
-      <c r="V20" s="128"/>
-      <c r="W20" s="119"/>
-      <c r="X20" s="118"/>
-      <c r="Y20" s="108"/>
-      <c r="Z20" s="108"/>
-      <c r="AA20" s="119"/>
-      <c r="AB20" s="86"/>
+      <c r="B20" s="140"/>
+      <c r="C20" s="130"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="132"/>
+      <c r="F20" s="144"/>
+      <c r="G20" s="116"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="108"/>
+      <c r="J20" s="108"/>
+      <c r="K20" s="108"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="108"/>
+      <c r="N20" s="117"/>
+      <c r="O20" s="130"/>
+      <c r="P20" s="131"/>
+      <c r="Q20" s="131"/>
+      <c r="R20" s="131"/>
+      <c r="S20" s="131"/>
+      <c r="T20" s="131"/>
+      <c r="U20" s="131"/>
+      <c r="V20" s="131"/>
+      <c r="W20" s="132"/>
+      <c r="X20" s="130"/>
+      <c r="Y20" s="99"/>
+      <c r="Z20" s="99"/>
+      <c r="AA20" s="132"/>
+      <c r="AB20" s="85"/>
       <c r="AC20" s="14"/>
       <c r="AD20" s="14"/>
       <c r="AE20" s="14"/>
@@ -2912,49 +2909,49 @@
     </row>
     <row r="21" spans="1:49" ht="34.5" customHeight="1">
       <c r="A21" s="15"/>
-      <c r="B21" s="122"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="119"/>
-      <c r="F21" s="126"/>
-      <c r="G21" s="120" t="s">
+      <c r="B21" s="140"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="132"/>
+      <c r="F21" s="144"/>
+      <c r="G21" s="138" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="102"/>
-      <c r="I21" s="120" t="s">
+      <c r="I21" s="138" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="102"/>
-      <c r="K21" s="120" t="s">
+      <c r="K21" s="138" t="s">
         <v>12</v>
       </c>
       <c r="L21" s="102"/>
-      <c r="M21" s="120" t="s">
+      <c r="M21" s="138" t="s">
         <v>13</v>
       </c>
       <c r="N21" s="101"/>
-      <c r="O21" s="99" t="s">
+      <c r="O21" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="P21" s="99"/>
-      <c r="Q21" s="99"/>
-      <c r="R21" s="99"/>
-      <c r="S21" s="98" t="s">
+      <c r="P21" s="147"/>
+      <c r="Q21" s="147"/>
+      <c r="R21" s="147"/>
+      <c r="S21" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="T21" s="99"/>
-      <c r="U21" s="93" t="s">
+      <c r="T21" s="147"/>
+      <c r="U21" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="V21" s="93" t="s">
+      <c r="V21" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="W21" s="89"/>
-      <c r="X21" s="115"/>
-      <c r="Y21" s="115"/>
-      <c r="Z21" s="115"/>
-      <c r="AA21" s="116"/>
-      <c r="AB21" s="86"/>
+      <c r="W21" s="88"/>
+      <c r="X21" s="108"/>
+      <c r="Y21" s="108"/>
+      <c r="Z21" s="108"/>
+      <c r="AA21" s="117"/>
+      <c r="AB21" s="85"/>
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
       <c r="AE21" s="15"/>
@@ -2978,15 +2975,15 @@
     </row>
     <row r="22" spans="1:49" ht="38.25" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="123"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="115"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="127"/>
+      <c r="B22" s="141"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="145"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J22" s="16" t="s">
         <v>14</v>
@@ -3000,40 +2997,40 @@
       <c r="M22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="N22" s="84" t="s">
+      <c r="N22" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="O22" s="92" t="s">
+      <c r="O22" s="91" t="s">
+        <v>57</v>
+      </c>
+      <c r="P22" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q22" s="95">
+      <c r="Q22" s="94">
         <v>10</v>
       </c>
-      <c r="R22" s="95">
+      <c r="R22" s="94">
         <v>11</v>
       </c>
-      <c r="S22" s="90" t="s">
-        <v>64</v>
+      <c r="S22" s="89" t="s">
+        <v>61</v>
       </c>
-      <c r="T22" s="88" t="s">
-        <v>65</v>
+      <c r="T22" s="87" t="s">
+        <v>62</v>
       </c>
-      <c r="U22" s="88" t="s">
-        <v>77</v>
+      <c r="U22" s="87" t="s">
+        <v>73</v>
       </c>
-      <c r="V22" s="88" t="s">
-        <v>78</v>
+      <c r="V22" s="87" t="s">
+        <v>74</v>
       </c>
-      <c r="W22" s="88"/>
-      <c r="X22" s="88"/>
-      <c r="Y22" s="100"/>
+      <c r="W22" s="87"/>
+      <c r="X22" s="87"/>
+      <c r="Y22" s="148"/>
       <c r="Z22" s="101"/>
       <c r="AA22" s="101"/>
       <c r="AB22" s="102"/>
-      <c r="AC22" s="87"/>
+      <c r="AC22" s="86"/>
       <c r="AD22" s="14"/>
       <c r="AE22" s="14"/>
       <c r="AF22" s="14"/>
@@ -3060,11 +3057,11 @@
       <c r="B23" s="18">
         <v>1</v>
       </c>
-      <c r="C23" s="103" t="s">
+      <c r="C23" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="104"/>
-      <c r="E23" s="105"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="110"/>
       <c r="F23" s="76">
         <v>1</v>
       </c>
@@ -3078,23 +3075,23 @@
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
-      <c r="O23" s="91"/>
-      <c r="P23" s="91"/>
-      <c r="Q23" s="91"/>
-      <c r="R23" s="94"/>
+      <c r="O23" s="90"/>
+      <c r="P23" s="90"/>
+      <c r="Q23" s="90"/>
+      <c r="R23" s="93"/>
       <c r="S23" s="22"/>
       <c r="T23" s="22"/>
       <c r="U23" s="22"/>
       <c r="V23" s="22"/>
       <c r="W23" s="22"/>
-      <c r="X23" s="106" t="s">
-        <v>61</v>
+      <c r="X23" s="100" t="s">
+        <v>58</v>
       </c>
       <c r="Y23" s="101"/>
       <c r="Z23" s="101"/>
       <c r="AA23" s="102"/>
       <c r="AB23" s="23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AC23" s="17"/>
       <c r="AD23" s="17"/>
@@ -3122,11 +3119,11 @@
       <c r="B24" s="18">
         <v>2</v>
       </c>
-      <c r="C24" s="103" t="s">
+      <c r="C24" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="104"/>
-      <c r="E24" s="105"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="110"/>
       <c r="F24" s="76">
         <v>2</v>
       </c>
@@ -3155,14 +3152,14 @@
       <c r="U24" s="22"/>
       <c r="V24" s="22"/>
       <c r="W24" s="22"/>
-      <c r="X24" s="106" t="s">
-        <v>75</v>
+      <c r="X24" s="100" t="s">
+        <v>88</v>
       </c>
       <c r="Y24" s="101"/>
       <c r="Z24" s="101"/>
       <c r="AA24" s="102"/>
       <c r="AB24" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AC24" s="17"/>
       <c r="AD24" s="17"/>
@@ -3190,11 +3187,11 @@
       <c r="B25" s="18">
         <v>3</v>
       </c>
-      <c r="C25" s="103" t="s">
+      <c r="C25" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="104"/>
-      <c r="E25" s="105"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="110"/>
       <c r="F25" s="76">
         <v>3</v>
       </c>
@@ -3219,14 +3216,14 @@
       <c r="U25" s="22"/>
       <c r="V25" s="22"/>
       <c r="W25" s="22"/>
-      <c r="X25" s="106" t="s">
-        <v>76</v>
+      <c r="X25" s="100" t="s">
+        <v>72</v>
       </c>
       <c r="Y25" s="101"/>
       <c r="Z25" s="101"/>
       <c r="AA25" s="102"/>
       <c r="AB25" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AC25" s="17"/>
       <c r="AD25" s="17"/>
@@ -3254,11 +3251,11 @@
       <c r="B26" s="18">
         <v>4</v>
       </c>
-      <c r="C26" s="103" t="s">
+      <c r="C26" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="104"/>
-      <c r="E26" s="105"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="110"/>
       <c r="F26" s="76">
         <v>4</v>
       </c>
@@ -3281,14 +3278,14 @@
       </c>
       <c r="V26" s="22"/>
       <c r="W26" s="22"/>
-      <c r="X26" s="106" t="s">
+      <c r="X26" s="100" t="s">
         <v>24</v>
       </c>
       <c r="Y26" s="101"/>
       <c r="Z26" s="101"/>
       <c r="AA26" s="102"/>
       <c r="AB26" s="23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AC26" s="17"/>
       <c r="AD26" s="17"/>
@@ -3316,11 +3313,11 @@
       <c r="B27" s="18">
         <v>5</v>
       </c>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="104"/>
-      <c r="E27" s="105"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="110"/>
       <c r="F27" s="81">
         <v>5</v>
       </c>
@@ -3343,14 +3340,14 @@
         <v>20</v>
       </c>
       <c r="W27" s="22"/>
-      <c r="X27" s="106" t="s">
+      <c r="X27" s="100" t="s">
         <v>26</v>
       </c>
       <c r="Y27" s="101"/>
       <c r="Z27" s="101"/>
       <c r="AA27" s="102"/>
       <c r="AB27" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AC27" s="17"/>
       <c r="AD27" s="17"/>
@@ -3376,9 +3373,9 @@
     <row r="28" spans="1:49" ht="163.5" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="104"/>
-      <c r="E28" s="105"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="106"/>
+      <c r="E28" s="110"/>
       <c r="F28" s="82"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
@@ -3397,7 +3394,7 @@
       <c r="U28" s="22"/>
       <c r="V28" s="22"/>
       <c r="W28" s="22"/>
-      <c r="X28" s="106" t="s">
+      <c r="X28" s="100" t="s">
         <v>27</v>
       </c>
       <c r="Y28" s="101"/>
@@ -3428,9 +3425,9 @@
     <row r="29" spans="1:49" ht="209.25" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
-      <c r="C29" s="103"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="105"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="110"/>
       <c r="F29" s="19"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
@@ -3449,7 +3446,7 @@
       <c r="U29" s="22"/>
       <c r="V29" s="22"/>
       <c r="W29" s="22"/>
-      <c r="X29" s="106"/>
+      <c r="X29" s="100"/>
       <c r="Y29" s="101"/>
       <c r="Z29" s="101"/>
       <c r="AA29" s="102"/>
@@ -3478,9 +3475,9 @@
     <row r="30" spans="1:49" ht="262.5" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
-      <c r="C30" s="103"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="105"/>
+      <c r="C30" s="109"/>
+      <c r="D30" s="106"/>
+      <c r="E30" s="110"/>
       <c r="F30" s="19"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -3499,7 +3496,7 @@
       <c r="U30" s="22"/>
       <c r="V30" s="22"/>
       <c r="W30" s="22"/>
-      <c r="X30" s="106"/>
+      <c r="X30" s="100"/>
       <c r="Y30" s="101"/>
       <c r="Z30" s="101"/>
       <c r="AA30" s="102"/>
@@ -3528,9 +3525,9 @@
     <row r="31" spans="1:49" ht="90.75" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
-      <c r="C31" s="142"/>
-      <c r="D31" s="104"/>
-      <c r="E31" s="105"/>
+      <c r="C31" s="111"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="110"/>
       <c r="F31" s="19"/>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
@@ -3549,7 +3546,7 @@
       <c r="U31" s="22"/>
       <c r="V31" s="22"/>
       <c r="W31" s="22"/>
-      <c r="X31" s="144"/>
+      <c r="X31" s="103"/>
       <c r="Y31" s="101"/>
       <c r="Z31" s="101"/>
       <c r="AA31" s="102"/>
@@ -3578,7 +3575,7 @@
     <row r="32" spans="1:49" ht="90.75" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
-      <c r="C32" s="143"/>
+      <c r="C32" s="112"/>
       <c r="D32" s="101"/>
       <c r="E32" s="102"/>
       <c r="F32" s="19"/>
@@ -3599,7 +3596,7 @@
       <c r="U32" s="22"/>
       <c r="V32" s="22"/>
       <c r="W32" s="22"/>
-      <c r="X32" s="144"/>
+      <c r="X32" s="103"/>
       <c r="Y32" s="101"/>
       <c r="Z32" s="101"/>
       <c r="AA32" s="102"/>
@@ -3649,10 +3646,10 @@
       <c r="U33" s="29"/>
       <c r="V33" s="29"/>
       <c r="W33" s="29"/>
-      <c r="X33" s="148"/>
-      <c r="Y33" s="108"/>
-      <c r="Z33" s="108"/>
-      <c r="AA33" s="108"/>
+      <c r="X33" s="104"/>
+      <c r="Y33" s="99"/>
+      <c r="Z33" s="99"/>
+      <c r="AA33" s="99"/>
       <c r="AB33" s="30"/>
     </row>
     <row r="34" spans="1:29" ht="12.75" customHeight="1">
@@ -3679,10 +3676,10 @@
       <c r="U34" s="29"/>
       <c r="V34" s="29"/>
       <c r="W34" s="29"/>
-      <c r="X34" s="148"/>
-      <c r="Y34" s="108"/>
-      <c r="Z34" s="108"/>
-      <c r="AA34" s="108"/>
+      <c r="X34" s="104"/>
+      <c r="Y34" s="99"/>
+      <c r="Z34" s="99"/>
+      <c r="AA34" s="99"/>
       <c r="AB34" s="30"/>
     </row>
     <row r="35" spans="1:29" ht="19.5" customHeight="1">
@@ -3700,10 +3697,10 @@
       <c r="J35" s="17"/>
       <c r="O35" s="38"/>
       <c r="P35" s="38"/>
-      <c r="X35" s="147"/>
-      <c r="Y35" s="108"/>
-      <c r="Z35" s="108"/>
-      <c r="AA35" s="108"/>
+      <c r="X35" s="98"/>
+      <c r="Y35" s="99"/>
+      <c r="Z35" s="99"/>
+      <c r="AA35" s="99"/>
       <c r="AB35" s="26"/>
     </row>
     <row r="36" spans="1:29" ht="18.75" customHeight="1">
@@ -3816,34 +3813,34 @@
     <row r="40" spans="1:29" ht="39.75" customHeight="1">
       <c r="A40" s="26"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="145" t="s">
+      <c r="C40" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="108"/>
-      <c r="E40" s="108"/>
-      <c r="F40" s="108"/>
-      <c r="G40" s="108"/>
-      <c r="H40" s="108"/>
-      <c r="I40" s="108"/>
-      <c r="J40" s="108"/>
-      <c r="K40" s="108"/>
-      <c r="L40" s="108"/>
-      <c r="M40" s="108"/>
-      <c r="N40" s="108"/>
-      <c r="O40" s="108"/>
-      <c r="P40" s="108"/>
-      <c r="Q40" s="108"/>
-      <c r="R40" s="108"/>
-      <c r="S40" s="108"/>
-      <c r="T40" s="108"/>
-      <c r="U40" s="108"/>
-      <c r="V40" s="108"/>
-      <c r="W40" s="108"/>
-      <c r="X40" s="108"/>
-      <c r="Y40" s="108"/>
-      <c r="Z40" s="108"/>
-      <c r="AA40" s="108"/>
-      <c r="AB40" s="146"/>
+      <c r="D40" s="99"/>
+      <c r="E40" s="99"/>
+      <c r="F40" s="99"/>
+      <c r="G40" s="99"/>
+      <c r="H40" s="99"/>
+      <c r="I40" s="99"/>
+      <c r="J40" s="99"/>
+      <c r="K40" s="99"/>
+      <c r="L40" s="99"/>
+      <c r="M40" s="99"/>
+      <c r="N40" s="99"/>
+      <c r="O40" s="99"/>
+      <c r="P40" s="99"/>
+      <c r="Q40" s="99"/>
+      <c r="R40" s="99"/>
+      <c r="S40" s="99"/>
+      <c r="T40" s="99"/>
+      <c r="U40" s="99"/>
+      <c r="V40" s="99"/>
+      <c r="W40" s="99"/>
+      <c r="X40" s="99"/>
+      <c r="Y40" s="99"/>
+      <c r="Z40" s="99"/>
+      <c r="AA40" s="99"/>
+      <c r="AB40" s="114"/>
     </row>
     <row r="41" spans="1:29" ht="11.25" customHeight="1">
       <c r="A41" s="26"/>
@@ -3922,14 +3919,14 @@
       <c r="C46" s="53"/>
     </row>
     <row r="47" spans="1:29" ht="15" customHeight="1">
-      <c r="B47" s="140" t="s">
+      <c r="B47" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="104"/>
-      <c r="D47" s="104"/>
-      <c r="E47" s="104"/>
-      <c r="F47" s="104"/>
-      <c r="G47" s="104"/>
+      <c r="C47" s="106"/>
+      <c r="D47" s="106"/>
+      <c r="E47" s="106"/>
+      <c r="F47" s="106"/>
+      <c r="G47" s="106"/>
       <c r="J47" s="17"/>
       <c r="K47" s="55" t="s">
         <v>33</v>
@@ -3949,17 +3946,17 @@
       </c>
       <c r="D50" s="59"/>
       <c r="E50" s="59"/>
-      <c r="F50" s="141"/>
-      <c r="G50" s="115"/>
-      <c r="H50" s="115"/>
+      <c r="F50" s="107"/>
+      <c r="G50" s="108"/>
+      <c r="H50" s="108"/>
       <c r="J50" s="60"/>
       <c r="K50" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="N50" s="141"/>
-      <c r="O50" s="115"/>
-      <c r="P50" s="115"/>
-      <c r="Q50" s="115"/>
+      <c r="N50" s="107"/>
+      <c r="O50" s="108"/>
+      <c r="P50" s="108"/>
+      <c r="Q50" s="108"/>
     </row>
     <row r="51" spans="1:17" ht="12" customHeight="1">
       <c r="F51" s="58"/>
@@ -34128,13 +34125,45 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="X35:AA35"/>
-    <mergeCell ref="X28:AA28"/>
-    <mergeCell ref="X30:AA30"/>
-    <mergeCell ref="X31:AA31"/>
-    <mergeCell ref="X33:AA33"/>
-    <mergeCell ref="X34:AA34"/>
-    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="Y22:AB22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="X23:AA23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="X24:AA24"/>
+    <mergeCell ref="B13:AB13"/>
+    <mergeCell ref="B15:AB15"/>
+    <mergeCell ref="B16:AB16"/>
+    <mergeCell ref="B17:AB17"/>
+    <mergeCell ref="G19:N20"/>
+    <mergeCell ref="X19:AA21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="B18:AB18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="O19:W20"/>
+    <mergeCell ref="B7:AB7"/>
+    <mergeCell ref="B8:AB8"/>
+    <mergeCell ref="B10:AB10"/>
+    <mergeCell ref="B11:AB11"/>
+    <mergeCell ref="B12:AB12"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="B6:AB6"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="G2:Q2"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="G3:Q3"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
     <mergeCell ref="X25:AA25"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="F50:H50"/>
@@ -34151,45 +34180,13 @@
     <mergeCell ref="X26:AA26"/>
     <mergeCell ref="X27:AA27"/>
     <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="G3:Q3"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="B6:AB6"/>
-    <mergeCell ref="O19:W20"/>
-    <mergeCell ref="B7:AB7"/>
-    <mergeCell ref="B8:AB8"/>
-    <mergeCell ref="B10:AB10"/>
-    <mergeCell ref="B11:AB11"/>
-    <mergeCell ref="B12:AB12"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="X24:AA24"/>
-    <mergeCell ref="B13:AB13"/>
-    <mergeCell ref="B15:AB15"/>
-    <mergeCell ref="B16:AB16"/>
-    <mergeCell ref="B17:AB17"/>
-    <mergeCell ref="G19:N20"/>
-    <mergeCell ref="X19:AA21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="B18:AB18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="Y22:AB22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="X23:AA23"/>
+    <mergeCell ref="X35:AA35"/>
+    <mergeCell ref="X28:AA28"/>
+    <mergeCell ref="X30:AA30"/>
+    <mergeCell ref="X31:AA31"/>
+    <mergeCell ref="X33:AA33"/>
+    <mergeCell ref="X34:AA34"/>
+    <mergeCell ref="X29:AA29"/>
   </mergeCells>
   <conditionalFormatting sqref="F49:G50">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
@@ -34218,8 +34215,8 @@
   </sheetPr>
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -34232,55 +34229,55 @@
   <sheetData>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="149" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
       <c r="H2" s="150"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="151"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="146"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="114"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="151"/>
-      <c r="B4" s="108"/>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="146"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="114"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="151"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="146"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="114"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="151"/>
-      <c r="B6" s="108"/>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="146"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="114"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="152"/>
@@ -34337,12 +34334,12 @@
         <v>45644</v>
       </c>
       <c r="F11" s="61"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="108"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="61" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="61"/>
@@ -34385,7 +34382,7 @@
         <v>44</v>
       </c>
       <c r="H14" s="72" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="122.25" customHeight="1">
@@ -34393,7 +34390,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C15" s="75" t="s">
         <v>46</v>
@@ -34402,16 +34399,16 @@
         <v>47</v>
       </c>
       <c r="E15" s="77" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
-      <c r="F15" s="96" t="s">
-        <v>83</v>
+      <c r="F15" s="97" t="s">
+        <v>63</v>
       </c>
-      <c r="G15" s="83" t="s">
-        <v>66</v>
+      <c r="G15" s="95" t="s">
+        <v>78</v>
       </c>
       <c r="H15" s="78" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="141.75" customHeight="1">
@@ -34426,16 +34423,16 @@
         <v>47</v>
       </c>
       <c r="E16" s="77" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
-      <c r="F16" s="96" t="s">
-        <v>83</v>
+      <c r="F16" s="97" t="s">
+        <v>63</v>
       </c>
-      <c r="G16" s="83" t="s">
-        <v>66</v>
+      <c r="G16" s="95" t="s">
+        <v>78</v>
       </c>
       <c r="H16" s="79" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="165" customHeight="1">
@@ -34444,22 +34441,22 @@
         <v>45667</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D17" s="76" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="77" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
-      <c r="F17" s="96" t="s">
-        <v>82</v>
+      <c r="F17" s="97" t="s">
+        <v>63</v>
       </c>
-      <c r="G17" s="83" t="s">
-        <v>66</v>
+      <c r="G17" s="95" t="s">
+        <v>78</v>
       </c>
       <c r="H17" s="80" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="132">
@@ -34468,22 +34465,22 @@
         <v>45668</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D18" s="76" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="77" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
-      <c r="F18" s="96" t="s">
-        <v>82</v>
+      <c r="F18" s="97" t="s">
+        <v>63</v>
       </c>
-      <c r="G18" s="83" t="s">
-        <v>66</v>
+      <c r="G18" s="95" t="s">
+        <v>78</v>
       </c>
-      <c r="H18" s="97" t="s">
-        <v>85</v>
+      <c r="H18" s="96" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -34498,6 +34495,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EDB39E34F5A9B445B025C05B2A05D030" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c21ef800502b5dc1190a9a0361733939">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f1f31ffb-9912-4459-99c8-b26e82094b51" xmlns:ns4="ce621958-37b1-43fe-a1f1-1aad67996a88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30daf50bb6192471b76b9808b4256f50" ns3:_="" ns4:_="">
     <xsd:import namespace="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
@@ -34692,24 +34706,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D01A9D5D-1824-48C2-8527-9D8749A8DDDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34726,29 +34748,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajustes en el plan de auditoria
</commit_message>
<xml_diff>
--- a/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
+++ b/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATIAS\Desktop\ESPE\Septimo_Semestre\Quality Assurance\Repo\2563_G3_ACSW\02_Proyecto\09. Programa de Auditoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{396B89BC-956B-44FD-B2C7-B8E74777C281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229D6D04-794D-48B0-B515-6A042A38C3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. PROGRAMA" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
   <si>
     <t>Fecha de Emisión:</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>6.2</t>
-  </si>
-  <si>
-    <t>6.3</t>
   </si>
   <si>
     <t>6.4</t>
@@ -438,39 +435,7 @@
     <t>6.5</t>
   </si>
   <si>
-    <t>Auditor: Mateo Román</t>
-  </si>
-  <si>
-    <t>Plan para la Auditoria el sistema de control de inventario de la distribuidora "El Oferton"</t>
-  </si>
-  <si>
     <t>Versión:1.0</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ALCANCE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> La auditoría abarcará toda la documentación relacionada con la especificación de requisitos generada durante el proceso de desarrollo de un producto software. Asimismo, se verificará la adecuación de un plan de pruebas optimizado mediante la revisión de casos de prueba alineados con los estándares de la norma ISO/IEC/IEEE 29119-5:2016, con especial atención a los aspectos indicados en:
-6.2: Identificación de palabras clave ("Identifying keywords").
-6.3: Composición de casos de prueba ("Composing test cases").
-6.4: Pruebas basadas en palabras clave y en datos ("Keywords and data-driven testing").
-6.5: Modularidad y refactorización ("Modularity and Refactoring").
-Además, se realizarán reuniones con el equipo auditado para validar el cumplimiento de los objetivos establecidos y garantizar un cierre eficiente del proceso de auditoría.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -491,27 +456,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Is a pivotal task in Keyword-Driven Testing as the contents, granularity and structure of the keywords can impact the way keyword test cases are defined. It is important to name keywords in a way that appears natural to the people who will be working with them.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Composing test cases(6.3):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Keyword test cases can be created from previously defined keywords and documented using tables or databases. These cases typically use keywords from a single layer, allowing different testers to design different layers.</t>
     </r>
   </si>
   <si>
@@ -563,9 +507,38 @@
   <si>
     <t xml:space="preserve">
 6.2 Identifying keywords
-6.3 Composing test cases
 6.4 Keywords and data-driven testing
 6.5 Modularity and refactoring </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ALCANCE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> La auditoría abarcará toda la documentación relacionada con la especificación de requisitos generada durante el proceso de desarrollo de un producto software. Asimismo, se verificará la adecuación de un plan de pruebas optimizado mediante la revisión de casos de prueba alineados con los estándares de la norma ISO/IEC/IEEE 29119-5:2016, con especial atención a los aspectos indicados en:
+6.2: Identificación de palabras clave ("Identifying keywords").
+6.4: Pruebas basadas en palabras clave y en datos ("Keywords and data-driven testing").
+6.5: Modularidad y refactorización ("Modularity and Refactoring").</t>
+    </r>
+  </si>
+  <si>
+    <t>Plan para la Auditoria del sistema de control de inventario de Bazar y Papeleria</t>
+  </si>
+  <si>
+    <t>Auditor: Cristopher Zambrano</t>
   </si>
 </sst>
 </file>
@@ -889,7 +862,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1307,6 +1280,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1314,7 +1326,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="29"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="29"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1513,9 +1525,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1548,12 +1557,6 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="18" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1563,87 +1566,29 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1651,8 +1596,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1669,14 +1624,62 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1692,6 +1695,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1954,8 +1975,8 @@
   </sheetPr>
   <dimension ref="A1:AW994"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E11" zoomScale="64" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24:AA24"/>
+    <sheetView showGridLines="0" topLeftCell="A30" zoomScale="64" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -1988,37 +2009,37 @@
     </row>
     <row r="2" spans="1:48" ht="42.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="119" t="s">
+      <c r="B2" s="133"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="120"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="101"/>
-      <c r="X2" s="101"/>
-      <c r="Y2" s="102"/>
-      <c r="Z2" s="119" t="s">
-        <v>52</v>
+      <c r="S2" s="135"/>
+      <c r="T2" s="135"/>
+      <c r="U2" s="135"/>
+      <c r="V2" s="135"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="131" t="s">
+        <v>51</v>
       </c>
-      <c r="AA2" s="101"/>
-      <c r="AB2" s="102"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="99"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -2042,37 +2063,37 @@
     </row>
     <row r="3" spans="1:48" ht="48.75" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="116"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
-      <c r="Q3" s="102"/>
-      <c r="R3" s="122" t="s">
+      <c r="B3" s="111"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="123"/>
-      <c r="T3" s="123"/>
-      <c r="U3" s="123"/>
-      <c r="V3" s="123"/>
-      <c r="W3" s="101"/>
-      <c r="X3" s="101"/>
-      <c r="Y3" s="102"/>
-      <c r="Z3" s="119" t="s">
-        <v>52</v>
+      <c r="S3" s="130"/>
+      <c r="T3" s="130"/>
+      <c r="U3" s="130"/>
+      <c r="V3" s="130"/>
+      <c r="W3" s="98"/>
+      <c r="X3" s="98"/>
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="131" t="s">
+        <v>51</v>
       </c>
-      <c r="AA3" s="101"/>
-      <c r="AB3" s="102"/>
+      <c r="AA3" s="98"/>
+      <c r="AB3" s="99"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
@@ -2096,39 +2117,39 @@
     </row>
     <row r="4" spans="1:48" ht="21" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="125"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="101"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="122" t="s">
-        <v>82</v>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="98"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="129" t="s">
+        <v>79</v>
       </c>
-      <c r="S4" s="123"/>
-      <c r="T4" s="123"/>
-      <c r="U4" s="123"/>
-      <c r="V4" s="123"/>
-      <c r="W4" s="101"/>
-      <c r="X4" s="101"/>
-      <c r="Y4" s="102"/>
-      <c r="Z4" s="119" t="s">
+      <c r="S4" s="130"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="130"/>
+      <c r="V4" s="130"/>
+      <c r="W4" s="98"/>
+      <c r="X4" s="98"/>
+      <c r="Y4" s="99"/>
+      <c r="Z4" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="101"/>
-      <c r="AB4" s="102"/>
+      <c r="AA4" s="98"/>
+      <c r="AB4" s="99"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
@@ -2201,35 +2222,35 @@
       <c r="AV5" s="2"/>
     </row>
     <row r="6" spans="1:48" ht="50.25" customHeight="1">
-      <c r="B6" s="126" t="s">
-        <v>66</v>
+      <c r="B6" s="132" t="s">
+        <v>65</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
-      <c r="N6" s="99"/>
-      <c r="O6" s="99"/>
-      <c r="P6" s="99"/>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="99"/>
-      <c r="S6" s="99"/>
-      <c r="T6" s="99"/>
-      <c r="U6" s="99"/>
-      <c r="V6" s="99"/>
-      <c r="W6" s="99"/>
-      <c r="X6" s="99"/>
-      <c r="Y6" s="99"/>
-      <c r="Z6" s="99"/>
-      <c r="AA6" s="99"/>
-      <c r="AB6" s="99"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="105"/>
+      <c r="M6" s="105"/>
+      <c r="N6" s="105"/>
+      <c r="O6" s="105"/>
+      <c r="P6" s="105"/>
+      <c r="Q6" s="105"/>
+      <c r="R6" s="105"/>
+      <c r="S6" s="105"/>
+      <c r="T6" s="105"/>
+      <c r="U6" s="105"/>
+      <c r="V6" s="105"/>
+      <c r="W6" s="105"/>
+      <c r="X6" s="105"/>
+      <c r="Y6" s="105"/>
+      <c r="Z6" s="105"/>
+      <c r="AA6" s="105"/>
+      <c r="AB6" s="105"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="6"/>
@@ -2246,35 +2267,35 @@
       <c r="AP6" s="7"/>
     </row>
     <row r="7" spans="1:48" ht="198" customHeight="1">
-      <c r="B7" s="133" t="s">
-        <v>83</v>
+      <c r="B7" s="104" t="s">
+        <v>84</v>
       </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="99"/>
-      <c r="S7" s="99"/>
-      <c r="T7" s="99"/>
-      <c r="U7" s="99"/>
-      <c r="V7" s="99"/>
-      <c r="W7" s="99"/>
-      <c r="X7" s="99"/>
-      <c r="Y7" s="99"/>
-      <c r="Z7" s="99"/>
-      <c r="AA7" s="99"/>
-      <c r="AB7" s="99"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="105"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="105"/>
+      <c r="N7" s="105"/>
+      <c r="O7" s="105"/>
+      <c r="P7" s="105"/>
+      <c r="Q7" s="105"/>
+      <c r="R7" s="105"/>
+      <c r="S7" s="105"/>
+      <c r="T7" s="105"/>
+      <c r="U7" s="105"/>
+      <c r="V7" s="105"/>
+      <c r="W7" s="105"/>
+      <c r="X7" s="105"/>
+      <c r="Y7" s="105"/>
+      <c r="Z7" s="105"/>
+      <c r="AA7" s="105"/>
+      <c r="AB7" s="105"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
       <c r="AE7" s="6"/>
@@ -2291,35 +2312,35 @@
       <c r="AP7" s="7"/>
     </row>
     <row r="8" spans="1:48" ht="51" customHeight="1">
-      <c r="B8" s="134" t="s">
-        <v>65</v>
+      <c r="B8" s="126" t="s">
+        <v>64</v>
       </c>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="99"/>
-      <c r="N8" s="99"/>
-      <c r="O8" s="99"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="99"/>
-      <c r="S8" s="99"/>
-      <c r="T8" s="99"/>
-      <c r="U8" s="99"/>
-      <c r="V8" s="99"/>
-      <c r="W8" s="99"/>
-      <c r="X8" s="99"/>
-      <c r="Y8" s="99"/>
-      <c r="Z8" s="99"/>
-      <c r="AA8" s="99"/>
-      <c r="AB8" s="99"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="105"/>
+      <c r="O8" s="105"/>
+      <c r="P8" s="105"/>
+      <c r="Q8" s="105"/>
+      <c r="R8" s="105"/>
+      <c r="S8" s="105"/>
+      <c r="T8" s="105"/>
+      <c r="U8" s="105"/>
+      <c r="V8" s="105"/>
+      <c r="W8" s="105"/>
+      <c r="X8" s="105"/>
+      <c r="Y8" s="105"/>
+      <c r="Z8" s="105"/>
+      <c r="AA8" s="105"/>
+      <c r="AB8" s="105"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="6"/>
@@ -2379,35 +2400,35 @@
       <c r="AP9" s="7"/>
     </row>
     <row r="10" spans="1:48" ht="20.25" customHeight="1">
-      <c r="B10" s="134" t="s">
-        <v>53</v>
+      <c r="B10" s="126" t="s">
+        <v>52</v>
       </c>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="99"/>
-      <c r="N10" s="99"/>
-      <c r="O10" s="99"/>
-      <c r="P10" s="99"/>
-      <c r="Q10" s="99"/>
-      <c r="R10" s="99"/>
-      <c r="S10" s="99"/>
-      <c r="T10" s="99"/>
-      <c r="U10" s="99"/>
-      <c r="V10" s="99"/>
-      <c r="W10" s="99"/>
-      <c r="X10" s="99"/>
-      <c r="Y10" s="99"/>
-      <c r="Z10" s="99"/>
-      <c r="AA10" s="99"/>
-      <c r="AB10" s="99"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="105"/>
+      <c r="N10" s="105"/>
+      <c r="O10" s="105"/>
+      <c r="P10" s="105"/>
+      <c r="Q10" s="105"/>
+      <c r="R10" s="105"/>
+      <c r="S10" s="105"/>
+      <c r="T10" s="105"/>
+      <c r="U10" s="105"/>
+      <c r="V10" s="105"/>
+      <c r="W10" s="105"/>
+      <c r="X10" s="105"/>
+      <c r="Y10" s="105"/>
+      <c r="Z10" s="105"/>
+      <c r="AA10" s="105"/>
+      <c r="AB10" s="105"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="6"/>
@@ -2425,35 +2446,35 @@
     </row>
     <row r="11" spans="1:48" ht="60" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="133" t="s">
-        <v>67</v>
+      <c r="B11" s="104" t="s">
+        <v>66</v>
       </c>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="99"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="99"/>
-      <c r="N11" s="99"/>
-      <c r="O11" s="99"/>
-      <c r="P11" s="99"/>
-      <c r="Q11" s="99"/>
-      <c r="R11" s="99"/>
-      <c r="S11" s="99"/>
-      <c r="T11" s="99"/>
-      <c r="U11" s="99"/>
-      <c r="V11" s="99"/>
-      <c r="W11" s="99"/>
-      <c r="X11" s="99"/>
-      <c r="Y11" s="99"/>
-      <c r="Z11" s="99"/>
-      <c r="AA11" s="99"/>
-      <c r="AB11" s="99"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="105"/>
+      <c r="N11" s="105"/>
+      <c r="O11" s="105"/>
+      <c r="P11" s="105"/>
+      <c r="Q11" s="105"/>
+      <c r="R11" s="105"/>
+      <c r="S11" s="105"/>
+      <c r="T11" s="105"/>
+      <c r="U11" s="105"/>
+      <c r="V11" s="105"/>
+      <c r="W11" s="105"/>
+      <c r="X11" s="105"/>
+      <c r="Y11" s="105"/>
+      <c r="Z11" s="105"/>
+      <c r="AA11" s="105"/>
+      <c r="AB11" s="105"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="9"/>
       <c r="AE11" s="9"/>
@@ -2476,35 +2497,35 @@
       <c r="AV11" s="8"/>
     </row>
     <row r="12" spans="1:48" ht="53.25" customHeight="1">
-      <c r="B12" s="133" t="s">
-        <v>68</v>
+      <c r="B12" s="104" t="s">
+        <v>67</v>
       </c>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="99"/>
-      <c r="H12" s="99"/>
-      <c r="I12" s="99"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="99"/>
-      <c r="M12" s="99"/>
-      <c r="N12" s="99"/>
-      <c r="O12" s="99"/>
-      <c r="P12" s="99"/>
-      <c r="Q12" s="99"/>
-      <c r="R12" s="99"/>
-      <c r="S12" s="99"/>
-      <c r="T12" s="99"/>
-      <c r="U12" s="99"/>
-      <c r="V12" s="99"/>
-      <c r="W12" s="99"/>
-      <c r="X12" s="99"/>
-      <c r="Y12" s="99"/>
-      <c r="Z12" s="99"/>
-      <c r="AA12" s="99"/>
-      <c r="AB12" s="99"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="105"/>
+      <c r="N12" s="105"/>
+      <c r="O12" s="105"/>
+      <c r="P12" s="105"/>
+      <c r="Q12" s="105"/>
+      <c r="R12" s="105"/>
+      <c r="S12" s="105"/>
+      <c r="T12" s="105"/>
+      <c r="U12" s="105"/>
+      <c r="V12" s="105"/>
+      <c r="W12" s="105"/>
+      <c r="X12" s="105"/>
+      <c r="Y12" s="105"/>
+      <c r="Z12" s="105"/>
+      <c r="AA12" s="105"/>
+      <c r="AB12" s="105"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
@@ -2521,35 +2542,35 @@
       <c r="AP12" s="7"/>
     </row>
     <row r="13" spans="1:48" ht="39.75" customHeight="1">
-      <c r="B13" s="133" t="s">
-        <v>69</v>
+      <c r="B13" s="104" t="s">
+        <v>68</v>
       </c>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="99"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="99"/>
-      <c r="M13" s="99"/>
-      <c r="N13" s="99"/>
-      <c r="O13" s="99"/>
-      <c r="P13" s="99"/>
-      <c r="Q13" s="99"/>
-      <c r="R13" s="99"/>
-      <c r="S13" s="99"/>
-      <c r="T13" s="99"/>
-      <c r="U13" s="99"/>
-      <c r="V13" s="99"/>
-      <c r="W13" s="99"/>
-      <c r="X13" s="99"/>
-      <c r="Y13" s="99"/>
-      <c r="Z13" s="99"/>
-      <c r="AA13" s="99"/>
-      <c r="AB13" s="99"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="105"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
+      <c r="N13" s="105"/>
+      <c r="O13" s="105"/>
+      <c r="P13" s="105"/>
+      <c r="Q13" s="105"/>
+      <c r="R13" s="105"/>
+      <c r="S13" s="105"/>
+      <c r="T13" s="105"/>
+      <c r="U13" s="105"/>
+      <c r="V13" s="105"/>
+      <c r="W13" s="105"/>
+      <c r="X13" s="105"/>
+      <c r="Y13" s="105"/>
+      <c r="Z13" s="105"/>
+      <c r="AA13" s="105"/>
+      <c r="AB13" s="105"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
@@ -2609,35 +2630,35 @@
       <c r="AP14" s="7"/>
     </row>
     <row r="15" spans="1:48" ht="99.75" customHeight="1">
-      <c r="B15" s="135" t="s">
-        <v>70</v>
+      <c r="B15" s="106" t="s">
+        <v>69</v>
       </c>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99"/>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99"/>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
-      <c r="R15" s="99"/>
-      <c r="S15" s="99"/>
-      <c r="T15" s="99"/>
-      <c r="U15" s="99"/>
-      <c r="V15" s="99"/>
-      <c r="W15" s="99"/>
-      <c r="X15" s="99"/>
-      <c r="Y15" s="99"/>
-      <c r="Z15" s="99"/>
-      <c r="AA15" s="99"/>
-      <c r="AB15" s="99"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="105"/>
+      <c r="O15" s="105"/>
+      <c r="P15" s="105"/>
+      <c r="Q15" s="105"/>
+      <c r="R15" s="105"/>
+      <c r="S15" s="105"/>
+      <c r="T15" s="105"/>
+      <c r="U15" s="105"/>
+      <c r="V15" s="105"/>
+      <c r="W15" s="105"/>
+      <c r="X15" s="105"/>
+      <c r="Y15" s="105"/>
+      <c r="Z15" s="105"/>
+      <c r="AA15" s="105"/>
+      <c r="AB15" s="105"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="6"/>
@@ -2655,35 +2676,35 @@
     </row>
     <row r="16" spans="1:48" ht="24.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="136" t="s">
-        <v>71</v>
+      <c r="B16" s="107" t="s">
+        <v>70</v>
       </c>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="99"/>
-      <c r="O16" s="99"/>
-      <c r="P16" s="99"/>
-      <c r="Q16" s="99"/>
-      <c r="R16" s="99"/>
-      <c r="S16" s="99"/>
-      <c r="T16" s="99"/>
-      <c r="U16" s="99"/>
-      <c r="V16" s="99"/>
-      <c r="W16" s="99"/>
-      <c r="X16" s="99"/>
-      <c r="Y16" s="99"/>
-      <c r="Z16" s="99"/>
-      <c r="AA16" s="99"/>
-      <c r="AB16" s="99"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="105"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="105"/>
+      <c r="Q16" s="105"/>
+      <c r="R16" s="105"/>
+      <c r="S16" s="105"/>
+      <c r="T16" s="105"/>
+      <c r="U16" s="105"/>
+      <c r="V16" s="105"/>
+      <c r="W16" s="105"/>
+      <c r="X16" s="105"/>
+      <c r="Y16" s="105"/>
+      <c r="Z16" s="105"/>
+      <c r="AA16" s="105"/>
+      <c r="AB16" s="105"/>
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
@@ -2706,35 +2727,35 @@
       <c r="AV16" s="2"/>
     </row>
     <row r="17" spans="1:49" ht="24.75" customHeight="1">
-      <c r="B17" s="135" t="s">
+      <c r="B17" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="99"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="99"/>
-      <c r="I17" s="99"/>
-      <c r="J17" s="99"/>
-      <c r="K17" s="99"/>
-      <c r="L17" s="99"/>
-      <c r="M17" s="99"/>
-      <c r="N17" s="99"/>
-      <c r="O17" s="99"/>
-      <c r="P17" s="99"/>
-      <c r="Q17" s="99"/>
-      <c r="R17" s="99"/>
-      <c r="S17" s="99"/>
-      <c r="T17" s="99"/>
-      <c r="U17" s="99"/>
-      <c r="V17" s="99"/>
-      <c r="W17" s="99"/>
-      <c r="X17" s="99"/>
-      <c r="Y17" s="99"/>
-      <c r="Z17" s="99"/>
-      <c r="AA17" s="99"/>
-      <c r="AB17" s="99"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="105"/>
+      <c r="N17" s="105"/>
+      <c r="O17" s="105"/>
+      <c r="P17" s="105"/>
+      <c r="Q17" s="105"/>
+      <c r="R17" s="105"/>
+      <c r="S17" s="105"/>
+      <c r="T17" s="105"/>
+      <c r="U17" s="105"/>
+      <c r="V17" s="105"/>
+      <c r="W17" s="105"/>
+      <c r="X17" s="105"/>
+      <c r="Y17" s="105"/>
+      <c r="Z17" s="105"/>
+      <c r="AA17" s="105"/>
+      <c r="AB17" s="105"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="6"/>
@@ -2751,33 +2772,33 @@
       <c r="AP17" s="7"/>
     </row>
     <row r="18" spans="1:49" ht="6.75" customHeight="1">
-      <c r="B18" s="135"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="99"/>
-      <c r="J18" s="99"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="99"/>
-      <c r="M18" s="99"/>
-      <c r="N18" s="99"/>
-      <c r="O18" s="99"/>
-      <c r="P18" s="99"/>
-      <c r="Q18" s="99"/>
-      <c r="R18" s="99"/>
-      <c r="S18" s="99"/>
-      <c r="T18" s="99"/>
-      <c r="U18" s="99"/>
-      <c r="V18" s="99"/>
-      <c r="W18" s="99"/>
-      <c r="X18" s="99"/>
-      <c r="Y18" s="99"/>
-      <c r="Z18" s="99"/>
-      <c r="AA18" s="99"/>
-      <c r="AB18" s="99"/>
+      <c r="B18" s="106"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="105"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="105"/>
+      <c r="L18" s="105"/>
+      <c r="M18" s="105"/>
+      <c r="N18" s="105"/>
+      <c r="O18" s="105"/>
+      <c r="P18" s="105"/>
+      <c r="Q18" s="105"/>
+      <c r="R18" s="105"/>
+      <c r="S18" s="105"/>
+      <c r="T18" s="105"/>
+      <c r="U18" s="105"/>
+      <c r="V18" s="105"/>
+      <c r="W18" s="105"/>
+      <c r="X18" s="105"/>
+      <c r="Y18" s="105"/>
+      <c r="Z18" s="105"/>
+      <c r="AA18" s="105"/>
+      <c r="AB18" s="105"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
@@ -2795,45 +2816,45 @@
     </row>
     <row r="19" spans="1:49" ht="36.75" customHeight="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="139" t="s">
+      <c r="B19" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="142" t="s">
+      <c r="C19" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="128"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="143" t="s">
+      <c r="D19" s="109"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="127" t="s">
+      <c r="G19" s="108" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="109"/>
+      <c r="K19" s="109"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="109"/>
+      <c r="N19" s="110"/>
+      <c r="O19" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="128"/>
-      <c r="I19" s="128"/>
-      <c r="J19" s="128"/>
-      <c r="K19" s="128"/>
-      <c r="L19" s="128"/>
-      <c r="M19" s="128"/>
-      <c r="N19" s="129"/>
-      <c r="O19" s="127" t="s">
-        <v>55</v>
-      </c>
-      <c r="P19" s="128"/>
-      <c r="Q19" s="128"/>
-      <c r="R19" s="128"/>
-      <c r="S19" s="128"/>
-      <c r="T19" s="128"/>
-      <c r="U19" s="128"/>
-      <c r="V19" s="128"/>
-      <c r="W19" s="129"/>
-      <c r="X19" s="137" t="s">
+      <c r="P19" s="109"/>
+      <c r="Q19" s="109"/>
+      <c r="R19" s="109"/>
+      <c r="S19" s="109"/>
+      <c r="T19" s="109"/>
+      <c r="U19" s="109"/>
+      <c r="V19" s="109"/>
+      <c r="W19" s="110"/>
+      <c r="X19" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="Y19" s="128"/>
-      <c r="Z19" s="128"/>
-      <c r="AA19" s="129"/>
-      <c r="AB19" s="84" t="s">
+      <c r="Y19" s="109"/>
+      <c r="Z19" s="109"/>
+      <c r="AA19" s="110"/>
+      <c r="AB19" s="83" t="s">
         <v>9</v>
       </c>
       <c r="AC19" s="14"/>
@@ -2859,33 +2880,33 @@
     </row>
     <row r="20" spans="1:49" ht="10.5" customHeight="1">
       <c r="A20" s="14"/>
-      <c r="B20" s="140"/>
-      <c r="C20" s="130"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="132"/>
-      <c r="F20" s="144"/>
-      <c r="G20" s="116"/>
-      <c r="H20" s="108"/>
-      <c r="I20" s="108"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="108"/>
-      <c r="L20" s="108"/>
-      <c r="M20" s="108"/>
-      <c r="N20" s="117"/>
-      <c r="O20" s="130"/>
-      <c r="P20" s="131"/>
-      <c r="Q20" s="131"/>
-      <c r="R20" s="131"/>
-      <c r="S20" s="131"/>
-      <c r="T20" s="131"/>
-      <c r="U20" s="131"/>
-      <c r="V20" s="131"/>
-      <c r="W20" s="132"/>
-      <c r="X20" s="130"/>
-      <c r="Y20" s="99"/>
-      <c r="Z20" s="99"/>
-      <c r="AA20" s="132"/>
-      <c r="AB20" s="85"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="115"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="123"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="112"/>
+      <c r="J20" s="112"/>
+      <c r="K20" s="112"/>
+      <c r="L20" s="112"/>
+      <c r="M20" s="112"/>
+      <c r="N20" s="113"/>
+      <c r="O20" s="115"/>
+      <c r="P20" s="125"/>
+      <c r="Q20" s="125"/>
+      <c r="R20" s="125"/>
+      <c r="S20" s="125"/>
+      <c r="T20" s="125"/>
+      <c r="U20" s="125"/>
+      <c r="V20" s="125"/>
+      <c r="W20" s="116"/>
+      <c r="X20" s="115"/>
+      <c r="Y20" s="105"/>
+      <c r="Z20" s="105"/>
+      <c r="AA20" s="116"/>
+      <c r="AB20" s="84"/>
       <c r="AC20" s="14"/>
       <c r="AD20" s="14"/>
       <c r="AE20" s="14"/>
@@ -2909,49 +2930,49 @@
     </row>
     <row r="21" spans="1:49" ht="34.5" customHeight="1">
       <c r="A21" s="15"/>
-      <c r="B21" s="140"/>
-      <c r="C21" s="130"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="144"/>
-      <c r="G21" s="138" t="s">
+      <c r="B21" s="119"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="102"/>
-      <c r="I21" s="138" t="s">
+      <c r="H21" s="99"/>
+      <c r="I21" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="102"/>
-      <c r="K21" s="138" t="s">
+      <c r="J21" s="99"/>
+      <c r="K21" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="102"/>
-      <c r="M21" s="138" t="s">
+      <c r="L21" s="99"/>
+      <c r="M21" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="101"/>
-      <c r="O21" s="147" t="s">
+      <c r="N21" s="98"/>
+      <c r="O21" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="P21" s="147"/>
-      <c r="Q21" s="147"/>
-      <c r="R21" s="147"/>
-      <c r="S21" s="146" t="s">
+      <c r="P21" s="96"/>
+      <c r="Q21" s="96"/>
+      <c r="R21" s="96"/>
+      <c r="S21" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="T21" s="147"/>
-      <c r="U21" s="92" t="s">
+      <c r="T21" s="96"/>
+      <c r="U21" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="V21" s="92" t="s">
+      <c r="V21" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="W21" s="88"/>
-      <c r="X21" s="108"/>
-      <c r="Y21" s="108"/>
-      <c r="Z21" s="108"/>
-      <c r="AA21" s="117"/>
-      <c r="AB21" s="85"/>
+      <c r="W21" s="87"/>
+      <c r="X21" s="112"/>
+      <c r="Y21" s="112"/>
+      <c r="Z21" s="112"/>
+      <c r="AA21" s="113"/>
+      <c r="AB21" s="84"/>
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
       <c r="AE21" s="15"/>
@@ -2975,15 +2996,15 @@
     </row>
     <row r="22" spans="1:49" ht="38.25" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="141"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="108"/>
-      <c r="E22" s="117"/>
-      <c r="F22" s="145"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="111"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="124"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J22" s="16" t="s">
         <v>14</v>
@@ -2997,40 +3018,38 @@
       <c r="M22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="N22" s="83" t="s">
+      <c r="N22" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="O22" s="91" t="s">
-        <v>57</v>
+      <c r="O22" s="90" t="s">
+        <v>56</v>
       </c>
-      <c r="P22" s="91" t="s">
+      <c r="P22" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q22" s="156">
+        <v>10</v>
+      </c>
+      <c r="R22" s="157"/>
+      <c r="S22" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="Q22" s="94">
-        <v>10</v>
-      </c>
-      <c r="R22" s="94">
-        <v>11</v>
-      </c>
-      <c r="S22" s="89" t="s">
+      <c r="T22" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="T22" s="87" t="s">
-        <v>62</v>
+      <c r="U22" s="86" t="s">
+        <v>72</v>
       </c>
-      <c r="U22" s="87" t="s">
+      <c r="V22" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="V22" s="87" t="s">
-        <v>74</v>
-      </c>
-      <c r="W22" s="87"/>
-      <c r="X22" s="87"/>
-      <c r="Y22" s="148"/>
-      <c r="Z22" s="101"/>
-      <c r="AA22" s="101"/>
-      <c r="AB22" s="102"/>
-      <c r="AC22" s="86"/>
+      <c r="W22" s="86"/>
+      <c r="X22" s="86"/>
+      <c r="Y22" s="97"/>
+      <c r="Z22" s="98"/>
+      <c r="AA22" s="98"/>
+      <c r="AB22" s="99"/>
+      <c r="AC22" s="85"/>
       <c r="AD22" s="14"/>
       <c r="AE22" s="14"/>
       <c r="AF22" s="14"/>
@@ -3057,11 +3076,11 @@
       <c r="B23" s="18">
         <v>1</v>
       </c>
-      <c r="C23" s="109" t="s">
+      <c r="C23" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="106"/>
-      <c r="E23" s="110"/>
+      <c r="D23" s="101"/>
+      <c r="E23" s="102"/>
       <c r="F23" s="76">
         <v>1</v>
       </c>
@@ -3075,23 +3094,23 @@
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
-      <c r="O23" s="90"/>
-      <c r="P23" s="90"/>
-      <c r="Q23" s="90"/>
-      <c r="R23" s="93"/>
+      <c r="O23" s="89"/>
+      <c r="P23" s="89"/>
+      <c r="Q23" s="158"/>
+      <c r="R23" s="159"/>
       <c r="S23" s="22"/>
       <c r="T23" s="22"/>
       <c r="U23" s="22"/>
       <c r="V23" s="22"/>
       <c r="W23" s="22"/>
-      <c r="X23" s="100" t="s">
+      <c r="X23" s="103" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y23" s="98"/>
+      <c r="Z23" s="98"/>
+      <c r="AA23" s="99"/>
+      <c r="AB23" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="Y23" s="101"/>
-      <c r="Z23" s="101"/>
-      <c r="AA23" s="102"/>
-      <c r="AB23" s="23" t="s">
-        <v>59</v>
       </c>
       <c r="AC23" s="17"/>
       <c r="AD23" s="17"/>
@@ -3119,11 +3138,11 @@
       <c r="B24" s="18">
         <v>2</v>
       </c>
-      <c r="C24" s="109" t="s">
+      <c r="C24" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="106"/>
-      <c r="E24" s="110"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="102"/>
       <c r="F24" s="76">
         <v>2</v>
       </c>
@@ -3141,25 +3160,23 @@
       <c r="P24" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Q24" s="21" t="s">
+      <c r="Q24" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="R24" s="22" t="s">
-        <v>20</v>
-      </c>
+      <c r="R24" s="161"/>
       <c r="S24" s="22"/>
       <c r="T24" s="22"/>
       <c r="U24" s="22"/>
       <c r="V24" s="22"/>
       <c r="W24" s="22"/>
-      <c r="X24" s="100" t="s">
-        <v>88</v>
+      <c r="X24" s="103" t="s">
+        <v>83</v>
       </c>
-      <c r="Y24" s="101"/>
-      <c r="Z24" s="101"/>
-      <c r="AA24" s="102"/>
+      <c r="Y24" s="98"/>
+      <c r="Z24" s="98"/>
+      <c r="AA24" s="99"/>
       <c r="AB24" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AC24" s="17"/>
       <c r="AD24" s="17"/>
@@ -3187,11 +3204,11 @@
       <c r="B25" s="18">
         <v>3</v>
       </c>
-      <c r="C25" s="109" t="s">
+      <c r="C25" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="106"/>
-      <c r="E25" s="110"/>
+      <c r="D25" s="101"/>
+      <c r="E25" s="102"/>
       <c r="F25" s="76">
         <v>3</v>
       </c>
@@ -3205,8 +3222,8 @@
       <c r="N25" s="21"/>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="22"/>
+      <c r="Q25" s="160"/>
+      <c r="R25" s="161"/>
       <c r="S25" s="22" t="s">
         <v>20</v>
       </c>
@@ -3216,14 +3233,14 @@
       <c r="U25" s="22"/>
       <c r="V25" s="22"/>
       <c r="W25" s="22"/>
-      <c r="X25" s="100" t="s">
-        <v>72</v>
+      <c r="X25" s="103" t="s">
+        <v>71</v>
       </c>
-      <c r="Y25" s="101"/>
-      <c r="Z25" s="101"/>
-      <c r="AA25" s="102"/>
+      <c r="Y25" s="98"/>
+      <c r="Z25" s="98"/>
+      <c r="AA25" s="99"/>
       <c r="AB25" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC25" s="17"/>
       <c r="AD25" s="17"/>
@@ -3251,11 +3268,11 @@
       <c r="B26" s="18">
         <v>4</v>
       </c>
-      <c r="C26" s="109" t="s">
+      <c r="C26" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="106"/>
-      <c r="E26" s="110"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="102"/>
       <c r="F26" s="76">
         <v>4</v>
       </c>
@@ -3269,8 +3286,8 @@
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="22"/>
+      <c r="Q26" s="160"/>
+      <c r="R26" s="161"/>
       <c r="S26" s="22"/>
       <c r="T26" s="22"/>
       <c r="U26" s="22" t="s">
@@ -3278,14 +3295,14 @@
       </c>
       <c r="V26" s="22"/>
       <c r="W26" s="22"/>
-      <c r="X26" s="100" t="s">
+      <c r="X26" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="Y26" s="101"/>
-      <c r="Z26" s="101"/>
-      <c r="AA26" s="102"/>
+      <c r="Y26" s="98"/>
+      <c r="Z26" s="98"/>
+      <c r="AA26" s="99"/>
       <c r="AB26" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC26" s="17"/>
       <c r="AD26" s="17"/>
@@ -3313,12 +3330,12 @@
       <c r="B27" s="18">
         <v>5</v>
       </c>
-      <c r="C27" s="109" t="s">
+      <c r="C27" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="106"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="81">
+      <c r="D27" s="101"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="80">
         <v>5</v>
       </c>
       <c r="G27" s="21"/>
@@ -3331,8 +3348,8 @@
       <c r="N27" s="21"/>
       <c r="O27" s="21"/>
       <c r="P27" s="21"/>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="22"/>
+      <c r="Q27" s="160"/>
+      <c r="R27" s="161"/>
       <c r="S27" s="22"/>
       <c r="T27" s="22"/>
       <c r="U27" s="22"/>
@@ -3340,14 +3357,14 @@
         <v>20</v>
       </c>
       <c r="W27" s="22"/>
-      <c r="X27" s="100" t="s">
+      <c r="X27" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="Y27" s="101"/>
-      <c r="Z27" s="101"/>
-      <c r="AA27" s="102"/>
+      <c r="Y27" s="98"/>
+      <c r="Z27" s="98"/>
+      <c r="AA27" s="99"/>
       <c r="AB27" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AC27" s="17"/>
       <c r="AD27" s="17"/>
@@ -3373,10 +3390,10 @@
     <row r="28" spans="1:49" ht="163.5" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="106"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="82"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="102"/>
+      <c r="F28" s="81"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
@@ -3387,19 +3404,19 @@
       <c r="N28" s="21"/>
       <c r="O28" s="21"/>
       <c r="P28" s="21"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="22"/>
+      <c r="Q28" s="160"/>
+      <c r="R28" s="161"/>
       <c r="S28" s="22"/>
       <c r="T28" s="22"/>
       <c r="U28" s="22"/>
       <c r="V28" s="22"/>
       <c r="W28" s="22"/>
-      <c r="X28" s="100" t="s">
+      <c r="X28" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="Y28" s="101"/>
-      <c r="Z28" s="101"/>
-      <c r="AA28" s="102"/>
+      <c r="Y28" s="98"/>
+      <c r="Z28" s="98"/>
+      <c r="AA28" s="99"/>
       <c r="AB28" s="23"/>
       <c r="AC28" s="17"/>
       <c r="AD28" s="17"/>
@@ -3425,9 +3442,9 @@
     <row r="29" spans="1:49" ht="209.25" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
-      <c r="C29" s="109"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="110"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="102"/>
       <c r="F29" s="19"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
@@ -3439,17 +3456,17 @@
       <c r="N29" s="25"/>
       <c r="O29" s="21"/>
       <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="22"/>
+      <c r="Q29" s="160"/>
+      <c r="R29" s="161"/>
       <c r="S29" s="22"/>
       <c r="T29" s="22"/>
       <c r="U29" s="22"/>
       <c r="V29" s="22"/>
       <c r="W29" s="22"/>
-      <c r="X29" s="100"/>
-      <c r="Y29" s="101"/>
-      <c r="Z29" s="101"/>
-      <c r="AA29" s="102"/>
+      <c r="X29" s="103"/>
+      <c r="Y29" s="98"/>
+      <c r="Z29" s="98"/>
+      <c r="AA29" s="99"/>
       <c r="AB29" s="23"/>
       <c r="AC29" s="17"/>
       <c r="AD29" s="17"/>
@@ -3475,9 +3492,9 @@
     <row r="30" spans="1:49" ht="262.5" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
-      <c r="C30" s="109"/>
-      <c r="D30" s="106"/>
-      <c r="E30" s="110"/>
+      <c r="C30" s="100"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="102"/>
       <c r="F30" s="19"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -3489,17 +3506,17 @@
       <c r="N30" s="21"/>
       <c r="O30" s="25"/>
       <c r="P30" s="21"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="22"/>
+      <c r="Q30" s="160"/>
+      <c r="R30" s="161"/>
       <c r="S30" s="22"/>
       <c r="T30" s="22"/>
       <c r="U30" s="22"/>
       <c r="V30" s="22"/>
       <c r="W30" s="22"/>
-      <c r="X30" s="100"/>
-      <c r="Y30" s="101"/>
-      <c r="Z30" s="101"/>
-      <c r="AA30" s="102"/>
+      <c r="X30" s="103"/>
+      <c r="Y30" s="98"/>
+      <c r="Z30" s="98"/>
+      <c r="AA30" s="99"/>
       <c r="AB30" s="23"/>
       <c r="AC30" s="17"/>
       <c r="AD30" s="17"/>
@@ -3525,9 +3542,9 @@
     <row r="31" spans="1:49" ht="90.75" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
-      <c r="C31" s="111"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="110"/>
+      <c r="C31" s="139"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="102"/>
       <c r="F31" s="19"/>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
@@ -3539,17 +3556,17 @@
       <c r="N31" s="21"/>
       <c r="O31" s="21"/>
       <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="22"/>
+      <c r="Q31" s="160"/>
+      <c r="R31" s="161"/>
       <c r="S31" s="22"/>
       <c r="T31" s="22"/>
       <c r="U31" s="22"/>
       <c r="V31" s="22"/>
       <c r="W31" s="22"/>
-      <c r="X31" s="103"/>
-      <c r="Y31" s="101"/>
-      <c r="Z31" s="101"/>
-      <c r="AA31" s="102"/>
+      <c r="X31" s="141"/>
+      <c r="Y31" s="98"/>
+      <c r="Z31" s="98"/>
+      <c r="AA31" s="99"/>
       <c r="AB31" s="23"/>
       <c r="AC31" s="17"/>
       <c r="AD31" s="17"/>
@@ -3575,9 +3592,9 @@
     <row r="32" spans="1:49" ht="90.75" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
-      <c r="C32" s="112"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="102"/>
+      <c r="C32" s="140"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="99"/>
       <c r="F32" s="19"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
@@ -3589,17 +3606,17 @@
       <c r="N32" s="21"/>
       <c r="O32" s="21"/>
       <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="22"/>
+      <c r="Q32" s="160"/>
+      <c r="R32" s="161"/>
       <c r="S32" s="22"/>
       <c r="T32" s="22"/>
       <c r="U32" s="22"/>
       <c r="V32" s="22"/>
       <c r="W32" s="22"/>
-      <c r="X32" s="103"/>
-      <c r="Y32" s="101"/>
-      <c r="Z32" s="101"/>
-      <c r="AA32" s="102"/>
+      <c r="X32" s="141"/>
+      <c r="Y32" s="98"/>
+      <c r="Z32" s="98"/>
+      <c r="AA32" s="99"/>
       <c r="AB32" s="23"/>
       <c r="AC32" s="17"/>
       <c r="AD32" s="17"/>
@@ -3646,10 +3663,10 @@
       <c r="U33" s="29"/>
       <c r="V33" s="29"/>
       <c r="W33" s="29"/>
-      <c r="X33" s="104"/>
-      <c r="Y33" s="99"/>
-      <c r="Z33" s="99"/>
-      <c r="AA33" s="99"/>
+      <c r="X33" s="145"/>
+      <c r="Y33" s="105"/>
+      <c r="Z33" s="105"/>
+      <c r="AA33" s="105"/>
       <c r="AB33" s="30"/>
     </row>
     <row r="34" spans="1:29" ht="12.75" customHeight="1">
@@ -3676,10 +3693,10 @@
       <c r="U34" s="29"/>
       <c r="V34" s="29"/>
       <c r="W34" s="29"/>
-      <c r="X34" s="104"/>
-      <c r="Y34" s="99"/>
-      <c r="Z34" s="99"/>
-      <c r="AA34" s="99"/>
+      <c r="X34" s="145"/>
+      <c r="Y34" s="105"/>
+      <c r="Z34" s="105"/>
+      <c r="AA34" s="105"/>
       <c r="AB34" s="30"/>
     </row>
     <row r="35" spans="1:29" ht="19.5" customHeight="1">
@@ -3697,10 +3714,10 @@
       <c r="J35" s="17"/>
       <c r="O35" s="38"/>
       <c r="P35" s="38"/>
-      <c r="X35" s="98"/>
-      <c r="Y35" s="99"/>
-      <c r="Z35" s="99"/>
-      <c r="AA35" s="99"/>
+      <c r="X35" s="144"/>
+      <c r="Y35" s="105"/>
+      <c r="Z35" s="105"/>
+      <c r="AA35" s="105"/>
       <c r="AB35" s="26"/>
     </row>
     <row r="36" spans="1:29" ht="18.75" customHeight="1">
@@ -3813,34 +3830,34 @@
     <row r="40" spans="1:29" ht="39.75" customHeight="1">
       <c r="A40" s="26"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="113" t="s">
+      <c r="C40" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="99"/>
-      <c r="E40" s="99"/>
-      <c r="F40" s="99"/>
-      <c r="G40" s="99"/>
-      <c r="H40" s="99"/>
-      <c r="I40" s="99"/>
-      <c r="J40" s="99"/>
-      <c r="K40" s="99"/>
-      <c r="L40" s="99"/>
-      <c r="M40" s="99"/>
-      <c r="N40" s="99"/>
-      <c r="O40" s="99"/>
-      <c r="P40" s="99"/>
-      <c r="Q40" s="99"/>
-      <c r="R40" s="99"/>
-      <c r="S40" s="99"/>
-      <c r="T40" s="99"/>
-      <c r="U40" s="99"/>
-      <c r="V40" s="99"/>
-      <c r="W40" s="99"/>
-      <c r="X40" s="99"/>
-      <c r="Y40" s="99"/>
-      <c r="Z40" s="99"/>
-      <c r="AA40" s="99"/>
-      <c r="AB40" s="114"/>
+      <c r="D40" s="105"/>
+      <c r="E40" s="105"/>
+      <c r="F40" s="105"/>
+      <c r="G40" s="105"/>
+      <c r="H40" s="105"/>
+      <c r="I40" s="105"/>
+      <c r="J40" s="105"/>
+      <c r="K40" s="105"/>
+      <c r="L40" s="105"/>
+      <c r="M40" s="105"/>
+      <c r="N40" s="105"/>
+      <c r="O40" s="105"/>
+      <c r="P40" s="105"/>
+      <c r="Q40" s="105"/>
+      <c r="R40" s="105"/>
+      <c r="S40" s="105"/>
+      <c r="T40" s="105"/>
+      <c r="U40" s="105"/>
+      <c r="V40" s="105"/>
+      <c r="W40" s="105"/>
+      <c r="X40" s="105"/>
+      <c r="Y40" s="105"/>
+      <c r="Z40" s="105"/>
+      <c r="AA40" s="105"/>
+      <c r="AB40" s="143"/>
     </row>
     <row r="41" spans="1:29" ht="11.25" customHeight="1">
       <c r="A41" s="26"/>
@@ -3919,14 +3936,14 @@
       <c r="C46" s="53"/>
     </row>
     <row r="47" spans="1:29" ht="15" customHeight="1">
-      <c r="B47" s="105" t="s">
+      <c r="B47" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="106"/>
-      <c r="D47" s="106"/>
-      <c r="E47" s="106"/>
-      <c r="F47" s="106"/>
-      <c r="G47" s="106"/>
+      <c r="C47" s="101"/>
+      <c r="D47" s="101"/>
+      <c r="E47" s="101"/>
+      <c r="F47" s="101"/>
+      <c r="G47" s="101"/>
       <c r="J47" s="17"/>
       <c r="K47" s="55" t="s">
         <v>33</v>
@@ -3946,17 +3963,17 @@
       </c>
       <c r="D50" s="59"/>
       <c r="E50" s="59"/>
-      <c r="F50" s="107"/>
-      <c r="G50" s="108"/>
-      <c r="H50" s="108"/>
+      <c r="F50" s="138"/>
+      <c r="G50" s="112"/>
+      <c r="H50" s="112"/>
       <c r="J50" s="60"/>
       <c r="K50" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="N50" s="107"/>
-      <c r="O50" s="108"/>
-      <c r="P50" s="108"/>
-      <c r="Q50" s="108"/>
+      <c r="N50" s="138"/>
+      <c r="O50" s="112"/>
+      <c r="P50" s="112"/>
+      <c r="Q50" s="112"/>
     </row>
     <row r="51" spans="1:17" ht="12" customHeight="1">
       <c r="F51" s="58"/>
@@ -34124,12 +34141,57 @@
       <c r="B994" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="Y22:AB22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="X23:AA23"/>
+  <mergeCells count="73">
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="X35:AA35"/>
+    <mergeCell ref="X28:AA28"/>
+    <mergeCell ref="X30:AA30"/>
+    <mergeCell ref="X31:AA31"/>
+    <mergeCell ref="X33:AA33"/>
+    <mergeCell ref="X34:AA34"/>
+    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="X25:AA25"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="X32:AA32"/>
+    <mergeCell ref="C40:AB40"/>
+    <mergeCell ref="N50:Q50"/>
+    <mergeCell ref="X26:AA26"/>
+    <mergeCell ref="X27:AA27"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="G2:Q2"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="G3:Q3"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="B6:AB6"/>
+    <mergeCell ref="O19:W20"/>
+    <mergeCell ref="B7:AB7"/>
+    <mergeCell ref="B8:AB8"/>
+    <mergeCell ref="B10:AB10"/>
+    <mergeCell ref="B11:AB11"/>
+    <mergeCell ref="B12:AB12"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="X24:AA24"/>
     <mergeCell ref="B13:AB13"/>
@@ -34146,47 +34208,13 @@
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="C19:E22"/>
     <mergeCell ref="F19:F22"/>
-    <mergeCell ref="O19:W20"/>
-    <mergeCell ref="B7:AB7"/>
-    <mergeCell ref="B8:AB8"/>
-    <mergeCell ref="B10:AB10"/>
-    <mergeCell ref="B11:AB11"/>
-    <mergeCell ref="B12:AB12"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="B6:AB6"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="G3:Q3"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="X25:AA25"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="X32:AA32"/>
-    <mergeCell ref="C40:AB40"/>
-    <mergeCell ref="N50:Q50"/>
-    <mergeCell ref="X26:AA26"/>
-    <mergeCell ref="X27:AA27"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="X35:AA35"/>
-    <mergeCell ref="X28:AA28"/>
-    <mergeCell ref="X30:AA30"/>
-    <mergeCell ref="X31:AA31"/>
-    <mergeCell ref="X33:AA33"/>
-    <mergeCell ref="X34:AA34"/>
-    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="Y22:AB22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="X23:AA23"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
   </mergeCells>
   <conditionalFormatting sqref="F49:G50">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
@@ -34215,12 +34243,13 @@
   </sheetPr>
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.140625" customWidth="1"/>
     <col min="6" max="6" width="22.140625" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
@@ -34228,66 +34257,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="149" t="s">
-        <v>81</v>
+      <c r="A2" s="146" t="s">
+        <v>85</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="150"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="147"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="151"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="114"/>
+      <c r="A3" s="148"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="143"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="151"/>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="114"/>
+      <c r="A4" s="148"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="143"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="151"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="114"/>
+      <c r="A5" s="148"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="143"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="151"/>
-      <c r="B6" s="99"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="114"/>
+      <c r="A6" s="148"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="143"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="152"/>
-      <c r="B7" s="153"/>
-      <c r="C7" s="153"/>
-      <c r="D7" s="153"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="154"/>
+      <c r="A7" s="149"/>
+      <c r="B7" s="150"/>
+      <c r="C7" s="150"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150"/>
+      <c r="G7" s="150"/>
+      <c r="H7" s="151"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="61"/>
@@ -34320,8 +34349,8 @@
         <v>1</v>
       </c>
       <c r="F10" s="61"/>
-      <c r="G10" s="155"/>
-      <c r="H10" s="156"/>
+      <c r="G10" s="152"/>
+      <c r="H10" s="153"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="61"/>
@@ -34334,12 +34363,12 @@
         <v>45644</v>
       </c>
       <c r="F11" s="61"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="61" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="61"/>
@@ -34382,15 +34411,15 @@
         <v>44</v>
       </c>
       <c r="H14" s="72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="122.25" customHeight="1">
-      <c r="A15" s="157" t="s">
+      <c r="A15" s="154" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="75" t="s">
         <v>46</v>
@@ -34399,44 +34428,44 @@
         <v>47</v>
       </c>
       <c r="E15" s="77" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
-      <c r="F15" s="97" t="s">
-        <v>63</v>
+      <c r="F15" s="94" t="s">
+        <v>62</v>
       </c>
-      <c r="G15" s="95" t="s">
-        <v>78</v>
+      <c r="G15" s="92" t="s">
+        <v>77</v>
       </c>
       <c r="H15" s="78" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="141.75" customHeight="1">
-      <c r="A16" s="158"/>
+      <c r="A16" s="155"/>
       <c r="B16" s="74">
         <v>45665</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="D16" s="76" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="77" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
-      <c r="F16" s="97" t="s">
-        <v>63</v>
+      <c r="F16" s="94" t="s">
+        <v>62</v>
       </c>
-      <c r="G16" s="95" t="s">
-        <v>78</v>
+      <c r="G16" s="92" t="s">
+        <v>77</v>
       </c>
       <c r="H16" s="79" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="165" customHeight="1">
-      <c r="A17" s="158"/>
+      <c r="A17" s="155"/>
       <c r="B17" s="74">
         <v>45667</v>
       </c>
@@ -34447,41 +34476,20 @@
         <v>47</v>
       </c>
       <c r="E17" s="77" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
-      <c r="F17" s="97" t="s">
-        <v>63</v>
+      <c r="F17" s="94" t="s">
+        <v>62</v>
       </c>
-      <c r="G17" s="95" t="s">
+      <c r="G17" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="80" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="132">
-      <c r="A18" s="158"/>
-      <c r="B18" s="74">
-        <v>45668</v>
-      </c>
-      <c r="C18" s="75" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="76" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="97" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="96" t="s">
-        <v>79</v>
-      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.75">
+      <c r="A18" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -34495,23 +34503,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EDB39E34F5A9B445B025C05B2A05D030" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c21ef800502b5dc1190a9a0361733939">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f1f31ffb-9912-4459-99c8-b26e82094b51" xmlns:ns4="ce621958-37b1-43fe-a1f1-1aad67996a88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30daf50bb6192471b76b9808b4256f50" ns3:_="" ns4:_="">
     <xsd:import namespace="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
@@ -34706,32 +34697,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D01A9D5D-1824-48C2-8527-9D8749A8DDDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34748,4 +34731,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correción año a 2025
</commit_message>
<xml_diff>
--- a/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
+++ b/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATIAS\Desktop\ESPE\Septimo_Semestre\Quality Assurance\Repo\2563_G3_ACSW\02_Proyecto\09. Programa de Auditoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229D6D04-794D-48B0-B515-6A042A38C3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B42AF92-C11C-48B5-9A6A-2C9A8225B4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>Fecha de Emisión:</t>
   </si>
@@ -416,9 +416,6 @@
   </si>
   <si>
     <t>27</t>
-  </si>
-  <si>
-    <t>06/01/20225</t>
   </si>
   <si>
     <t>17:00
@@ -1566,29 +1563,93 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1596,18 +1657,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1624,62 +1675,26 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1695,24 +1710,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1975,7 +1972,7 @@
   </sheetPr>
   <dimension ref="A1:AW994"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A30" zoomScale="64" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="64" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:AB8"/>
     </sheetView>
   </sheetViews>
@@ -2009,37 +2006,37 @@
     </row>
     <row r="2" spans="1:48" ht="42.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="133"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="131" t="s">
+      <c r="B2" s="114"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="135"/>
-      <c r="T2" s="135"/>
-      <c r="U2" s="135"/>
-      <c r="V2" s="135"/>
-      <c r="W2" s="98"/>
-      <c r="X2" s="98"/>
-      <c r="Y2" s="99"/>
-      <c r="Z2" s="131" t="s">
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="100"/>
+      <c r="X2" s="100"/>
+      <c r="Y2" s="101"/>
+      <c r="Z2" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="AA2" s="98"/>
-      <c r="AB2" s="99"/>
+      <c r="AA2" s="100"/>
+      <c r="AB2" s="101"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -2063,37 +2060,37 @@
     </row>
     <row r="3" spans="1:48" ht="48.75" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="111"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="99"/>
-      <c r="R3" s="129" t="s">
+      <c r="B3" s="115"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="130"/>
-      <c r="T3" s="130"/>
-      <c r="U3" s="130"/>
-      <c r="V3" s="130"/>
-      <c r="W3" s="98"/>
-      <c r="X3" s="98"/>
-      <c r="Y3" s="99"/>
-      <c r="Z3" s="131" t="s">
+      <c r="S3" s="122"/>
+      <c r="T3" s="122"/>
+      <c r="U3" s="122"/>
+      <c r="V3" s="122"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" s="98"/>
-      <c r="AB3" s="99"/>
+      <c r="AA3" s="100"/>
+      <c r="AB3" s="101"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
@@ -2117,39 +2114,39 @@
     </row>
     <row r="4" spans="1:48" ht="21" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="127" t="s">
+      <c r="B4" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="98"/>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="129" t="s">
-        <v>79</v>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
+      <c r="O4" s="100"/>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="121" t="s">
+        <v>78</v>
       </c>
-      <c r="S4" s="130"/>
-      <c r="T4" s="130"/>
-      <c r="U4" s="130"/>
-      <c r="V4" s="130"/>
-      <c r="W4" s="98"/>
-      <c r="X4" s="98"/>
-      <c r="Y4" s="99"/>
-      <c r="Z4" s="131" t="s">
+      <c r="S4" s="122"/>
+      <c r="T4" s="122"/>
+      <c r="U4" s="122"/>
+      <c r="V4" s="122"/>
+      <c r="W4" s="100"/>
+      <c r="X4" s="100"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="98"/>
-      <c r="AB4" s="99"/>
+      <c r="AA4" s="100"/>
+      <c r="AB4" s="101"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
@@ -2222,35 +2219,35 @@
       <c r="AV5" s="2"/>
     </row>
     <row r="6" spans="1:48" ht="50.25" customHeight="1">
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="125" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="105"/>
-      <c r="P6" s="105"/>
-      <c r="Q6" s="105"/>
-      <c r="R6" s="105"/>
-      <c r="S6" s="105"/>
-      <c r="T6" s="105"/>
-      <c r="U6" s="105"/>
-      <c r="V6" s="105"/>
-      <c r="W6" s="105"/>
-      <c r="X6" s="105"/>
-      <c r="Y6" s="105"/>
-      <c r="Z6" s="105"/>
-      <c r="AA6" s="105"/>
-      <c r="AB6" s="105"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
+      <c r="O6" s="98"/>
+      <c r="P6" s="98"/>
+      <c r="Q6" s="98"/>
+      <c r="R6" s="98"/>
+      <c r="S6" s="98"/>
+      <c r="T6" s="98"/>
+      <c r="U6" s="98"/>
+      <c r="V6" s="98"/>
+      <c r="W6" s="98"/>
+      <c r="X6" s="98"/>
+      <c r="Y6" s="98"/>
+      <c r="Z6" s="98"/>
+      <c r="AA6" s="98"/>
+      <c r="AB6" s="98"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="6"/>
@@ -2267,35 +2264,35 @@
       <c r="AP6" s="7"/>
     </row>
     <row r="7" spans="1:48" ht="198" customHeight="1">
-      <c r="B7" s="104" t="s">
-        <v>84</v>
+      <c r="B7" s="132" t="s">
+        <v>83</v>
       </c>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="105"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="105"/>
-      <c r="L7" s="105"/>
-      <c r="M7" s="105"/>
-      <c r="N7" s="105"/>
-      <c r="O7" s="105"/>
-      <c r="P7" s="105"/>
-      <c r="Q7" s="105"/>
-      <c r="R7" s="105"/>
-      <c r="S7" s="105"/>
-      <c r="T7" s="105"/>
-      <c r="U7" s="105"/>
-      <c r="V7" s="105"/>
-      <c r="W7" s="105"/>
-      <c r="X7" s="105"/>
-      <c r="Y7" s="105"/>
-      <c r="Z7" s="105"/>
-      <c r="AA7" s="105"/>
-      <c r="AB7" s="105"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="98"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="98"/>
+      <c r="U7" s="98"/>
+      <c r="V7" s="98"/>
+      <c r="W7" s="98"/>
+      <c r="X7" s="98"/>
+      <c r="Y7" s="98"/>
+      <c r="Z7" s="98"/>
+      <c r="AA7" s="98"/>
+      <c r="AB7" s="98"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
       <c r="AE7" s="6"/>
@@ -2312,35 +2309,35 @@
       <c r="AP7" s="7"/>
     </row>
     <row r="8" spans="1:48" ht="51" customHeight="1">
-      <c r="B8" s="126" t="s">
+      <c r="B8" s="133" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="105"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="105"/>
-      <c r="O8" s="105"/>
-      <c r="P8" s="105"/>
-      <c r="Q8" s="105"/>
-      <c r="R8" s="105"/>
-      <c r="S8" s="105"/>
-      <c r="T8" s="105"/>
-      <c r="U8" s="105"/>
-      <c r="V8" s="105"/>
-      <c r="W8" s="105"/>
-      <c r="X8" s="105"/>
-      <c r="Y8" s="105"/>
-      <c r="Z8" s="105"/>
-      <c r="AA8" s="105"/>
-      <c r="AB8" s="105"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="98"/>
+      <c r="S8" s="98"/>
+      <c r="T8" s="98"/>
+      <c r="U8" s="98"/>
+      <c r="V8" s="98"/>
+      <c r="W8" s="98"/>
+      <c r="X8" s="98"/>
+      <c r="Y8" s="98"/>
+      <c r="Z8" s="98"/>
+      <c r="AA8" s="98"/>
+      <c r="AB8" s="98"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="6"/>
@@ -2400,35 +2397,35 @@
       <c r="AP9" s="7"/>
     </row>
     <row r="10" spans="1:48" ht="20.25" customHeight="1">
-      <c r="B10" s="126" t="s">
+      <c r="B10" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="105"/>
-      <c r="J10" s="105"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="105"/>
-      <c r="M10" s="105"/>
-      <c r="N10" s="105"/>
-      <c r="O10" s="105"/>
-      <c r="P10" s="105"/>
-      <c r="Q10" s="105"/>
-      <c r="R10" s="105"/>
-      <c r="S10" s="105"/>
-      <c r="T10" s="105"/>
-      <c r="U10" s="105"/>
-      <c r="V10" s="105"/>
-      <c r="W10" s="105"/>
-      <c r="X10" s="105"/>
-      <c r="Y10" s="105"/>
-      <c r="Z10" s="105"/>
-      <c r="AA10" s="105"/>
-      <c r="AB10" s="105"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="98"/>
+      <c r="O10" s="98"/>
+      <c r="P10" s="98"/>
+      <c r="Q10" s="98"/>
+      <c r="R10" s="98"/>
+      <c r="S10" s="98"/>
+      <c r="T10" s="98"/>
+      <c r="U10" s="98"/>
+      <c r="V10" s="98"/>
+      <c r="W10" s="98"/>
+      <c r="X10" s="98"/>
+      <c r="Y10" s="98"/>
+      <c r="Z10" s="98"/>
+      <c r="AA10" s="98"/>
+      <c r="AB10" s="98"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="6"/>
@@ -2446,35 +2443,35 @@
     </row>
     <row r="11" spans="1:48" ht="60" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="104" t="s">
+      <c r="B11" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="105"/>
-      <c r="J11" s="105"/>
-      <c r="K11" s="105"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="105"/>
-      <c r="O11" s="105"/>
-      <c r="P11" s="105"/>
-      <c r="Q11" s="105"/>
-      <c r="R11" s="105"/>
-      <c r="S11" s="105"/>
-      <c r="T11" s="105"/>
-      <c r="U11" s="105"/>
-      <c r="V11" s="105"/>
-      <c r="W11" s="105"/>
-      <c r="X11" s="105"/>
-      <c r="Y11" s="105"/>
-      <c r="Z11" s="105"/>
-      <c r="AA11" s="105"/>
-      <c r="AB11" s="105"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="98"/>
+      <c r="P11" s="98"/>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="98"/>
+      <c r="T11" s="98"/>
+      <c r="U11" s="98"/>
+      <c r="V11" s="98"/>
+      <c r="W11" s="98"/>
+      <c r="X11" s="98"/>
+      <c r="Y11" s="98"/>
+      <c r="Z11" s="98"/>
+      <c r="AA11" s="98"/>
+      <c r="AB11" s="98"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="9"/>
       <c r="AE11" s="9"/>
@@ -2497,35 +2494,35 @@
       <c r="AV11" s="8"/>
     </row>
     <row r="12" spans="1:48" ht="53.25" customHeight="1">
-      <c r="B12" s="104" t="s">
+      <c r="B12" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="105"/>
-      <c r="I12" s="105"/>
-      <c r="J12" s="105"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="105"/>
-      <c r="M12" s="105"/>
-      <c r="N12" s="105"/>
-      <c r="O12" s="105"/>
-      <c r="P12" s="105"/>
-      <c r="Q12" s="105"/>
-      <c r="R12" s="105"/>
-      <c r="S12" s="105"/>
-      <c r="T12" s="105"/>
-      <c r="U12" s="105"/>
-      <c r="V12" s="105"/>
-      <c r="W12" s="105"/>
-      <c r="X12" s="105"/>
-      <c r="Y12" s="105"/>
-      <c r="Z12" s="105"/>
-      <c r="AA12" s="105"/>
-      <c r="AB12" s="105"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="98"/>
+      <c r="P12" s="98"/>
+      <c r="Q12" s="98"/>
+      <c r="R12" s="98"/>
+      <c r="S12" s="98"/>
+      <c r="T12" s="98"/>
+      <c r="U12" s="98"/>
+      <c r="V12" s="98"/>
+      <c r="W12" s="98"/>
+      <c r="X12" s="98"/>
+      <c r="Y12" s="98"/>
+      <c r="Z12" s="98"/>
+      <c r="AA12" s="98"/>
+      <c r="AB12" s="98"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
@@ -2542,35 +2539,35 @@
       <c r="AP12" s="7"/>
     </row>
     <row r="13" spans="1:48" ht="39.75" customHeight="1">
-      <c r="B13" s="104" t="s">
+      <c r="B13" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="105"/>
-      <c r="O13" s="105"/>
-      <c r="P13" s="105"/>
-      <c r="Q13" s="105"/>
-      <c r="R13" s="105"/>
-      <c r="S13" s="105"/>
-      <c r="T13" s="105"/>
-      <c r="U13" s="105"/>
-      <c r="V13" s="105"/>
-      <c r="W13" s="105"/>
-      <c r="X13" s="105"/>
-      <c r="Y13" s="105"/>
-      <c r="Z13" s="105"/>
-      <c r="AA13" s="105"/>
-      <c r="AB13" s="105"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="98"/>
+      <c r="Q13" s="98"/>
+      <c r="R13" s="98"/>
+      <c r="S13" s="98"/>
+      <c r="T13" s="98"/>
+      <c r="U13" s="98"/>
+      <c r="V13" s="98"/>
+      <c r="W13" s="98"/>
+      <c r="X13" s="98"/>
+      <c r="Y13" s="98"/>
+      <c r="Z13" s="98"/>
+      <c r="AA13" s="98"/>
+      <c r="AB13" s="98"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
@@ -2630,35 +2627,35 @@
       <c r="AP14" s="7"/>
     </row>
     <row r="15" spans="1:48" ht="99.75" customHeight="1">
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="105"/>
-      <c r="O15" s="105"/>
-      <c r="P15" s="105"/>
-      <c r="Q15" s="105"/>
-      <c r="R15" s="105"/>
-      <c r="S15" s="105"/>
-      <c r="T15" s="105"/>
-      <c r="U15" s="105"/>
-      <c r="V15" s="105"/>
-      <c r="W15" s="105"/>
-      <c r="X15" s="105"/>
-      <c r="Y15" s="105"/>
-      <c r="Z15" s="105"/>
-      <c r="AA15" s="105"/>
-      <c r="AB15" s="105"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="98"/>
+      <c r="P15" s="98"/>
+      <c r="Q15" s="98"/>
+      <c r="R15" s="98"/>
+      <c r="S15" s="98"/>
+      <c r="T15" s="98"/>
+      <c r="U15" s="98"/>
+      <c r="V15" s="98"/>
+      <c r="W15" s="98"/>
+      <c r="X15" s="98"/>
+      <c r="Y15" s="98"/>
+      <c r="Z15" s="98"/>
+      <c r="AA15" s="98"/>
+      <c r="AB15" s="98"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="6"/>
@@ -2676,35 +2673,35 @@
     </row>
     <row r="16" spans="1:48" ht="24.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="107" t="s">
+      <c r="B16" s="135" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="105"/>
-      <c r="N16" s="105"/>
-      <c r="O16" s="105"/>
-      <c r="P16" s="105"/>
-      <c r="Q16" s="105"/>
-      <c r="R16" s="105"/>
-      <c r="S16" s="105"/>
-      <c r="T16" s="105"/>
-      <c r="U16" s="105"/>
-      <c r="V16" s="105"/>
-      <c r="W16" s="105"/>
-      <c r="X16" s="105"/>
-      <c r="Y16" s="105"/>
-      <c r="Z16" s="105"/>
-      <c r="AA16" s="105"/>
-      <c r="AB16" s="105"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="98"/>
+      <c r="P16" s="98"/>
+      <c r="Q16" s="98"/>
+      <c r="R16" s="98"/>
+      <c r="S16" s="98"/>
+      <c r="T16" s="98"/>
+      <c r="U16" s="98"/>
+      <c r="V16" s="98"/>
+      <c r="W16" s="98"/>
+      <c r="X16" s="98"/>
+      <c r="Y16" s="98"/>
+      <c r="Z16" s="98"/>
+      <c r="AA16" s="98"/>
+      <c r="AB16" s="98"/>
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
@@ -2727,35 +2724,35 @@
       <c r="AV16" s="2"/>
     </row>
     <row r="17" spans="1:49" ht="24.75" customHeight="1">
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
-      <c r="J17" s="105"/>
-      <c r="K17" s="105"/>
-      <c r="L17" s="105"/>
-      <c r="M17" s="105"/>
-      <c r="N17" s="105"/>
-      <c r="O17" s="105"/>
-      <c r="P17" s="105"/>
-      <c r="Q17" s="105"/>
-      <c r="R17" s="105"/>
-      <c r="S17" s="105"/>
-      <c r="T17" s="105"/>
-      <c r="U17" s="105"/>
-      <c r="V17" s="105"/>
-      <c r="W17" s="105"/>
-      <c r="X17" s="105"/>
-      <c r="Y17" s="105"/>
-      <c r="Z17" s="105"/>
-      <c r="AA17" s="105"/>
-      <c r="AB17" s="105"/>
+      <c r="C17" s="98"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="98"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="98"/>
+      <c r="P17" s="98"/>
+      <c r="Q17" s="98"/>
+      <c r="R17" s="98"/>
+      <c r="S17" s="98"/>
+      <c r="T17" s="98"/>
+      <c r="U17" s="98"/>
+      <c r="V17" s="98"/>
+      <c r="W17" s="98"/>
+      <c r="X17" s="98"/>
+      <c r="Y17" s="98"/>
+      <c r="Z17" s="98"/>
+      <c r="AA17" s="98"/>
+      <c r="AB17" s="98"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="6"/>
@@ -2772,33 +2769,33 @@
       <c r="AP17" s="7"/>
     </row>
     <row r="18" spans="1:49" ht="6.75" customHeight="1">
-      <c r="B18" s="106"/>
-      <c r="C18" s="105"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="105"/>
-      <c r="I18" s="105"/>
-      <c r="J18" s="105"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="105"/>
-      <c r="N18" s="105"/>
-      <c r="O18" s="105"/>
-      <c r="P18" s="105"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="105"/>
-      <c r="S18" s="105"/>
-      <c r="T18" s="105"/>
-      <c r="U18" s="105"/>
-      <c r="V18" s="105"/>
-      <c r="W18" s="105"/>
-      <c r="X18" s="105"/>
-      <c r="Y18" s="105"/>
-      <c r="Z18" s="105"/>
-      <c r="AA18" s="105"/>
-      <c r="AB18" s="105"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="98"/>
+      <c r="O18" s="98"/>
+      <c r="P18" s="98"/>
+      <c r="Q18" s="98"/>
+      <c r="R18" s="98"/>
+      <c r="S18" s="98"/>
+      <c r="T18" s="98"/>
+      <c r="U18" s="98"/>
+      <c r="V18" s="98"/>
+      <c r="W18" s="98"/>
+      <c r="X18" s="98"/>
+      <c r="Y18" s="98"/>
+      <c r="Z18" s="98"/>
+      <c r="AA18" s="98"/>
+      <c r="AB18" s="98"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
@@ -2816,44 +2813,44 @@
     </row>
     <row r="19" spans="1:49" ht="36.75" customHeight="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="118" t="s">
+      <c r="B19" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="121" t="s">
+      <c r="C19" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="109"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="122" t="s">
+      <c r="D19" s="127"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="142" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="108" t="s">
+      <c r="G19" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="109"/>
-      <c r="I19" s="109"/>
-      <c r="J19" s="109"/>
-      <c r="K19" s="109"/>
-      <c r="L19" s="109"/>
-      <c r="M19" s="109"/>
-      <c r="N19" s="110"/>
-      <c r="O19" s="108" t="s">
+      <c r="H19" s="127"/>
+      <c r="I19" s="127"/>
+      <c r="J19" s="127"/>
+      <c r="K19" s="127"/>
+      <c r="L19" s="127"/>
+      <c r="M19" s="127"/>
+      <c r="N19" s="128"/>
+      <c r="O19" s="126" t="s">
         <v>54</v>
       </c>
-      <c r="P19" s="109"/>
-      <c r="Q19" s="109"/>
-      <c r="R19" s="109"/>
-      <c r="S19" s="109"/>
-      <c r="T19" s="109"/>
-      <c r="U19" s="109"/>
-      <c r="V19" s="109"/>
-      <c r="W19" s="110"/>
-      <c r="X19" s="114" t="s">
+      <c r="P19" s="127"/>
+      <c r="Q19" s="127"/>
+      <c r="R19" s="127"/>
+      <c r="S19" s="127"/>
+      <c r="T19" s="127"/>
+      <c r="U19" s="127"/>
+      <c r="V19" s="127"/>
+      <c r="W19" s="128"/>
+      <c r="X19" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="Y19" s="109"/>
-      <c r="Z19" s="109"/>
-      <c r="AA19" s="110"/>
+      <c r="Y19" s="127"/>
+      <c r="Z19" s="127"/>
+      <c r="AA19" s="128"/>
       <c r="AB19" s="83" t="s">
         <v>9</v>
       </c>
@@ -2880,32 +2877,32 @@
     </row>
     <row r="20" spans="1:49" ht="10.5" customHeight="1">
       <c r="A20" s="14"/>
-      <c r="B20" s="119"/>
-      <c r="C20" s="115"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="112"/>
-      <c r="K20" s="112"/>
-      <c r="L20" s="112"/>
-      <c r="M20" s="112"/>
-      <c r="N20" s="113"/>
-      <c r="O20" s="115"/>
-      <c r="P20" s="125"/>
-      <c r="Q20" s="125"/>
-      <c r="R20" s="125"/>
-      <c r="S20" s="125"/>
-      <c r="T20" s="125"/>
-      <c r="U20" s="125"/>
-      <c r="V20" s="125"/>
-      <c r="W20" s="116"/>
-      <c r="X20" s="115"/>
-      <c r="Y20" s="105"/>
-      <c r="Z20" s="105"/>
-      <c r="AA20" s="116"/>
+      <c r="B20" s="139"/>
+      <c r="C20" s="129"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="131"/>
+      <c r="F20" s="143"/>
+      <c r="G20" s="115"/>
+      <c r="H20" s="107"/>
+      <c r="I20" s="107"/>
+      <c r="J20" s="107"/>
+      <c r="K20" s="107"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="107"/>
+      <c r="N20" s="116"/>
+      <c r="O20" s="129"/>
+      <c r="P20" s="130"/>
+      <c r="Q20" s="130"/>
+      <c r="R20" s="130"/>
+      <c r="S20" s="130"/>
+      <c r="T20" s="130"/>
+      <c r="U20" s="130"/>
+      <c r="V20" s="130"/>
+      <c r="W20" s="131"/>
+      <c r="X20" s="129"/>
+      <c r="Y20" s="98"/>
+      <c r="Z20" s="98"/>
+      <c r="AA20" s="131"/>
       <c r="AB20" s="84"/>
       <c r="AC20" s="14"/>
       <c r="AD20" s="14"/>
@@ -2930,37 +2927,37 @@
     </row>
     <row r="21" spans="1:49" ht="34.5" customHeight="1">
       <c r="A21" s="15"/>
-      <c r="B21" s="119"/>
-      <c r="C21" s="115"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="116"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="117" t="s">
+      <c r="B21" s="139"/>
+      <c r="C21" s="129"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="131"/>
+      <c r="F21" s="143"/>
+      <c r="G21" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="99"/>
-      <c r="I21" s="117" t="s">
+      <c r="H21" s="101"/>
+      <c r="I21" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="99"/>
-      <c r="K21" s="117" t="s">
+      <c r="J21" s="101"/>
+      <c r="K21" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="99"/>
-      <c r="M21" s="117" t="s">
+      <c r="L21" s="101"/>
+      <c r="M21" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="98"/>
-      <c r="O21" s="96" t="s">
+      <c r="N21" s="100"/>
+      <c r="O21" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="95" t="s">
+      <c r="P21" s="146"/>
+      <c r="Q21" s="146"/>
+      <c r="R21" s="146"/>
+      <c r="S21" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="T21" s="96"/>
+      <c r="T21" s="146"/>
       <c r="U21" s="91" t="s">
         <v>12</v>
       </c>
@@ -2968,10 +2965,10 @@
         <v>13</v>
       </c>
       <c r="W21" s="87"/>
-      <c r="X21" s="112"/>
-      <c r="Y21" s="112"/>
-      <c r="Z21" s="112"/>
-      <c r="AA21" s="113"/>
+      <c r="X21" s="107"/>
+      <c r="Y21" s="107"/>
+      <c r="Z21" s="107"/>
+      <c r="AA21" s="116"/>
       <c r="AB21" s="84"/>
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
@@ -2996,11 +2993,11 @@
     </row>
     <row r="22" spans="1:49" ht="38.25" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="111"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="124"/>
+      <c r="B22" s="140"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="144"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
@@ -3027,10 +3024,10 @@
       <c r="P22" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="Q22" s="156">
+      <c r="Q22" s="148">
         <v>10</v>
       </c>
-      <c r="R22" s="157"/>
+      <c r="R22" s="149"/>
       <c r="S22" s="88" t="s">
         <v>60</v>
       </c>
@@ -3045,10 +3042,10 @@
       </c>
       <c r="W22" s="86"/>
       <c r="X22" s="86"/>
-      <c r="Y22" s="97"/>
-      <c r="Z22" s="98"/>
-      <c r="AA22" s="98"/>
-      <c r="AB22" s="99"/>
+      <c r="Y22" s="147"/>
+      <c r="Z22" s="100"/>
+      <c r="AA22" s="100"/>
+      <c r="AB22" s="101"/>
       <c r="AC22" s="85"/>
       <c r="AD22" s="14"/>
       <c r="AE22" s="14"/>
@@ -3076,11 +3073,11 @@
       <c r="B23" s="18">
         <v>1</v>
       </c>
-      <c r="C23" s="100" t="s">
+      <c r="C23" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="101"/>
-      <c r="E23" s="102"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="109"/>
       <c r="F23" s="76">
         <v>1</v>
       </c>
@@ -3096,19 +3093,19 @@
       <c r="N23" s="21"/>
       <c r="O23" s="89"/>
       <c r="P23" s="89"/>
-      <c r="Q23" s="158"/>
-      <c r="R23" s="159"/>
+      <c r="Q23" s="150"/>
+      <c r="R23" s="151"/>
       <c r="S23" s="22"/>
       <c r="T23" s="22"/>
       <c r="U23" s="22"/>
       <c r="V23" s="22"/>
       <c r="W23" s="22"/>
-      <c r="X23" s="103" t="s">
+      <c r="X23" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="Y23" s="98"/>
-      <c r="Z23" s="98"/>
-      <c r="AA23" s="99"/>
+      <c r="Y23" s="100"/>
+      <c r="Z23" s="100"/>
+      <c r="AA23" s="101"/>
       <c r="AB23" s="23" t="s">
         <v>58</v>
       </c>
@@ -3138,11 +3135,11 @@
       <c r="B24" s="18">
         <v>2</v>
       </c>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="101"/>
-      <c r="E24" s="102"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="109"/>
       <c r="F24" s="76">
         <v>2</v>
       </c>
@@ -3160,21 +3157,21 @@
       <c r="P24" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Q24" s="160" t="s">
+      <c r="Q24" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="R24" s="161"/>
+      <c r="R24" s="96"/>
       <c r="S24" s="22"/>
       <c r="T24" s="22"/>
       <c r="U24" s="22"/>
       <c r="V24" s="22"/>
       <c r="W24" s="22"/>
-      <c r="X24" s="103" t="s">
-        <v>83</v>
+      <c r="X24" s="99" t="s">
+        <v>82</v>
       </c>
-      <c r="Y24" s="98"/>
-      <c r="Z24" s="98"/>
-      <c r="AA24" s="99"/>
+      <c r="Y24" s="100"/>
+      <c r="Z24" s="100"/>
+      <c r="AA24" s="101"/>
       <c r="AB24" s="23" t="s">
         <v>62</v>
       </c>
@@ -3204,11 +3201,11 @@
       <c r="B25" s="18">
         <v>3</v>
       </c>
-      <c r="C25" s="100" t="s">
+      <c r="C25" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="101"/>
-      <c r="E25" s="102"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="109"/>
       <c r="F25" s="76">
         <v>3</v>
       </c>
@@ -3222,8 +3219,8 @@
       <c r="N25" s="21"/>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
-      <c r="Q25" s="160"/>
-      <c r="R25" s="161"/>
+      <c r="Q25" s="95"/>
+      <c r="R25" s="96"/>
       <c r="S25" s="22" t="s">
         <v>20</v>
       </c>
@@ -3233,12 +3230,12 @@
       <c r="U25" s="22"/>
       <c r="V25" s="22"/>
       <c r="W25" s="22"/>
-      <c r="X25" s="103" t="s">
+      <c r="X25" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="Y25" s="98"/>
-      <c r="Z25" s="98"/>
-      <c r="AA25" s="99"/>
+      <c r="Y25" s="100"/>
+      <c r="Z25" s="100"/>
+      <c r="AA25" s="101"/>
       <c r="AB25" s="23" t="s">
         <v>63</v>
       </c>
@@ -3268,11 +3265,11 @@
       <c r="B26" s="18">
         <v>4</v>
       </c>
-      <c r="C26" s="100" t="s">
+      <c r="C26" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="101"/>
-      <c r="E26" s="102"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="109"/>
       <c r="F26" s="76">
         <v>4</v>
       </c>
@@ -3286,8 +3283,8 @@
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21"/>
-      <c r="Q26" s="160"/>
-      <c r="R26" s="161"/>
+      <c r="Q26" s="95"/>
+      <c r="R26" s="96"/>
       <c r="S26" s="22"/>
       <c r="T26" s="22"/>
       <c r="U26" s="22" t="s">
@@ -3295,12 +3292,12 @@
       </c>
       <c r="V26" s="22"/>
       <c r="W26" s="22"/>
-      <c r="X26" s="103" t="s">
+      <c r="X26" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Y26" s="98"/>
-      <c r="Z26" s="98"/>
-      <c r="AA26" s="99"/>
+      <c r="Y26" s="100"/>
+      <c r="Z26" s="100"/>
+      <c r="AA26" s="101"/>
       <c r="AB26" s="23" t="s">
         <v>58</v>
       </c>
@@ -3330,11 +3327,11 @@
       <c r="B27" s="18">
         <v>5</v>
       </c>
-      <c r="C27" s="100" t="s">
+      <c r="C27" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="101"/>
-      <c r="E27" s="102"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="109"/>
       <c r="F27" s="80">
         <v>5</v>
       </c>
@@ -3348,8 +3345,8 @@
       <c r="N27" s="21"/>
       <c r="O27" s="21"/>
       <c r="P27" s="21"/>
-      <c r="Q27" s="160"/>
-      <c r="R27" s="161"/>
+      <c r="Q27" s="95"/>
+      <c r="R27" s="96"/>
       <c r="S27" s="22"/>
       <c r="T27" s="22"/>
       <c r="U27" s="22"/>
@@ -3357,12 +3354,12 @@
         <v>20</v>
       </c>
       <c r="W27" s="22"/>
-      <c r="X27" s="103" t="s">
+      <c r="X27" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="Y27" s="98"/>
-      <c r="Z27" s="98"/>
-      <c r="AA27" s="99"/>
+      <c r="Y27" s="100"/>
+      <c r="Z27" s="100"/>
+      <c r="AA27" s="101"/>
       <c r="AB27" s="23" t="s">
         <v>62</v>
       </c>
@@ -3390,9 +3387,9 @@
     <row r="28" spans="1:49" ht="163.5" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="102"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="105"/>
+      <c r="E28" s="109"/>
       <c r="F28" s="81"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
@@ -3404,19 +3401,19 @@
       <c r="N28" s="21"/>
       <c r="O28" s="21"/>
       <c r="P28" s="21"/>
-      <c r="Q28" s="160"/>
-      <c r="R28" s="161"/>
+      <c r="Q28" s="95"/>
+      <c r="R28" s="96"/>
       <c r="S28" s="22"/>
       <c r="T28" s="22"/>
       <c r="U28" s="22"/>
       <c r="V28" s="22"/>
       <c r="W28" s="22"/>
-      <c r="X28" s="103" t="s">
+      <c r="X28" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="Y28" s="98"/>
-      <c r="Z28" s="98"/>
-      <c r="AA28" s="99"/>
+      <c r="Y28" s="100"/>
+      <c r="Z28" s="100"/>
+      <c r="AA28" s="101"/>
       <c r="AB28" s="23"/>
       <c r="AC28" s="17"/>
       <c r="AD28" s="17"/>
@@ -3442,9 +3439,9 @@
     <row r="29" spans="1:49" ht="209.25" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
-      <c r="C29" s="100"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="102"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="109"/>
       <c r="F29" s="19"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
@@ -3456,17 +3453,17 @@
       <c r="N29" s="25"/>
       <c r="O29" s="21"/>
       <c r="P29" s="21"/>
-      <c r="Q29" s="160"/>
-      <c r="R29" s="161"/>
+      <c r="Q29" s="95"/>
+      <c r="R29" s="96"/>
       <c r="S29" s="22"/>
       <c r="T29" s="22"/>
       <c r="U29" s="22"/>
       <c r="V29" s="22"/>
       <c r="W29" s="22"/>
-      <c r="X29" s="103"/>
-      <c r="Y29" s="98"/>
-      <c r="Z29" s="98"/>
-      <c r="AA29" s="99"/>
+      <c r="X29" s="99"/>
+      <c r="Y29" s="100"/>
+      <c r="Z29" s="100"/>
+      <c r="AA29" s="101"/>
       <c r="AB29" s="23"/>
       <c r="AC29" s="17"/>
       <c r="AD29" s="17"/>
@@ -3492,9 +3489,9 @@
     <row r="30" spans="1:49" ht="262.5" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
-      <c r="C30" s="100"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="102"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="105"/>
+      <c r="E30" s="109"/>
       <c r="F30" s="19"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -3506,17 +3503,17 @@
       <c r="N30" s="21"/>
       <c r="O30" s="25"/>
       <c r="P30" s="21"/>
-      <c r="Q30" s="160"/>
-      <c r="R30" s="161"/>
+      <c r="Q30" s="95"/>
+      <c r="R30" s="96"/>
       <c r="S30" s="22"/>
       <c r="T30" s="22"/>
       <c r="U30" s="22"/>
       <c r="V30" s="22"/>
       <c r="W30" s="22"/>
-      <c r="X30" s="103"/>
-      <c r="Y30" s="98"/>
-      <c r="Z30" s="98"/>
-      <c r="AA30" s="99"/>
+      <c r="X30" s="99"/>
+      <c r="Y30" s="100"/>
+      <c r="Z30" s="100"/>
+      <c r="AA30" s="101"/>
       <c r="AB30" s="23"/>
       <c r="AC30" s="17"/>
       <c r="AD30" s="17"/>
@@ -3542,9 +3539,9 @@
     <row r="31" spans="1:49" ht="90.75" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
-      <c r="C31" s="139"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="102"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="105"/>
+      <c r="E31" s="109"/>
       <c r="F31" s="19"/>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
@@ -3556,17 +3553,17 @@
       <c r="N31" s="21"/>
       <c r="O31" s="21"/>
       <c r="P31" s="21"/>
-      <c r="Q31" s="160"/>
-      <c r="R31" s="161"/>
+      <c r="Q31" s="95"/>
+      <c r="R31" s="96"/>
       <c r="S31" s="22"/>
       <c r="T31" s="22"/>
       <c r="U31" s="22"/>
       <c r="V31" s="22"/>
       <c r="W31" s="22"/>
-      <c r="X31" s="141"/>
-      <c r="Y31" s="98"/>
-      <c r="Z31" s="98"/>
-      <c r="AA31" s="99"/>
+      <c r="X31" s="102"/>
+      <c r="Y31" s="100"/>
+      <c r="Z31" s="100"/>
+      <c r="AA31" s="101"/>
       <c r="AB31" s="23"/>
       <c r="AC31" s="17"/>
       <c r="AD31" s="17"/>
@@ -3592,9 +3589,9 @@
     <row r="32" spans="1:49" ht="90.75" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
-      <c r="C32" s="140"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="99"/>
+      <c r="C32" s="111"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="101"/>
       <c r="F32" s="19"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
@@ -3606,17 +3603,17 @@
       <c r="N32" s="21"/>
       <c r="O32" s="21"/>
       <c r="P32" s="21"/>
-      <c r="Q32" s="160"/>
-      <c r="R32" s="161"/>
+      <c r="Q32" s="95"/>
+      <c r="R32" s="96"/>
       <c r="S32" s="22"/>
       <c r="T32" s="22"/>
       <c r="U32" s="22"/>
       <c r="V32" s="22"/>
       <c r="W32" s="22"/>
-      <c r="X32" s="141"/>
-      <c r="Y32" s="98"/>
-      <c r="Z32" s="98"/>
-      <c r="AA32" s="99"/>
+      <c r="X32" s="102"/>
+      <c r="Y32" s="100"/>
+      <c r="Z32" s="100"/>
+      <c r="AA32" s="101"/>
       <c r="AB32" s="23"/>
       <c r="AC32" s="17"/>
       <c r="AD32" s="17"/>
@@ -3663,10 +3660,10 @@
       <c r="U33" s="29"/>
       <c r="V33" s="29"/>
       <c r="W33" s="29"/>
-      <c r="X33" s="145"/>
-      <c r="Y33" s="105"/>
-      <c r="Z33" s="105"/>
-      <c r="AA33" s="105"/>
+      <c r="X33" s="103"/>
+      <c r="Y33" s="98"/>
+      <c r="Z33" s="98"/>
+      <c r="AA33" s="98"/>
       <c r="AB33" s="30"/>
     </row>
     <row r="34" spans="1:29" ht="12.75" customHeight="1">
@@ -3693,10 +3690,10 @@
       <c r="U34" s="29"/>
       <c r="V34" s="29"/>
       <c r="W34" s="29"/>
-      <c r="X34" s="145"/>
-      <c r="Y34" s="105"/>
-      <c r="Z34" s="105"/>
-      <c r="AA34" s="105"/>
+      <c r="X34" s="103"/>
+      <c r="Y34" s="98"/>
+      <c r="Z34" s="98"/>
+      <c r="AA34" s="98"/>
       <c r="AB34" s="30"/>
     </row>
     <row r="35" spans="1:29" ht="19.5" customHeight="1">
@@ -3714,10 +3711,10 @@
       <c r="J35" s="17"/>
       <c r="O35" s="38"/>
       <c r="P35" s="38"/>
-      <c r="X35" s="144"/>
-      <c r="Y35" s="105"/>
-      <c r="Z35" s="105"/>
-      <c r="AA35" s="105"/>
+      <c r="X35" s="97"/>
+      <c r="Y35" s="98"/>
+      <c r="Z35" s="98"/>
+      <c r="AA35" s="98"/>
       <c r="AB35" s="26"/>
     </row>
     <row r="36" spans="1:29" ht="18.75" customHeight="1">
@@ -3830,34 +3827,34 @@
     <row r="40" spans="1:29" ht="39.75" customHeight="1">
       <c r="A40" s="26"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="142" t="s">
+      <c r="C40" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="105"/>
-      <c r="E40" s="105"/>
-      <c r="F40" s="105"/>
-      <c r="G40" s="105"/>
-      <c r="H40" s="105"/>
-      <c r="I40" s="105"/>
-      <c r="J40" s="105"/>
-      <c r="K40" s="105"/>
-      <c r="L40" s="105"/>
-      <c r="M40" s="105"/>
-      <c r="N40" s="105"/>
-      <c r="O40" s="105"/>
-      <c r="P40" s="105"/>
-      <c r="Q40" s="105"/>
-      <c r="R40" s="105"/>
-      <c r="S40" s="105"/>
-      <c r="T40" s="105"/>
-      <c r="U40" s="105"/>
-      <c r="V40" s="105"/>
-      <c r="W40" s="105"/>
-      <c r="X40" s="105"/>
-      <c r="Y40" s="105"/>
-      <c r="Z40" s="105"/>
-      <c r="AA40" s="105"/>
-      <c r="AB40" s="143"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="98"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="98"/>
+      <c r="H40" s="98"/>
+      <c r="I40" s="98"/>
+      <c r="J40" s="98"/>
+      <c r="K40" s="98"/>
+      <c r="L40" s="98"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="98"/>
+      <c r="O40" s="98"/>
+      <c r="P40" s="98"/>
+      <c r="Q40" s="98"/>
+      <c r="R40" s="98"/>
+      <c r="S40" s="98"/>
+      <c r="T40" s="98"/>
+      <c r="U40" s="98"/>
+      <c r="V40" s="98"/>
+      <c r="W40" s="98"/>
+      <c r="X40" s="98"/>
+      <c r="Y40" s="98"/>
+      <c r="Z40" s="98"/>
+      <c r="AA40" s="98"/>
+      <c r="AB40" s="113"/>
     </row>
     <row r="41" spans="1:29" ht="11.25" customHeight="1">
       <c r="A41" s="26"/>
@@ -3936,14 +3933,14 @@
       <c r="C46" s="53"/>
     </row>
     <row r="47" spans="1:29" ht="15" customHeight="1">
-      <c r="B47" s="137" t="s">
+      <c r="B47" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="101"/>
-      <c r="D47" s="101"/>
-      <c r="E47" s="101"/>
-      <c r="F47" s="101"/>
-      <c r="G47" s="101"/>
+      <c r="C47" s="105"/>
+      <c r="D47" s="105"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="105"/>
       <c r="J47" s="17"/>
       <c r="K47" s="55" t="s">
         <v>33</v>
@@ -3963,17 +3960,17 @@
       </c>
       <c r="D50" s="59"/>
       <c r="E50" s="59"/>
-      <c r="F50" s="138"/>
-      <c r="G50" s="112"/>
-      <c r="H50" s="112"/>
+      <c r="F50" s="106"/>
+      <c r="G50" s="107"/>
+      <c r="H50" s="107"/>
       <c r="J50" s="60"/>
       <c r="K50" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="N50" s="138"/>
-      <c r="O50" s="112"/>
-      <c r="P50" s="112"/>
-      <c r="Q50" s="112"/>
+      <c r="N50" s="106"/>
+      <c r="O50" s="107"/>
+      <c r="P50" s="107"/>
+      <c r="Q50" s="107"/>
     </row>
     <row r="51" spans="1:17" ht="12" customHeight="1">
       <c r="F51" s="58"/>
@@ -34142,22 +34139,47 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="X35:AA35"/>
-    <mergeCell ref="X28:AA28"/>
-    <mergeCell ref="X30:AA30"/>
-    <mergeCell ref="X31:AA31"/>
-    <mergeCell ref="X33:AA33"/>
-    <mergeCell ref="X34:AA34"/>
-    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="Y22:AB22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="X23:AA23"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="X24:AA24"/>
+    <mergeCell ref="B13:AB13"/>
+    <mergeCell ref="B15:AB15"/>
+    <mergeCell ref="B16:AB16"/>
+    <mergeCell ref="B17:AB17"/>
+    <mergeCell ref="G19:N20"/>
+    <mergeCell ref="X19:AA21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="B18:AB18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="O19:W20"/>
+    <mergeCell ref="B7:AB7"/>
+    <mergeCell ref="B8:AB8"/>
+    <mergeCell ref="B10:AB10"/>
+    <mergeCell ref="B11:AB11"/>
+    <mergeCell ref="B12:AB12"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="B6:AB6"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="G2:Q2"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="G3:Q3"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
     <mergeCell ref="X25:AA25"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="F50:H50"/>
@@ -34174,47 +34196,22 @@
     <mergeCell ref="X26:AA26"/>
     <mergeCell ref="X27:AA27"/>
     <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="G3:Q3"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="B6:AB6"/>
-    <mergeCell ref="O19:W20"/>
-    <mergeCell ref="B7:AB7"/>
-    <mergeCell ref="B8:AB8"/>
-    <mergeCell ref="B10:AB10"/>
-    <mergeCell ref="B11:AB11"/>
-    <mergeCell ref="B12:AB12"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="X24:AA24"/>
-    <mergeCell ref="B13:AB13"/>
-    <mergeCell ref="B15:AB15"/>
-    <mergeCell ref="B16:AB16"/>
-    <mergeCell ref="B17:AB17"/>
-    <mergeCell ref="G19:N20"/>
-    <mergeCell ref="X19:AA21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="B18:AB18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="Y22:AB22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="X23:AA23"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="X35:AA35"/>
+    <mergeCell ref="X28:AA28"/>
+    <mergeCell ref="X30:AA30"/>
+    <mergeCell ref="X31:AA31"/>
+    <mergeCell ref="X33:AA33"/>
+    <mergeCell ref="X34:AA34"/>
+    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
   </mergeCells>
   <conditionalFormatting sqref="F49:G50">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
@@ -34243,8 +34240,8 @@
   </sheetPr>
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -34257,66 +34254,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="146" t="s">
-        <v>85</v>
+      <c r="A2" s="152" t="s">
+        <v>84</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="147"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="148"/>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="143"/>
+      <c r="A3" s="154"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="113"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="148"/>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="143"/>
+      <c r="A4" s="154"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="113"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="143"/>
+      <c r="A5" s="154"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="113"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="148"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="143"/>
+      <c r="A6" s="154"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="113"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="149"/>
-      <c r="B7" s="150"/>
-      <c r="C7" s="150"/>
-      <c r="D7" s="150"/>
-      <c r="E7" s="150"/>
-      <c r="F7" s="150"/>
-      <c r="G7" s="150"/>
-      <c r="H7" s="151"/>
+      <c r="A7" s="155"/>
+      <c r="B7" s="156"/>
+      <c r="C7" s="156"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="156"/>
+      <c r="H7" s="157"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="61"/>
@@ -34349,8 +34346,8 @@
         <v>1</v>
       </c>
       <c r="F10" s="61"/>
-      <c r="G10" s="152"/>
-      <c r="H10" s="153"/>
+      <c r="G10" s="158"/>
+      <c r="H10" s="159"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="61"/>
@@ -34363,12 +34360,12 @@
         <v>45644</v>
       </c>
       <c r="F11" s="61"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="105"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="61"/>
@@ -34415,11 +34412,11 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="122.25" customHeight="1">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="74" t="s">
-        <v>74</v>
+      <c r="B15" s="74">
+        <v>45663</v>
       </c>
       <c r="C15" s="75" t="s">
         <v>46</v>
@@ -34428,68 +34425,68 @@
         <v>47</v>
       </c>
       <c r="E15" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" s="94" t="s">
         <v>62</v>
       </c>
       <c r="G15" s="92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H15" s="78" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="141.75" customHeight="1">
-      <c r="A16" s="155"/>
+      <c r="A16" s="161"/>
       <c r="B16" s="74">
         <v>45665</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="76" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F16" s="94" t="s">
         <v>62</v>
       </c>
       <c r="G16" s="92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H16" s="79" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="165" customHeight="1">
-      <c r="A17" s="155"/>
+      <c r="A17" s="161"/>
       <c r="B17" s="74">
         <v>45667</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="76" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="94" t="s">
         <v>62</v>
       </c>
       <c r="G17" s="92" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="93" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="18" spans="1:8" ht="12.75">
-      <c r="A18" s="155"/>
+      <c r="A18" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -34503,6 +34500,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EDB39E34F5A9B445B025C05B2A05D030" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c21ef800502b5dc1190a9a0361733939">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f1f31ffb-9912-4459-99c8-b26e82094b51" xmlns:ns4="ce621958-37b1-43fe-a1f1-1aad67996a88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30daf50bb6192471b76b9808b4256f50" ns3:_="" ns4:_="">
     <xsd:import namespace="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
@@ -34697,24 +34711,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D01A9D5D-1824-48C2-8527-9D8749A8DDDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34731,29 +34753,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cambio de fecha en el programa de auditoria
</commit_message>
<xml_diff>
--- a/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
+++ b/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATIAS\Desktop\ESPE\Septimo_Semestre\Quality Assurance\Repo\2563_G3_ACSW\02_Proyecto\09. Programa de Auditoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4CE55A-1364-46DE-82F6-92DD9A15284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCB2C6E-1D7F-483C-8F95-80FEB00ACAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. PROGRAMA" sheetId="1" r:id="rId1"/>
@@ -245,9 +245,6 @@
   </si>
   <si>
     <t>11</t>
-  </si>
-  <si>
-    <t>6</t>
   </si>
   <si>
     <t>Lista de Asistencia
@@ -532,6 +529,9 @@
   </si>
   <si>
     <t>Auditor: Cristopher Zambrano</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -1559,41 +1559,93 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1601,18 +1653,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1629,67 +1671,25 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1968,8 +1968,8 @@
   </sheetPr>
   <dimension ref="A1:AW994"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A21" zoomScale="64" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24:AA24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="64" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -2002,37 +2002,37 @@
     </row>
     <row r="2" spans="1:48" ht="42.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="137"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="135" t="s">
+      <c r="B2" s="114"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="139"/>
-      <c r="T2" s="139"/>
-      <c r="U2" s="139"/>
-      <c r="V2" s="139"/>
-      <c r="W2" s="98"/>
-      <c r="X2" s="98"/>
-      <c r="Y2" s="99"/>
-      <c r="Z2" s="135" t="s">
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="100"/>
+      <c r="X2" s="100"/>
+      <c r="Y2" s="101"/>
+      <c r="Z2" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="98"/>
-      <c r="AB2" s="99"/>
+      <c r="AA2" s="100"/>
+      <c r="AB2" s="101"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -2057,36 +2057,36 @@
     <row r="3" spans="1:48" ht="48.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="99"/>
-      <c r="R3" s="133" t="s">
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="134"/>
-      <c r="T3" s="134"/>
-      <c r="U3" s="134"/>
-      <c r="V3" s="134"/>
-      <c r="W3" s="98"/>
-      <c r="X3" s="98"/>
-      <c r="Y3" s="99"/>
-      <c r="Z3" s="135" t="s">
+      <c r="S3" s="122"/>
+      <c r="T3" s="122"/>
+      <c r="U3" s="122"/>
+      <c r="V3" s="122"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" s="98"/>
-      <c r="AB3" s="99"/>
+      <c r="AA3" s="100"/>
+      <c r="AB3" s="101"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
@@ -2110,39 +2110,39 @@
     </row>
     <row r="4" spans="1:48" ht="21" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="98"/>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="133" t="s">
-        <v>77</v>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
+      <c r="O4" s="100"/>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="121" t="s">
+        <v>76</v>
       </c>
-      <c r="S4" s="134"/>
-      <c r="T4" s="134"/>
-      <c r="U4" s="134"/>
-      <c r="V4" s="134"/>
-      <c r="W4" s="98"/>
-      <c r="X4" s="98"/>
-      <c r="Y4" s="99"/>
-      <c r="Z4" s="135" t="s">
+      <c r="S4" s="122"/>
+      <c r="T4" s="122"/>
+      <c r="U4" s="122"/>
+      <c r="V4" s="122"/>
+      <c r="W4" s="100"/>
+      <c r="X4" s="100"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="98"/>
-      <c r="AB4" s="99"/>
+      <c r="AA4" s="100"/>
+      <c r="AB4" s="101"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
@@ -2215,35 +2215,35 @@
       <c r="AV5" s="2"/>
     </row>
     <row r="6" spans="1:48" ht="50.25" customHeight="1">
-      <c r="B6" s="136" t="s">
-        <v>64</v>
+      <c r="B6" s="125" t="s">
+        <v>63</v>
       </c>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="109"/>
-      <c r="M6" s="109"/>
-      <c r="N6" s="109"/>
-      <c r="O6" s="109"/>
-      <c r="P6" s="109"/>
-      <c r="Q6" s="109"/>
-      <c r="R6" s="109"/>
-      <c r="S6" s="109"/>
-      <c r="T6" s="109"/>
-      <c r="U6" s="109"/>
-      <c r="V6" s="109"/>
-      <c r="W6" s="109"/>
-      <c r="X6" s="109"/>
-      <c r="Y6" s="109"/>
-      <c r="Z6" s="109"/>
-      <c r="AA6" s="109"/>
-      <c r="AB6" s="109"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
+      <c r="O6" s="98"/>
+      <c r="P6" s="98"/>
+      <c r="Q6" s="98"/>
+      <c r="R6" s="98"/>
+      <c r="S6" s="98"/>
+      <c r="T6" s="98"/>
+      <c r="U6" s="98"/>
+      <c r="V6" s="98"/>
+      <c r="W6" s="98"/>
+      <c r="X6" s="98"/>
+      <c r="Y6" s="98"/>
+      <c r="Z6" s="98"/>
+      <c r="AA6" s="98"/>
+      <c r="AB6" s="98"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="6"/>
@@ -2260,35 +2260,35 @@
       <c r="AP6" s="7"/>
     </row>
     <row r="7" spans="1:48" ht="198" customHeight="1">
-      <c r="B7" s="108" t="s">
-        <v>82</v>
+      <c r="B7" s="132" t="s">
+        <v>81</v>
       </c>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="109"/>
-      <c r="N7" s="109"/>
-      <c r="O7" s="109"/>
-      <c r="P7" s="109"/>
-      <c r="Q7" s="109"/>
-      <c r="R7" s="109"/>
-      <c r="S7" s="109"/>
-      <c r="T7" s="109"/>
-      <c r="U7" s="109"/>
-      <c r="V7" s="109"/>
-      <c r="W7" s="109"/>
-      <c r="X7" s="109"/>
-      <c r="Y7" s="109"/>
-      <c r="Z7" s="109"/>
-      <c r="AA7" s="109"/>
-      <c r="AB7" s="109"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="98"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="98"/>
+      <c r="U7" s="98"/>
+      <c r="V7" s="98"/>
+      <c r="W7" s="98"/>
+      <c r="X7" s="98"/>
+      <c r="Y7" s="98"/>
+      <c r="Z7" s="98"/>
+      <c r="AA7" s="98"/>
+      <c r="AB7" s="98"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
       <c r="AE7" s="6"/>
@@ -2305,35 +2305,35 @@
       <c r="AP7" s="7"/>
     </row>
     <row r="8" spans="1:48" ht="51" customHeight="1">
-      <c r="B8" s="130" t="s">
-        <v>63</v>
+      <c r="B8" s="133" t="s">
+        <v>62</v>
       </c>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
-      <c r="M8" s="109"/>
-      <c r="N8" s="109"/>
-      <c r="O8" s="109"/>
-      <c r="P8" s="109"/>
-      <c r="Q8" s="109"/>
-      <c r="R8" s="109"/>
-      <c r="S8" s="109"/>
-      <c r="T8" s="109"/>
-      <c r="U8" s="109"/>
-      <c r="V8" s="109"/>
-      <c r="W8" s="109"/>
-      <c r="X8" s="109"/>
-      <c r="Y8" s="109"/>
-      <c r="Z8" s="109"/>
-      <c r="AA8" s="109"/>
-      <c r="AB8" s="109"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="98"/>
+      <c r="S8" s="98"/>
+      <c r="T8" s="98"/>
+      <c r="U8" s="98"/>
+      <c r="V8" s="98"/>
+      <c r="W8" s="98"/>
+      <c r="X8" s="98"/>
+      <c r="Y8" s="98"/>
+      <c r="Z8" s="98"/>
+      <c r="AA8" s="98"/>
+      <c r="AB8" s="98"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="6"/>
@@ -2393,35 +2393,35 @@
       <c r="AP9" s="7"/>
     </row>
     <row r="10" spans="1:48" ht="20.25" customHeight="1">
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="133" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="109"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="109"/>
-      <c r="K10" s="109"/>
-      <c r="L10" s="109"/>
-      <c r="M10" s="109"/>
-      <c r="N10" s="109"/>
-      <c r="O10" s="109"/>
-      <c r="P10" s="109"/>
-      <c r="Q10" s="109"/>
-      <c r="R10" s="109"/>
-      <c r="S10" s="109"/>
-      <c r="T10" s="109"/>
-      <c r="U10" s="109"/>
-      <c r="V10" s="109"/>
-      <c r="W10" s="109"/>
-      <c r="X10" s="109"/>
-      <c r="Y10" s="109"/>
-      <c r="Z10" s="109"/>
-      <c r="AA10" s="109"/>
-      <c r="AB10" s="109"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="98"/>
+      <c r="O10" s="98"/>
+      <c r="P10" s="98"/>
+      <c r="Q10" s="98"/>
+      <c r="R10" s="98"/>
+      <c r="S10" s="98"/>
+      <c r="T10" s="98"/>
+      <c r="U10" s="98"/>
+      <c r="V10" s="98"/>
+      <c r="W10" s="98"/>
+      <c r="X10" s="98"/>
+      <c r="Y10" s="98"/>
+      <c r="Z10" s="98"/>
+      <c r="AA10" s="98"/>
+      <c r="AB10" s="98"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="6"/>
@@ -2439,35 +2439,35 @@
     </row>
     <row r="11" spans="1:48" ht="60" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="108" t="s">
-        <v>65</v>
+      <c r="B11" s="132" t="s">
+        <v>64</v>
       </c>
-      <c r="C11" s="109"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="109"/>
-      <c r="J11" s="109"/>
-      <c r="K11" s="109"/>
-      <c r="L11" s="109"/>
-      <c r="M11" s="109"/>
-      <c r="N11" s="109"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="109"/>
-      <c r="W11" s="109"/>
-      <c r="X11" s="109"/>
-      <c r="Y11" s="109"/>
-      <c r="Z11" s="109"/>
-      <c r="AA11" s="109"/>
-      <c r="AB11" s="109"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="98"/>
+      <c r="P11" s="98"/>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="98"/>
+      <c r="T11" s="98"/>
+      <c r="U11" s="98"/>
+      <c r="V11" s="98"/>
+      <c r="W11" s="98"/>
+      <c r="X11" s="98"/>
+      <c r="Y11" s="98"/>
+      <c r="Z11" s="98"/>
+      <c r="AA11" s="98"/>
+      <c r="AB11" s="98"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="9"/>
       <c r="AE11" s="9"/>
@@ -2490,35 +2490,35 @@
       <c r="AV11" s="8"/>
     </row>
     <row r="12" spans="1:48" ht="53.25" customHeight="1">
-      <c r="B12" s="108" t="s">
-        <v>66</v>
+      <c r="B12" s="132" t="s">
+        <v>65</v>
       </c>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109"/>
-      <c r="J12" s="109"/>
-      <c r="K12" s="109"/>
-      <c r="L12" s="109"/>
-      <c r="M12" s="109"/>
-      <c r="N12" s="109"/>
-      <c r="O12" s="109"/>
-      <c r="P12" s="109"/>
-      <c r="Q12" s="109"/>
-      <c r="R12" s="109"/>
-      <c r="S12" s="109"/>
-      <c r="T12" s="109"/>
-      <c r="U12" s="109"/>
-      <c r="V12" s="109"/>
-      <c r="W12" s="109"/>
-      <c r="X12" s="109"/>
-      <c r="Y12" s="109"/>
-      <c r="Z12" s="109"/>
-      <c r="AA12" s="109"/>
-      <c r="AB12" s="109"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="98"/>
+      <c r="P12" s="98"/>
+      <c r="Q12" s="98"/>
+      <c r="R12" s="98"/>
+      <c r="S12" s="98"/>
+      <c r="T12" s="98"/>
+      <c r="U12" s="98"/>
+      <c r="V12" s="98"/>
+      <c r="W12" s="98"/>
+      <c r="X12" s="98"/>
+      <c r="Y12" s="98"/>
+      <c r="Z12" s="98"/>
+      <c r="AA12" s="98"/>
+      <c r="AB12" s="98"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
@@ -2535,35 +2535,35 @@
       <c r="AP12" s="7"/>
     </row>
     <row r="13" spans="1:48" ht="39.75" customHeight="1">
-      <c r="B13" s="108" t="s">
-        <v>67</v>
+      <c r="B13" s="132" t="s">
+        <v>66</v>
       </c>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
-      <c r="K13" s="109"/>
-      <c r="L13" s="109"/>
-      <c r="M13" s="109"/>
-      <c r="N13" s="109"/>
-      <c r="O13" s="109"/>
-      <c r="P13" s="109"/>
-      <c r="Q13" s="109"/>
-      <c r="R13" s="109"/>
-      <c r="S13" s="109"/>
-      <c r="T13" s="109"/>
-      <c r="U13" s="109"/>
-      <c r="V13" s="109"/>
-      <c r="W13" s="109"/>
-      <c r="X13" s="109"/>
-      <c r="Y13" s="109"/>
-      <c r="Z13" s="109"/>
-      <c r="AA13" s="109"/>
-      <c r="AB13" s="109"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="98"/>
+      <c r="Q13" s="98"/>
+      <c r="R13" s="98"/>
+      <c r="S13" s="98"/>
+      <c r="T13" s="98"/>
+      <c r="U13" s="98"/>
+      <c r="V13" s="98"/>
+      <c r="W13" s="98"/>
+      <c r="X13" s="98"/>
+      <c r="Y13" s="98"/>
+      <c r="Z13" s="98"/>
+      <c r="AA13" s="98"/>
+      <c r="AB13" s="98"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
@@ -2623,35 +2623,35 @@
       <c r="AP14" s="7"/>
     </row>
     <row r="15" spans="1:48" ht="99.75" customHeight="1">
-      <c r="B15" s="110" t="s">
-        <v>68</v>
+      <c r="B15" s="134" t="s">
+        <v>67</v>
       </c>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="109"/>
-      <c r="J15" s="109"/>
-      <c r="K15" s="109"/>
-      <c r="L15" s="109"/>
-      <c r="M15" s="109"/>
-      <c r="N15" s="109"/>
-      <c r="O15" s="109"/>
-      <c r="P15" s="109"/>
-      <c r="Q15" s="109"/>
-      <c r="R15" s="109"/>
-      <c r="S15" s="109"/>
-      <c r="T15" s="109"/>
-      <c r="U15" s="109"/>
-      <c r="V15" s="109"/>
-      <c r="W15" s="109"/>
-      <c r="X15" s="109"/>
-      <c r="Y15" s="109"/>
-      <c r="Z15" s="109"/>
-      <c r="AA15" s="109"/>
-      <c r="AB15" s="109"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="98"/>
+      <c r="P15" s="98"/>
+      <c r="Q15" s="98"/>
+      <c r="R15" s="98"/>
+      <c r="S15" s="98"/>
+      <c r="T15" s="98"/>
+      <c r="U15" s="98"/>
+      <c r="V15" s="98"/>
+      <c r="W15" s="98"/>
+      <c r="X15" s="98"/>
+      <c r="Y15" s="98"/>
+      <c r="Z15" s="98"/>
+      <c r="AA15" s="98"/>
+      <c r="AB15" s="98"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="6"/>
@@ -2669,35 +2669,35 @@
     </row>
     <row r="16" spans="1:48" ht="24.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="111" t="s">
-        <v>69</v>
+      <c r="B16" s="135" t="s">
+        <v>68</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="109"/>
-      <c r="J16" s="109"/>
-      <c r="K16" s="109"/>
-      <c r="L16" s="109"/>
-      <c r="M16" s="109"/>
-      <c r="N16" s="109"/>
-      <c r="O16" s="109"/>
-      <c r="P16" s="109"/>
-      <c r="Q16" s="109"/>
-      <c r="R16" s="109"/>
-      <c r="S16" s="109"/>
-      <c r="T16" s="109"/>
-      <c r="U16" s="109"/>
-      <c r="V16" s="109"/>
-      <c r="W16" s="109"/>
-      <c r="X16" s="109"/>
-      <c r="Y16" s="109"/>
-      <c r="Z16" s="109"/>
-      <c r="AA16" s="109"/>
-      <c r="AB16" s="109"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="98"/>
+      <c r="P16" s="98"/>
+      <c r="Q16" s="98"/>
+      <c r="R16" s="98"/>
+      <c r="S16" s="98"/>
+      <c r="T16" s="98"/>
+      <c r="U16" s="98"/>
+      <c r="V16" s="98"/>
+      <c r="W16" s="98"/>
+      <c r="X16" s="98"/>
+      <c r="Y16" s="98"/>
+      <c r="Z16" s="98"/>
+      <c r="AA16" s="98"/>
+      <c r="AB16" s="98"/>
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
@@ -2720,35 +2720,35 @@
       <c r="AV16" s="2"/>
     </row>
     <row r="17" spans="1:49" ht="24.75" customHeight="1">
-      <c r="B17" s="110" t="s">
+      <c r="B17" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="109"/>
-      <c r="J17" s="109"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="109"/>
-      <c r="M17" s="109"/>
-      <c r="N17" s="109"/>
-      <c r="O17" s="109"/>
-      <c r="P17" s="109"/>
-      <c r="Q17" s="109"/>
-      <c r="R17" s="109"/>
-      <c r="S17" s="109"/>
-      <c r="T17" s="109"/>
-      <c r="U17" s="109"/>
-      <c r="V17" s="109"/>
-      <c r="W17" s="109"/>
-      <c r="X17" s="109"/>
-      <c r="Y17" s="109"/>
-      <c r="Z17" s="109"/>
-      <c r="AA17" s="109"/>
-      <c r="AB17" s="109"/>
+      <c r="C17" s="98"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="98"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="98"/>
+      <c r="P17" s="98"/>
+      <c r="Q17" s="98"/>
+      <c r="R17" s="98"/>
+      <c r="S17" s="98"/>
+      <c r="T17" s="98"/>
+      <c r="U17" s="98"/>
+      <c r="V17" s="98"/>
+      <c r="W17" s="98"/>
+      <c r="X17" s="98"/>
+      <c r="Y17" s="98"/>
+      <c r="Z17" s="98"/>
+      <c r="AA17" s="98"/>
+      <c r="AB17" s="98"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="6"/>
@@ -2765,33 +2765,33 @@
       <c r="AP17" s="7"/>
     </row>
     <row r="18" spans="1:49" ht="6.75" customHeight="1">
-      <c r="B18" s="110"/>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="109"/>
-      <c r="H18" s="109"/>
-      <c r="I18" s="109"/>
-      <c r="J18" s="109"/>
-      <c r="K18" s="109"/>
-      <c r="L18" s="109"/>
-      <c r="M18" s="109"/>
-      <c r="N18" s="109"/>
-      <c r="O18" s="109"/>
-      <c r="P18" s="109"/>
-      <c r="Q18" s="109"/>
-      <c r="R18" s="109"/>
-      <c r="S18" s="109"/>
-      <c r="T18" s="109"/>
-      <c r="U18" s="109"/>
-      <c r="V18" s="109"/>
-      <c r="W18" s="109"/>
-      <c r="X18" s="109"/>
-      <c r="Y18" s="109"/>
-      <c r="Z18" s="109"/>
-      <c r="AA18" s="109"/>
-      <c r="AB18" s="109"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="98"/>
+      <c r="O18" s="98"/>
+      <c r="P18" s="98"/>
+      <c r="Q18" s="98"/>
+      <c r="R18" s="98"/>
+      <c r="S18" s="98"/>
+      <c r="T18" s="98"/>
+      <c r="U18" s="98"/>
+      <c r="V18" s="98"/>
+      <c r="W18" s="98"/>
+      <c r="X18" s="98"/>
+      <c r="Y18" s="98"/>
+      <c r="Z18" s="98"/>
+      <c r="AA18" s="98"/>
+      <c r="AB18" s="98"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
@@ -2809,44 +2809,44 @@
     </row>
     <row r="19" spans="1:49" ht="36.75" customHeight="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="122" t="s">
+      <c r="B19" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="125" t="s">
+      <c r="C19" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="113"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="126" t="s">
+      <c r="D19" s="127"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="142" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="112" t="s">
+      <c r="G19" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="113"/>
-      <c r="I19" s="113"/>
-      <c r="J19" s="113"/>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="113"/>
-      <c r="N19" s="114"/>
-      <c r="O19" s="112" t="s">
+      <c r="H19" s="127"/>
+      <c r="I19" s="127"/>
+      <c r="J19" s="127"/>
+      <c r="K19" s="127"/>
+      <c r="L19" s="127"/>
+      <c r="M19" s="127"/>
+      <c r="N19" s="128"/>
+      <c r="O19" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="P19" s="113"/>
-      <c r="Q19" s="113"/>
-      <c r="R19" s="113"/>
-      <c r="S19" s="113"/>
-      <c r="T19" s="113"/>
-      <c r="U19" s="113"/>
-      <c r="V19" s="113"/>
-      <c r="W19" s="114"/>
-      <c r="X19" s="118" t="s">
+      <c r="P19" s="127"/>
+      <c r="Q19" s="127"/>
+      <c r="R19" s="127"/>
+      <c r="S19" s="127"/>
+      <c r="T19" s="127"/>
+      <c r="U19" s="127"/>
+      <c r="V19" s="127"/>
+      <c r="W19" s="128"/>
+      <c r="X19" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="Y19" s="113"/>
-      <c r="Z19" s="113"/>
-      <c r="AA19" s="114"/>
+      <c r="Y19" s="127"/>
+      <c r="Z19" s="127"/>
+      <c r="AA19" s="128"/>
       <c r="AB19" s="83" t="s">
         <v>9</v>
       </c>
@@ -2873,32 +2873,32 @@
     </row>
     <row r="20" spans="1:49" ht="10.5" customHeight="1">
       <c r="A20" s="14"/>
-      <c r="B20" s="123"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="127"/>
+      <c r="B20" s="139"/>
+      <c r="C20" s="129"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="131"/>
+      <c r="F20" s="143"/>
       <c r="G20" s="115"/>
-      <c r="H20" s="116"/>
-      <c r="I20" s="116"/>
-      <c r="J20" s="116"/>
-      <c r="K20" s="116"/>
-      <c r="L20" s="116"/>
-      <c r="M20" s="116"/>
-      <c r="N20" s="117"/>
-      <c r="O20" s="119"/>
-      <c r="P20" s="129"/>
-      <c r="Q20" s="129"/>
-      <c r="R20" s="129"/>
-      <c r="S20" s="129"/>
-      <c r="T20" s="129"/>
-      <c r="U20" s="129"/>
-      <c r="V20" s="129"/>
-      <c r="W20" s="120"/>
-      <c r="X20" s="119"/>
-      <c r="Y20" s="109"/>
-      <c r="Z20" s="109"/>
-      <c r="AA20" s="120"/>
+      <c r="H20" s="107"/>
+      <c r="I20" s="107"/>
+      <c r="J20" s="107"/>
+      <c r="K20" s="107"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="107"/>
+      <c r="N20" s="116"/>
+      <c r="O20" s="129"/>
+      <c r="P20" s="130"/>
+      <c r="Q20" s="130"/>
+      <c r="R20" s="130"/>
+      <c r="S20" s="130"/>
+      <c r="T20" s="130"/>
+      <c r="U20" s="130"/>
+      <c r="V20" s="130"/>
+      <c r="W20" s="131"/>
+      <c r="X20" s="129"/>
+      <c r="Y20" s="98"/>
+      <c r="Z20" s="98"/>
+      <c r="AA20" s="131"/>
       <c r="AB20" s="84"/>
       <c r="AC20" s="14"/>
       <c r="AD20" s="14"/>
@@ -2923,37 +2923,37 @@
     </row>
     <row r="21" spans="1:49" ht="34.5" customHeight="1">
       <c r="A21" s="15"/>
-      <c r="B21" s="123"/>
-      <c r="C21" s="119"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="127"/>
-      <c r="G21" s="121" t="s">
+      <c r="B21" s="139"/>
+      <c r="C21" s="129"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="131"/>
+      <c r="F21" s="143"/>
+      <c r="G21" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="99"/>
-      <c r="I21" s="121" t="s">
+      <c r="H21" s="101"/>
+      <c r="I21" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="99"/>
-      <c r="K21" s="121" t="s">
+      <c r="J21" s="101"/>
+      <c r="K21" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="99"/>
-      <c r="M21" s="121" t="s">
+      <c r="L21" s="101"/>
+      <c r="M21" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="98"/>
-      <c r="O21" s="96" t="s">
+      <c r="N21" s="100"/>
+      <c r="O21" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="95" t="s">
+      <c r="P21" s="146"/>
+      <c r="Q21" s="146"/>
+      <c r="R21" s="146"/>
+      <c r="S21" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="T21" s="96"/>
+      <c r="T21" s="146"/>
       <c r="U21" s="91" t="s">
         <v>12</v>
       </c>
@@ -2961,10 +2961,10 @@
         <v>13</v>
       </c>
       <c r="W21" s="87"/>
-      <c r="X21" s="116"/>
-      <c r="Y21" s="116"/>
-      <c r="Z21" s="116"/>
-      <c r="AA21" s="117"/>
+      <c r="X21" s="107"/>
+      <c r="Y21" s="107"/>
+      <c r="Z21" s="107"/>
+      <c r="AA21" s="116"/>
       <c r="AB21" s="84"/>
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
@@ -2989,11 +2989,11 @@
     </row>
     <row r="22" spans="1:49" ht="38.25" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="124"/>
+      <c r="B22" s="140"/>
       <c r="C22" s="115"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="117"/>
-      <c r="F22" s="128"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="144"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
@@ -3015,33 +3015,33 @@
         <v>18</v>
       </c>
       <c r="O22" s="90" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="P22" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q22" s="148">
+        <v>10</v>
+      </c>
+      <c r="R22" s="149"/>
+      <c r="S22" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="Q22" s="104">
-        <v>10</v>
-      </c>
-      <c r="R22" s="105"/>
-      <c r="S22" s="88" t="s">
+      <c r="T22" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="T22" s="86" t="s">
-        <v>60</v>
-      </c>
       <c r="U22" s="86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V22" s="86" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W22" s="86"/>
       <c r="X22" s="86"/>
-      <c r="Y22" s="97"/>
-      <c r="Z22" s="98"/>
-      <c r="AA22" s="98"/>
-      <c r="AB22" s="99"/>
+      <c r="Y22" s="147"/>
+      <c r="Z22" s="100"/>
+      <c r="AA22" s="100"/>
+      <c r="AB22" s="101"/>
       <c r="AC22" s="85"/>
       <c r="AD22" s="14"/>
       <c r="AE22" s="14"/>
@@ -3069,11 +3069,11 @@
       <c r="B23" s="18">
         <v>1</v>
       </c>
-      <c r="C23" s="100" t="s">
+      <c r="C23" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="101"/>
-      <c r="E23" s="102"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="109"/>
       <c r="F23" s="76">
         <v>1</v>
       </c>
@@ -3089,21 +3089,21 @@
       <c r="N23" s="21"/>
       <c r="O23" s="89"/>
       <c r="P23" s="89"/>
-      <c r="Q23" s="106"/>
-      <c r="R23" s="107"/>
+      <c r="Q23" s="150"/>
+      <c r="R23" s="151"/>
       <c r="S23" s="22"/>
       <c r="T23" s="22"/>
       <c r="U23" s="22"/>
       <c r="V23" s="22"/>
       <c r="W23" s="22"/>
-      <c r="X23" s="103" t="s">
+      <c r="X23" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y23" s="100"/>
+      <c r="Z23" s="100"/>
+      <c r="AA23" s="101"/>
+      <c r="AB23" s="23" t="s">
         <v>56</v>
-      </c>
-      <c r="Y23" s="98"/>
-      <c r="Z23" s="98"/>
-      <c r="AA23" s="99"/>
-      <c r="AB23" s="23" t="s">
-        <v>57</v>
       </c>
       <c r="AC23" s="17"/>
       <c r="AD23" s="17"/>
@@ -3131,11 +3131,11 @@
       <c r="B24" s="18">
         <v>2</v>
       </c>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="101"/>
-      <c r="E24" s="102"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="109"/>
       <c r="F24" s="76">
         <v>2</v>
       </c>
@@ -3153,23 +3153,23 @@
       <c r="P24" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Q24" s="150" t="s">
+      <c r="Q24" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="R24" s="151"/>
+      <c r="R24" s="96"/>
       <c r="S24" s="22"/>
       <c r="T24" s="22"/>
       <c r="U24" s="22"/>
       <c r="V24" s="22"/>
       <c r="W24" s="22"/>
-      <c r="X24" s="103" t="s">
-        <v>81</v>
+      <c r="X24" s="99" t="s">
+        <v>80</v>
       </c>
-      <c r="Y24" s="98"/>
-      <c r="Z24" s="98"/>
-      <c r="AA24" s="99"/>
+      <c r="Y24" s="100"/>
+      <c r="Z24" s="100"/>
+      <c r="AA24" s="101"/>
       <c r="AB24" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC24" s="17"/>
       <c r="AD24" s="17"/>
@@ -3197,11 +3197,11 @@
       <c r="B25" s="18">
         <v>3</v>
       </c>
-      <c r="C25" s="100" t="s">
+      <c r="C25" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="101"/>
-      <c r="E25" s="102"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="109"/>
       <c r="F25" s="76">
         <v>3</v>
       </c>
@@ -3215,8 +3215,8 @@
       <c r="N25" s="21"/>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
-      <c r="Q25" s="150"/>
-      <c r="R25" s="151"/>
+      <c r="Q25" s="95"/>
+      <c r="R25" s="96"/>
       <c r="S25" s="22" t="s">
         <v>20</v>
       </c>
@@ -3226,14 +3226,14 @@
       <c r="U25" s="22"/>
       <c r="V25" s="22"/>
       <c r="W25" s="22"/>
-      <c r="X25" s="103" t="s">
-        <v>70</v>
+      <c r="X25" s="99" t="s">
+        <v>69</v>
       </c>
-      <c r="Y25" s="98"/>
-      <c r="Z25" s="98"/>
-      <c r="AA25" s="99"/>
+      <c r="Y25" s="100"/>
+      <c r="Z25" s="100"/>
+      <c r="AA25" s="101"/>
       <c r="AB25" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC25" s="17"/>
       <c r="AD25" s="17"/>
@@ -3261,11 +3261,11 @@
       <c r="B26" s="18">
         <v>4</v>
       </c>
-      <c r="C26" s="100" t="s">
+      <c r="C26" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="101"/>
-      <c r="E26" s="102"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="109"/>
       <c r="F26" s="76">
         <v>4</v>
       </c>
@@ -3279,8 +3279,8 @@
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21"/>
-      <c r="Q26" s="150"/>
-      <c r="R26" s="151"/>
+      <c r="Q26" s="95"/>
+      <c r="R26" s="96"/>
       <c r="S26" s="22"/>
       <c r="T26" s="22"/>
       <c r="U26" s="22" t="s">
@@ -3288,14 +3288,14 @@
       </c>
       <c r="V26" s="22"/>
       <c r="W26" s="22"/>
-      <c r="X26" s="103" t="s">
+      <c r="X26" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Y26" s="98"/>
-      <c r="Z26" s="98"/>
-      <c r="AA26" s="99"/>
+      <c r="Y26" s="100"/>
+      <c r="Z26" s="100"/>
+      <c r="AA26" s="101"/>
       <c r="AB26" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC26" s="17"/>
       <c r="AD26" s="17"/>
@@ -3323,11 +3323,11 @@
       <c r="B27" s="18">
         <v>5</v>
       </c>
-      <c r="C27" s="100" t="s">
+      <c r="C27" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="101"/>
-      <c r="E27" s="102"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="109"/>
       <c r="F27" s="80">
         <v>5</v>
       </c>
@@ -3341,8 +3341,8 @@
       <c r="N27" s="21"/>
       <c r="O27" s="21"/>
       <c r="P27" s="21"/>
-      <c r="Q27" s="150"/>
-      <c r="R27" s="151"/>
+      <c r="Q27" s="95"/>
+      <c r="R27" s="96"/>
       <c r="S27" s="22"/>
       <c r="T27" s="22"/>
       <c r="U27" s="22"/>
@@ -3350,14 +3350,14 @@
         <v>20</v>
       </c>
       <c r="W27" s="22"/>
-      <c r="X27" s="103" t="s">
+      <c r="X27" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="Y27" s="98"/>
-      <c r="Z27" s="98"/>
-      <c r="AA27" s="99"/>
+      <c r="Y27" s="100"/>
+      <c r="Z27" s="100"/>
+      <c r="AA27" s="101"/>
       <c r="AB27" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC27" s="17"/>
       <c r="AD27" s="17"/>
@@ -3383,9 +3383,9 @@
     <row r="28" spans="1:49" ht="163.5" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="102"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="105"/>
+      <c r="E28" s="109"/>
       <c r="F28" s="81"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
@@ -3397,19 +3397,19 @@
       <c r="N28" s="21"/>
       <c r="O28" s="21"/>
       <c r="P28" s="21"/>
-      <c r="Q28" s="150"/>
-      <c r="R28" s="151"/>
+      <c r="Q28" s="95"/>
+      <c r="R28" s="96"/>
       <c r="S28" s="22"/>
       <c r="T28" s="22"/>
       <c r="U28" s="22"/>
       <c r="V28" s="22"/>
       <c r="W28" s="22"/>
-      <c r="X28" s="103" t="s">
+      <c r="X28" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="Y28" s="98"/>
-      <c r="Z28" s="98"/>
-      <c r="AA28" s="99"/>
+      <c r="Y28" s="100"/>
+      <c r="Z28" s="100"/>
+      <c r="AA28" s="101"/>
       <c r="AB28" s="23"/>
       <c r="AC28" s="17"/>
       <c r="AD28" s="17"/>
@@ -3435,9 +3435,9 @@
     <row r="29" spans="1:49" ht="209.25" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
-      <c r="C29" s="100"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="102"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="109"/>
       <c r="F29" s="19"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
@@ -3449,17 +3449,17 @@
       <c r="N29" s="25"/>
       <c r="O29" s="21"/>
       <c r="P29" s="21"/>
-      <c r="Q29" s="150"/>
-      <c r="R29" s="151"/>
+      <c r="Q29" s="95"/>
+      <c r="R29" s="96"/>
       <c r="S29" s="22"/>
       <c r="T29" s="22"/>
       <c r="U29" s="22"/>
       <c r="V29" s="22"/>
       <c r="W29" s="22"/>
-      <c r="X29" s="103"/>
-      <c r="Y29" s="98"/>
-      <c r="Z29" s="98"/>
-      <c r="AA29" s="99"/>
+      <c r="X29" s="99"/>
+      <c r="Y29" s="100"/>
+      <c r="Z29" s="100"/>
+      <c r="AA29" s="101"/>
       <c r="AB29" s="23"/>
       <c r="AC29" s="17"/>
       <c r="AD29" s="17"/>
@@ -3485,9 +3485,9 @@
     <row r="30" spans="1:49" ht="262.5" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
-      <c r="C30" s="100"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="102"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="105"/>
+      <c r="E30" s="109"/>
       <c r="F30" s="19"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -3499,17 +3499,17 @@
       <c r="N30" s="21"/>
       <c r="O30" s="25"/>
       <c r="P30" s="21"/>
-      <c r="Q30" s="150"/>
-      <c r="R30" s="151"/>
+      <c r="Q30" s="95"/>
+      <c r="R30" s="96"/>
       <c r="S30" s="22"/>
       <c r="T30" s="22"/>
       <c r="U30" s="22"/>
       <c r="V30" s="22"/>
       <c r="W30" s="22"/>
-      <c r="X30" s="103"/>
-      <c r="Y30" s="98"/>
-      <c r="Z30" s="98"/>
-      <c r="AA30" s="99"/>
+      <c r="X30" s="99"/>
+      <c r="Y30" s="100"/>
+      <c r="Z30" s="100"/>
+      <c r="AA30" s="101"/>
       <c r="AB30" s="23"/>
       <c r="AC30" s="17"/>
       <c r="AD30" s="17"/>
@@ -3535,9 +3535,9 @@
     <row r="31" spans="1:49" ht="90.75" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
-      <c r="C31" s="143"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="102"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="105"/>
+      <c r="E31" s="109"/>
       <c r="F31" s="19"/>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
@@ -3549,17 +3549,17 @@
       <c r="N31" s="21"/>
       <c r="O31" s="21"/>
       <c r="P31" s="21"/>
-      <c r="Q31" s="150"/>
-      <c r="R31" s="151"/>
+      <c r="Q31" s="95"/>
+      <c r="R31" s="96"/>
       <c r="S31" s="22"/>
       <c r="T31" s="22"/>
       <c r="U31" s="22"/>
       <c r="V31" s="22"/>
       <c r="W31" s="22"/>
-      <c r="X31" s="145"/>
-      <c r="Y31" s="98"/>
-      <c r="Z31" s="98"/>
-      <c r="AA31" s="99"/>
+      <c r="X31" s="102"/>
+      <c r="Y31" s="100"/>
+      <c r="Z31" s="100"/>
+      <c r="AA31" s="101"/>
       <c r="AB31" s="23"/>
       <c r="AC31" s="17"/>
       <c r="AD31" s="17"/>
@@ -3585,9 +3585,9 @@
     <row r="32" spans="1:49" ht="90.75" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
-      <c r="C32" s="144"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="99"/>
+      <c r="C32" s="111"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="101"/>
       <c r="F32" s="19"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
@@ -3599,17 +3599,17 @@
       <c r="N32" s="21"/>
       <c r="O32" s="21"/>
       <c r="P32" s="21"/>
-      <c r="Q32" s="150"/>
-      <c r="R32" s="151"/>
+      <c r="Q32" s="95"/>
+      <c r="R32" s="96"/>
       <c r="S32" s="22"/>
       <c r="T32" s="22"/>
       <c r="U32" s="22"/>
       <c r="V32" s="22"/>
       <c r="W32" s="22"/>
-      <c r="X32" s="145"/>
-      <c r="Y32" s="98"/>
-      <c r="Z32" s="98"/>
-      <c r="AA32" s="99"/>
+      <c r="X32" s="102"/>
+      <c r="Y32" s="100"/>
+      <c r="Z32" s="100"/>
+      <c r="AA32" s="101"/>
       <c r="AB32" s="23"/>
       <c r="AC32" s="17"/>
       <c r="AD32" s="17"/>
@@ -3656,10 +3656,10 @@
       <c r="U33" s="29"/>
       <c r="V33" s="29"/>
       <c r="W33" s="29"/>
-      <c r="X33" s="149"/>
-      <c r="Y33" s="109"/>
-      <c r="Z33" s="109"/>
-      <c r="AA33" s="109"/>
+      <c r="X33" s="103"/>
+      <c r="Y33" s="98"/>
+      <c r="Z33" s="98"/>
+      <c r="AA33" s="98"/>
       <c r="AB33" s="30"/>
     </row>
     <row r="34" spans="1:29" ht="12.75" customHeight="1">
@@ -3686,10 +3686,10 @@
       <c r="U34" s="29"/>
       <c r="V34" s="29"/>
       <c r="W34" s="29"/>
-      <c r="X34" s="149"/>
-      <c r="Y34" s="109"/>
-      <c r="Z34" s="109"/>
-      <c r="AA34" s="109"/>
+      <c r="X34" s="103"/>
+      <c r="Y34" s="98"/>
+      <c r="Z34" s="98"/>
+      <c r="AA34" s="98"/>
       <c r="AB34" s="30"/>
     </row>
     <row r="35" spans="1:29" ht="19.5" customHeight="1">
@@ -3707,10 +3707,10 @@
       <c r="J35" s="17"/>
       <c r="O35" s="38"/>
       <c r="P35" s="38"/>
-      <c r="X35" s="148"/>
-      <c r="Y35" s="109"/>
-      <c r="Z35" s="109"/>
-      <c r="AA35" s="109"/>
+      <c r="X35" s="97"/>
+      <c r="Y35" s="98"/>
+      <c r="Z35" s="98"/>
+      <c r="AA35" s="98"/>
       <c r="AB35" s="26"/>
     </row>
     <row r="36" spans="1:29" ht="18.75" customHeight="1">
@@ -3823,34 +3823,34 @@
     <row r="40" spans="1:29" ht="39.75" customHeight="1">
       <c r="A40" s="26"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="146" t="s">
+      <c r="C40" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="109"/>
-      <c r="E40" s="109"/>
-      <c r="F40" s="109"/>
-      <c r="G40" s="109"/>
-      <c r="H40" s="109"/>
-      <c r="I40" s="109"/>
-      <c r="J40" s="109"/>
-      <c r="K40" s="109"/>
-      <c r="L40" s="109"/>
-      <c r="M40" s="109"/>
-      <c r="N40" s="109"/>
-      <c r="O40" s="109"/>
-      <c r="P40" s="109"/>
-      <c r="Q40" s="109"/>
-      <c r="R40" s="109"/>
-      <c r="S40" s="109"/>
-      <c r="T40" s="109"/>
-      <c r="U40" s="109"/>
-      <c r="V40" s="109"/>
-      <c r="W40" s="109"/>
-      <c r="X40" s="109"/>
-      <c r="Y40" s="109"/>
-      <c r="Z40" s="109"/>
-      <c r="AA40" s="109"/>
-      <c r="AB40" s="147"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="98"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="98"/>
+      <c r="H40" s="98"/>
+      <c r="I40" s="98"/>
+      <c r="J40" s="98"/>
+      <c r="K40" s="98"/>
+      <c r="L40" s="98"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="98"/>
+      <c r="O40" s="98"/>
+      <c r="P40" s="98"/>
+      <c r="Q40" s="98"/>
+      <c r="R40" s="98"/>
+      <c r="S40" s="98"/>
+      <c r="T40" s="98"/>
+      <c r="U40" s="98"/>
+      <c r="V40" s="98"/>
+      <c r="W40" s="98"/>
+      <c r="X40" s="98"/>
+      <c r="Y40" s="98"/>
+      <c r="Z40" s="98"/>
+      <c r="AA40" s="98"/>
+      <c r="AB40" s="113"/>
     </row>
     <row r="41" spans="1:29" ht="11.25" customHeight="1">
       <c r="A41" s="26"/>
@@ -3929,14 +3929,14 @@
       <c r="C46" s="53"/>
     </row>
     <row r="47" spans="1:29" ht="15" customHeight="1">
-      <c r="B47" s="141" t="s">
+      <c r="B47" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="101"/>
-      <c r="D47" s="101"/>
-      <c r="E47" s="101"/>
-      <c r="F47" s="101"/>
-      <c r="G47" s="101"/>
+      <c r="C47" s="105"/>
+      <c r="D47" s="105"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="105"/>
       <c r="J47" s="17"/>
       <c r="K47" s="55" t="s">
         <v>33</v>
@@ -3956,17 +3956,17 @@
       </c>
       <c r="D50" s="59"/>
       <c r="E50" s="59"/>
-      <c r="F50" s="142"/>
-      <c r="G50" s="116"/>
-      <c r="H50" s="116"/>
+      <c r="F50" s="106"/>
+      <c r="G50" s="107"/>
+      <c r="H50" s="107"/>
       <c r="J50" s="60"/>
       <c r="K50" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="N50" s="142"/>
-      <c r="O50" s="116"/>
-      <c r="P50" s="116"/>
-      <c r="Q50" s="116"/>
+      <c r="N50" s="106"/>
+      <c r="O50" s="107"/>
+      <c r="P50" s="107"/>
+      <c r="Q50" s="107"/>
     </row>
     <row r="51" spans="1:17" ht="12" customHeight="1">
       <c r="F51" s="58"/>
@@ -34135,22 +34135,47 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="X35:AA35"/>
-    <mergeCell ref="X28:AA28"/>
-    <mergeCell ref="X30:AA30"/>
-    <mergeCell ref="X31:AA31"/>
-    <mergeCell ref="X33:AA33"/>
-    <mergeCell ref="X34:AA34"/>
-    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="Y22:AB22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="X23:AA23"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="X24:AA24"/>
+    <mergeCell ref="B13:AB13"/>
+    <mergeCell ref="B15:AB15"/>
+    <mergeCell ref="B16:AB16"/>
+    <mergeCell ref="B17:AB17"/>
+    <mergeCell ref="G19:N20"/>
+    <mergeCell ref="X19:AA21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="B18:AB18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="O19:W20"/>
+    <mergeCell ref="B7:AB7"/>
+    <mergeCell ref="B8:AB8"/>
+    <mergeCell ref="B10:AB10"/>
+    <mergeCell ref="B11:AB11"/>
+    <mergeCell ref="B12:AB12"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="B6:AB6"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="G2:Q2"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="G3:Q3"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
     <mergeCell ref="X25:AA25"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="F50:H50"/>
@@ -34167,47 +34192,22 @@
     <mergeCell ref="X26:AA26"/>
     <mergeCell ref="X27:AA27"/>
     <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="G3:Q3"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="B6:AB6"/>
-    <mergeCell ref="O19:W20"/>
-    <mergeCell ref="B7:AB7"/>
-    <mergeCell ref="B8:AB8"/>
-    <mergeCell ref="B10:AB10"/>
-    <mergeCell ref="B11:AB11"/>
-    <mergeCell ref="B12:AB12"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="X24:AA24"/>
-    <mergeCell ref="B13:AB13"/>
-    <mergeCell ref="B15:AB15"/>
-    <mergeCell ref="B16:AB16"/>
-    <mergeCell ref="B17:AB17"/>
-    <mergeCell ref="G19:N20"/>
-    <mergeCell ref="X19:AA21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="B18:AB18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="Y22:AB22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="X23:AA23"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="X35:AA35"/>
+    <mergeCell ref="X28:AA28"/>
+    <mergeCell ref="X30:AA30"/>
+    <mergeCell ref="X31:AA31"/>
+    <mergeCell ref="X33:AA33"/>
+    <mergeCell ref="X34:AA34"/>
+    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
   </mergeCells>
   <conditionalFormatting sqref="F49:G50">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
@@ -34236,7 +34236,7 @@
   </sheetPr>
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -34251,55 +34251,55 @@
   <sheetData>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="152" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
       <c r="H2" s="153"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="154"/>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="147"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="113"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="154"/>
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="147"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="113"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="154"/>
-      <c r="B5" s="109"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="147"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="113"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="154"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="147"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="113"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="155"/>
@@ -34356,12 +34356,12 @@
         <v>45644</v>
       </c>
       <c r="F11" s="61"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="61"/>
@@ -34415,19 +34415,19 @@
         <v>45664</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="76" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F15" s="94" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G15" s="92" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H15" s="78" t="s">
         <v>47</v>
@@ -34439,19 +34439,19 @@
         <v>45665</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="76" t="s">
         <v>46</v>
       </c>
       <c r="E16" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F16" s="94" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="92" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H16" s="79" t="s">
         <v>48</v>
@@ -34463,22 +34463,22 @@
         <v>45667</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="76" t="s">
         <v>46</v>
       </c>
       <c r="E17" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F17" s="94" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" s="92" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H17" s="93" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="12.75">
@@ -34496,6 +34496,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EDB39E34F5A9B445B025C05B2A05D030" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c21ef800502b5dc1190a9a0361733939">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f1f31ffb-9912-4459-99c8-b26e82094b51" xmlns:ns4="ce621958-37b1-43fe-a1f1-1aad67996a88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30daf50bb6192471b76b9808b4256f50" ns3:_="" ns4:_="">
     <xsd:import namespace="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
@@ -34690,24 +34707,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D01A9D5D-1824-48C2-8527-9D8749A8DDDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34724,29 +34749,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Carga de los reportes de prueba
</commit_message>
<xml_diff>
--- a/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
+++ b/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATIAS\Desktop\ESPE\Septimo_Semestre\Quality Assurance\Repo\2563_G3_ACSW\02_Proyecto\09. Programa de Auditoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95CB2D8-2F87-47C0-A395-0AC9CB52F16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EC0227-981D-4A5B-AF7D-DD11F7B5BBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2722,7 +2722,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2887,7 +2887,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3076,21 +3075,33 @@
     <xf numFmtId="10" fontId="48" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="19" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="8" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3100,10 +3111,50 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="50" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3111,57 +3162,27 @@
     <xf numFmtId="10" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="44" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3173,6 +3194,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3183,6 +3208,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3205,89 +3233,63 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="19" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="50" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3298,15 +3300,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="8" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3573,8 +3570,8 @@
   </sheetPr>
   <dimension ref="A1:AW998"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A30" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AB7"/>
+    <sheetView showGridLines="0" topLeftCell="A29" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AB31" sqref="AB31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -3609,37 +3606,37 @@
     </row>
     <row r="2" spans="1:48" ht="42.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="156"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="159"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="136"/>
-      <c r="M2" s="136"/>
-      <c r="N2" s="136"/>
-      <c r="O2" s="136"/>
-      <c r="P2" s="136"/>
-      <c r="Q2" s="137"/>
-      <c r="R2" s="160" t="s">
+      <c r="B2" s="205"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
+      <c r="L2" s="164"/>
+      <c r="M2" s="164"/>
+      <c r="N2" s="164"/>
+      <c r="O2" s="164"/>
+      <c r="P2" s="164"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="203" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="161"/>
-      <c r="T2" s="161"/>
-      <c r="U2" s="161"/>
-      <c r="V2" s="161"/>
-      <c r="W2" s="136"/>
-      <c r="X2" s="136"/>
-      <c r="Y2" s="137"/>
-      <c r="Z2" s="160" t="s">
+      <c r="S2" s="207"/>
+      <c r="T2" s="207"/>
+      <c r="U2" s="207"/>
+      <c r="V2" s="207"/>
+      <c r="W2" s="164"/>
+      <c r="X2" s="164"/>
+      <c r="Y2" s="165"/>
+      <c r="Z2" s="203" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="136"/>
-      <c r="AB2" s="137"/>
+      <c r="AA2" s="164"/>
+      <c r="AB2" s="165"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -3663,37 +3660,37 @@
     </row>
     <row r="3" spans="1:48" ht="48.75" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="157"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="158"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="136"/>
-      <c r="L3" s="136"/>
-      <c r="M3" s="136"/>
-      <c r="N3" s="136"/>
-      <c r="O3" s="136"/>
-      <c r="P3" s="136"/>
-      <c r="Q3" s="137"/>
-      <c r="R3" s="163" t="s">
+      <c r="B3" s="183"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="164"/>
+      <c r="J3" s="164"/>
+      <c r="K3" s="164"/>
+      <c r="L3" s="164"/>
+      <c r="M3" s="164"/>
+      <c r="N3" s="164"/>
+      <c r="O3" s="164"/>
+      <c r="P3" s="164"/>
+      <c r="Q3" s="165"/>
+      <c r="R3" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="164"/>
-      <c r="T3" s="164"/>
-      <c r="U3" s="164"/>
-      <c r="V3" s="164"/>
-      <c r="W3" s="136"/>
-      <c r="X3" s="136"/>
-      <c r="Y3" s="137"/>
-      <c r="Z3" s="160" t="s">
+      <c r="S3" s="202"/>
+      <c r="T3" s="202"/>
+      <c r="U3" s="202"/>
+      <c r="V3" s="202"/>
+      <c r="W3" s="164"/>
+      <c r="X3" s="164"/>
+      <c r="Y3" s="165"/>
+      <c r="Z3" s="203" t="s">
         <v>49</v>
       </c>
-      <c r="AA3" s="136"/>
-      <c r="AB3" s="137"/>
+      <c r="AA3" s="164"/>
+      <c r="AB3" s="165"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
@@ -3717,39 +3714,39 @@
     </row>
     <row r="4" spans="1:48" ht="21" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="165" t="s">
+      <c r="B4" s="199" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="166"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="136"/>
-      <c r="L4" s="136"/>
-      <c r="M4" s="136"/>
-      <c r="N4" s="136"/>
-      <c r="O4" s="136"/>
-      <c r="P4" s="136"/>
-      <c r="Q4" s="137"/>
-      <c r="R4" s="163" t="s">
+      <c r="C4" s="164"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="164"/>
+      <c r="F4" s="165"/>
+      <c r="G4" s="200"/>
+      <c r="H4" s="164"/>
+      <c r="I4" s="164"/>
+      <c r="J4" s="164"/>
+      <c r="K4" s="164"/>
+      <c r="L4" s="164"/>
+      <c r="M4" s="164"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="164"/>
+      <c r="P4" s="164"/>
+      <c r="Q4" s="165"/>
+      <c r="R4" s="201" t="s">
         <v>75</v>
       </c>
-      <c r="S4" s="164"/>
-      <c r="T4" s="164"/>
-      <c r="U4" s="164"/>
-      <c r="V4" s="164"/>
-      <c r="W4" s="136"/>
-      <c r="X4" s="136"/>
-      <c r="Y4" s="137"/>
-      <c r="Z4" s="160" t="s">
+      <c r="S4" s="202"/>
+      <c r="T4" s="202"/>
+      <c r="U4" s="202"/>
+      <c r="V4" s="202"/>
+      <c r="W4" s="164"/>
+      <c r="X4" s="164"/>
+      <c r="Y4" s="165"/>
+      <c r="Z4" s="203" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="136"/>
-      <c r="AB4" s="137"/>
+      <c r="AA4" s="164"/>
+      <c r="AB4" s="165"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
@@ -3822,35 +3819,35 @@
       <c r="AV5" s="2"/>
     </row>
     <row r="6" spans="1:48" ht="81.75" customHeight="1">
-      <c r="B6" s="167" t="s">
+      <c r="B6" s="204" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="146"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="146"/>
-      <c r="J6" s="146"/>
-      <c r="K6" s="146"/>
-      <c r="L6" s="146"/>
-      <c r="M6" s="146"/>
-      <c r="N6" s="146"/>
-      <c r="O6" s="146"/>
-      <c r="P6" s="146"/>
-      <c r="Q6" s="146"/>
-      <c r="R6" s="146"/>
-      <c r="S6" s="146"/>
-      <c r="T6" s="146"/>
-      <c r="U6" s="146"/>
-      <c r="V6" s="146"/>
-      <c r="W6" s="146"/>
-      <c r="X6" s="146"/>
-      <c r="Y6" s="146"/>
-      <c r="Z6" s="146"/>
-      <c r="AA6" s="146"/>
-      <c r="AB6" s="146"/>
+      <c r="C6" s="177"/>
+      <c r="D6" s="177"/>
+      <c r="E6" s="177"/>
+      <c r="F6" s="177"/>
+      <c r="G6" s="177"/>
+      <c r="H6" s="177"/>
+      <c r="I6" s="177"/>
+      <c r="J6" s="177"/>
+      <c r="K6" s="177"/>
+      <c r="L6" s="177"/>
+      <c r="M6" s="177"/>
+      <c r="N6" s="177"/>
+      <c r="O6" s="177"/>
+      <c r="P6" s="177"/>
+      <c r="Q6" s="177"/>
+      <c r="R6" s="177"/>
+      <c r="S6" s="177"/>
+      <c r="T6" s="177"/>
+      <c r="U6" s="177"/>
+      <c r="V6" s="177"/>
+      <c r="W6" s="177"/>
+      <c r="X6" s="177"/>
+      <c r="Y6" s="177"/>
+      <c r="Z6" s="177"/>
+      <c r="AA6" s="177"/>
+      <c r="AB6" s="177"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="6"/>
@@ -3867,35 +3864,35 @@
       <c r="AP6" s="7"/>
     </row>
     <row r="7" spans="1:48" ht="198" customHeight="1">
-      <c r="B7" s="168" t="s">
+      <c r="B7" s="176" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="146"/>
-      <c r="D7" s="146"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="146"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="146"/>
-      <c r="K7" s="146"/>
-      <c r="L7" s="146"/>
-      <c r="M7" s="146"/>
-      <c r="N7" s="146"/>
-      <c r="O7" s="146"/>
-      <c r="P7" s="146"/>
-      <c r="Q7" s="146"/>
-      <c r="R7" s="146"/>
-      <c r="S7" s="146"/>
-      <c r="T7" s="146"/>
-      <c r="U7" s="146"/>
-      <c r="V7" s="146"/>
-      <c r="W7" s="146"/>
-      <c r="X7" s="146"/>
-      <c r="Y7" s="146"/>
-      <c r="Z7" s="146"/>
-      <c r="AA7" s="146"/>
-      <c r="AB7" s="146"/>
+      <c r="C7" s="177"/>
+      <c r="D7" s="177"/>
+      <c r="E7" s="177"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="177"/>
+      <c r="L7" s="177"/>
+      <c r="M7" s="177"/>
+      <c r="N7" s="177"/>
+      <c r="O7" s="177"/>
+      <c r="P7" s="177"/>
+      <c r="Q7" s="177"/>
+      <c r="R7" s="177"/>
+      <c r="S7" s="177"/>
+      <c r="T7" s="177"/>
+      <c r="U7" s="177"/>
+      <c r="V7" s="177"/>
+      <c r="W7" s="177"/>
+      <c r="X7" s="177"/>
+      <c r="Y7" s="177"/>
+      <c r="Z7" s="177"/>
+      <c r="AA7" s="177"/>
+      <c r="AB7" s="177"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
       <c r="AE7" s="6"/>
@@ -3912,35 +3909,35 @@
       <c r="AP7" s="7"/>
     </row>
     <row r="8" spans="1:48" ht="51" customHeight="1">
-      <c r="B8" s="169" t="s">
+      <c r="B8" s="198" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="146"/>
-      <c r="H8" s="146"/>
-      <c r="I8" s="146"/>
-      <c r="J8" s="146"/>
-      <c r="K8" s="146"/>
-      <c r="L8" s="146"/>
-      <c r="M8" s="146"/>
-      <c r="N8" s="146"/>
-      <c r="O8" s="146"/>
-      <c r="P8" s="146"/>
-      <c r="Q8" s="146"/>
-      <c r="R8" s="146"/>
-      <c r="S8" s="146"/>
-      <c r="T8" s="146"/>
-      <c r="U8" s="146"/>
-      <c r="V8" s="146"/>
-      <c r="W8" s="146"/>
-      <c r="X8" s="146"/>
-      <c r="Y8" s="146"/>
-      <c r="Z8" s="146"/>
-      <c r="AA8" s="146"/>
-      <c r="AB8" s="146"/>
+      <c r="C8" s="177"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="177"/>
+      <c r="F8" s="177"/>
+      <c r="G8" s="177"/>
+      <c r="H8" s="177"/>
+      <c r="I8" s="177"/>
+      <c r="J8" s="177"/>
+      <c r="K8" s="177"/>
+      <c r="L8" s="177"/>
+      <c r="M8" s="177"/>
+      <c r="N8" s="177"/>
+      <c r="O8" s="177"/>
+      <c r="P8" s="177"/>
+      <c r="Q8" s="177"/>
+      <c r="R8" s="177"/>
+      <c r="S8" s="177"/>
+      <c r="T8" s="177"/>
+      <c r="U8" s="177"/>
+      <c r="V8" s="177"/>
+      <c r="W8" s="177"/>
+      <c r="X8" s="177"/>
+      <c r="Y8" s="177"/>
+      <c r="Z8" s="177"/>
+      <c r="AA8" s="177"/>
+      <c r="AB8" s="177"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="6"/>
@@ -4000,35 +3997,35 @@
       <c r="AP9" s="7"/>
     </row>
     <row r="10" spans="1:48" ht="20.25" customHeight="1">
-      <c r="B10" s="169" t="s">
+      <c r="B10" s="198" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="146"/>
-      <c r="D10" s="146"/>
-      <c r="E10" s="146"/>
-      <c r="F10" s="146"/>
-      <c r="G10" s="146"/>
-      <c r="H10" s="146"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="146"/>
-      <c r="K10" s="146"/>
-      <c r="L10" s="146"/>
-      <c r="M10" s="146"/>
-      <c r="N10" s="146"/>
-      <c r="O10" s="146"/>
-      <c r="P10" s="146"/>
-      <c r="Q10" s="146"/>
-      <c r="R10" s="146"/>
-      <c r="S10" s="146"/>
-      <c r="T10" s="146"/>
-      <c r="U10" s="146"/>
-      <c r="V10" s="146"/>
-      <c r="W10" s="146"/>
-      <c r="X10" s="146"/>
-      <c r="Y10" s="146"/>
-      <c r="Z10" s="146"/>
-      <c r="AA10" s="146"/>
-      <c r="AB10" s="146"/>
+      <c r="C10" s="177"/>
+      <c r="D10" s="177"/>
+      <c r="E10" s="177"/>
+      <c r="F10" s="177"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="177"/>
+      <c r="I10" s="177"/>
+      <c r="J10" s="177"/>
+      <c r="K10" s="177"/>
+      <c r="L10" s="177"/>
+      <c r="M10" s="177"/>
+      <c r="N10" s="177"/>
+      <c r="O10" s="177"/>
+      <c r="P10" s="177"/>
+      <c r="Q10" s="177"/>
+      <c r="R10" s="177"/>
+      <c r="S10" s="177"/>
+      <c r="T10" s="177"/>
+      <c r="U10" s="177"/>
+      <c r="V10" s="177"/>
+      <c r="W10" s="177"/>
+      <c r="X10" s="177"/>
+      <c r="Y10" s="177"/>
+      <c r="Z10" s="177"/>
+      <c r="AA10" s="177"/>
+      <c r="AB10" s="177"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="6"/>
@@ -4046,35 +4043,35 @@
     </row>
     <row r="11" spans="1:48" ht="60" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="168" t="s">
+      <c r="B11" s="176" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="146"/>
-      <c r="D11" s="146"/>
-      <c r="E11" s="146"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="146"/>
-      <c r="I11" s="146"/>
-      <c r="J11" s="146"/>
-      <c r="K11" s="146"/>
-      <c r="L11" s="146"/>
-      <c r="M11" s="146"/>
-      <c r="N11" s="146"/>
-      <c r="O11" s="146"/>
-      <c r="P11" s="146"/>
-      <c r="Q11" s="146"/>
-      <c r="R11" s="146"/>
-      <c r="S11" s="146"/>
-      <c r="T11" s="146"/>
-      <c r="U11" s="146"/>
-      <c r="V11" s="146"/>
-      <c r="W11" s="146"/>
-      <c r="X11" s="146"/>
-      <c r="Y11" s="146"/>
-      <c r="Z11" s="146"/>
-      <c r="AA11" s="146"/>
-      <c r="AB11" s="146"/>
+      <c r="C11" s="177"/>
+      <c r="D11" s="177"/>
+      <c r="E11" s="177"/>
+      <c r="F11" s="177"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="177"/>
+      <c r="I11" s="177"/>
+      <c r="J11" s="177"/>
+      <c r="K11" s="177"/>
+      <c r="L11" s="177"/>
+      <c r="M11" s="177"/>
+      <c r="N11" s="177"/>
+      <c r="O11" s="177"/>
+      <c r="P11" s="177"/>
+      <c r="Q11" s="177"/>
+      <c r="R11" s="177"/>
+      <c r="S11" s="177"/>
+      <c r="T11" s="177"/>
+      <c r="U11" s="177"/>
+      <c r="V11" s="177"/>
+      <c r="W11" s="177"/>
+      <c r="X11" s="177"/>
+      <c r="Y11" s="177"/>
+      <c r="Z11" s="177"/>
+      <c r="AA11" s="177"/>
+      <c r="AB11" s="177"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="9"/>
       <c r="AE11" s="9"/>
@@ -4097,35 +4094,35 @@
       <c r="AV11" s="8"/>
     </row>
     <row r="12" spans="1:48" ht="53.25" customHeight="1">
-      <c r="B12" s="168" t="s">
+      <c r="B12" s="176" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="146"/>
-      <c r="D12" s="146"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="146"/>
-      <c r="K12" s="146"/>
-      <c r="L12" s="146"/>
-      <c r="M12" s="146"/>
-      <c r="N12" s="146"/>
-      <c r="O12" s="146"/>
-      <c r="P12" s="146"/>
-      <c r="Q12" s="146"/>
-      <c r="R12" s="146"/>
-      <c r="S12" s="146"/>
-      <c r="T12" s="146"/>
-      <c r="U12" s="146"/>
-      <c r="V12" s="146"/>
-      <c r="W12" s="146"/>
-      <c r="X12" s="146"/>
-      <c r="Y12" s="146"/>
-      <c r="Z12" s="146"/>
-      <c r="AA12" s="146"/>
-      <c r="AB12" s="146"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="177"/>
+      <c r="E12" s="177"/>
+      <c r="F12" s="177"/>
+      <c r="G12" s="177"/>
+      <c r="H12" s="177"/>
+      <c r="I12" s="177"/>
+      <c r="J12" s="177"/>
+      <c r="K12" s="177"/>
+      <c r="L12" s="177"/>
+      <c r="M12" s="177"/>
+      <c r="N12" s="177"/>
+      <c r="O12" s="177"/>
+      <c r="P12" s="177"/>
+      <c r="Q12" s="177"/>
+      <c r="R12" s="177"/>
+      <c r="S12" s="177"/>
+      <c r="T12" s="177"/>
+      <c r="U12" s="177"/>
+      <c r="V12" s="177"/>
+      <c r="W12" s="177"/>
+      <c r="X12" s="177"/>
+      <c r="Y12" s="177"/>
+      <c r="Z12" s="177"/>
+      <c r="AA12" s="177"/>
+      <c r="AB12" s="177"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
@@ -4142,35 +4139,35 @@
       <c r="AP12" s="7"/>
     </row>
     <row r="13" spans="1:48" ht="39.75" customHeight="1">
-      <c r="B13" s="168" t="s">
+      <c r="B13" s="176" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="146"/>
-      <c r="D13" s="146"/>
-      <c r="E13" s="146"/>
-      <c r="F13" s="146"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="146"/>
-      <c r="K13" s="146"/>
-      <c r="L13" s="146"/>
-      <c r="M13" s="146"/>
-      <c r="N13" s="146"/>
-      <c r="O13" s="146"/>
-      <c r="P13" s="146"/>
-      <c r="Q13" s="146"/>
-      <c r="R13" s="146"/>
-      <c r="S13" s="146"/>
-      <c r="T13" s="146"/>
-      <c r="U13" s="146"/>
-      <c r="V13" s="146"/>
-      <c r="W13" s="146"/>
-      <c r="X13" s="146"/>
-      <c r="Y13" s="146"/>
-      <c r="Z13" s="146"/>
-      <c r="AA13" s="146"/>
-      <c r="AB13" s="146"/>
+      <c r="C13" s="177"/>
+      <c r="D13" s="177"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="177"/>
+      <c r="H13" s="177"/>
+      <c r="I13" s="177"/>
+      <c r="J13" s="177"/>
+      <c r="K13" s="177"/>
+      <c r="L13" s="177"/>
+      <c r="M13" s="177"/>
+      <c r="N13" s="177"/>
+      <c r="O13" s="177"/>
+      <c r="P13" s="177"/>
+      <c r="Q13" s="177"/>
+      <c r="R13" s="177"/>
+      <c r="S13" s="177"/>
+      <c r="T13" s="177"/>
+      <c r="U13" s="177"/>
+      <c r="V13" s="177"/>
+      <c r="W13" s="177"/>
+      <c r="X13" s="177"/>
+      <c r="Y13" s="177"/>
+      <c r="Z13" s="177"/>
+      <c r="AA13" s="177"/>
+      <c r="AB13" s="177"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
@@ -4230,35 +4227,35 @@
       <c r="AP14" s="7"/>
     </row>
     <row r="15" spans="1:48" ht="99.75" customHeight="1">
-      <c r="B15" s="173" t="s">
+      <c r="B15" s="178" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="146"/>
-      <c r="D15" s="146"/>
-      <c r="E15" s="146"/>
-      <c r="F15" s="146"/>
-      <c r="G15" s="146"/>
-      <c r="H15" s="146"/>
-      <c r="I15" s="146"/>
-      <c r="J15" s="146"/>
-      <c r="K15" s="146"/>
-      <c r="L15" s="146"/>
-      <c r="M15" s="146"/>
-      <c r="N15" s="146"/>
-      <c r="O15" s="146"/>
-      <c r="P15" s="146"/>
-      <c r="Q15" s="146"/>
-      <c r="R15" s="146"/>
-      <c r="S15" s="146"/>
-      <c r="T15" s="146"/>
-      <c r="U15" s="146"/>
-      <c r="V15" s="146"/>
-      <c r="W15" s="146"/>
-      <c r="X15" s="146"/>
-      <c r="Y15" s="146"/>
-      <c r="Z15" s="146"/>
-      <c r="AA15" s="146"/>
-      <c r="AB15" s="146"/>
+      <c r="C15" s="177"/>
+      <c r="D15" s="177"/>
+      <c r="E15" s="177"/>
+      <c r="F15" s="177"/>
+      <c r="G15" s="177"/>
+      <c r="H15" s="177"/>
+      <c r="I15" s="177"/>
+      <c r="J15" s="177"/>
+      <c r="K15" s="177"/>
+      <c r="L15" s="177"/>
+      <c r="M15" s="177"/>
+      <c r="N15" s="177"/>
+      <c r="O15" s="177"/>
+      <c r="P15" s="177"/>
+      <c r="Q15" s="177"/>
+      <c r="R15" s="177"/>
+      <c r="S15" s="177"/>
+      <c r="T15" s="177"/>
+      <c r="U15" s="177"/>
+      <c r="V15" s="177"/>
+      <c r="W15" s="177"/>
+      <c r="X15" s="177"/>
+      <c r="Y15" s="177"/>
+      <c r="Z15" s="177"/>
+      <c r="AA15" s="177"/>
+      <c r="AB15" s="177"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="6"/>
@@ -4276,35 +4273,35 @@
     </row>
     <row r="16" spans="1:48" ht="24.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="174" t="s">
+      <c r="B16" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="146"/>
-      <c r="D16" s="146"/>
-      <c r="E16" s="146"/>
-      <c r="F16" s="146"/>
-      <c r="G16" s="146"/>
-      <c r="H16" s="146"/>
-      <c r="I16" s="146"/>
-      <c r="J16" s="146"/>
-      <c r="K16" s="146"/>
-      <c r="L16" s="146"/>
-      <c r="M16" s="146"/>
-      <c r="N16" s="146"/>
-      <c r="O16" s="146"/>
-      <c r="P16" s="146"/>
-      <c r="Q16" s="146"/>
-      <c r="R16" s="146"/>
-      <c r="S16" s="146"/>
-      <c r="T16" s="146"/>
-      <c r="U16" s="146"/>
-      <c r="V16" s="146"/>
-      <c r="W16" s="146"/>
-      <c r="X16" s="146"/>
-      <c r="Y16" s="146"/>
-      <c r="Z16" s="146"/>
-      <c r="AA16" s="146"/>
-      <c r="AB16" s="146"/>
+      <c r="C16" s="177"/>
+      <c r="D16" s="177"/>
+      <c r="E16" s="177"/>
+      <c r="F16" s="177"/>
+      <c r="G16" s="177"/>
+      <c r="H16" s="177"/>
+      <c r="I16" s="177"/>
+      <c r="J16" s="177"/>
+      <c r="K16" s="177"/>
+      <c r="L16" s="177"/>
+      <c r="M16" s="177"/>
+      <c r="N16" s="177"/>
+      <c r="O16" s="177"/>
+      <c r="P16" s="177"/>
+      <c r="Q16" s="177"/>
+      <c r="R16" s="177"/>
+      <c r="S16" s="177"/>
+      <c r="T16" s="177"/>
+      <c r="U16" s="177"/>
+      <c r="V16" s="177"/>
+      <c r="W16" s="177"/>
+      <c r="X16" s="177"/>
+      <c r="Y16" s="177"/>
+      <c r="Z16" s="177"/>
+      <c r="AA16" s="177"/>
+      <c r="AB16" s="177"/>
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
@@ -4327,35 +4324,35 @@
       <c r="AV16" s="2"/>
     </row>
     <row r="17" spans="1:49" ht="24.75" customHeight="1">
-      <c r="B17" s="173" t="s">
+      <c r="B17" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="146"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
-      <c r="G17" s="146"/>
-      <c r="H17" s="146"/>
-      <c r="I17" s="146"/>
-      <c r="J17" s="146"/>
-      <c r="K17" s="146"/>
-      <c r="L17" s="146"/>
-      <c r="M17" s="146"/>
-      <c r="N17" s="146"/>
-      <c r="O17" s="146"/>
-      <c r="P17" s="146"/>
-      <c r="Q17" s="146"/>
-      <c r="R17" s="146"/>
-      <c r="S17" s="146"/>
-      <c r="T17" s="146"/>
-      <c r="U17" s="146"/>
-      <c r="V17" s="146"/>
-      <c r="W17" s="146"/>
-      <c r="X17" s="146"/>
-      <c r="Y17" s="146"/>
-      <c r="Z17" s="146"/>
-      <c r="AA17" s="146"/>
-      <c r="AB17" s="146"/>
+      <c r="C17" s="177"/>
+      <c r="D17" s="177"/>
+      <c r="E17" s="177"/>
+      <c r="F17" s="177"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="177"/>
+      <c r="I17" s="177"/>
+      <c r="J17" s="177"/>
+      <c r="K17" s="177"/>
+      <c r="L17" s="177"/>
+      <c r="M17" s="177"/>
+      <c r="N17" s="177"/>
+      <c r="O17" s="177"/>
+      <c r="P17" s="177"/>
+      <c r="Q17" s="177"/>
+      <c r="R17" s="177"/>
+      <c r="S17" s="177"/>
+      <c r="T17" s="177"/>
+      <c r="U17" s="177"/>
+      <c r="V17" s="177"/>
+      <c r="W17" s="177"/>
+      <c r="X17" s="177"/>
+      <c r="Y17" s="177"/>
+      <c r="Z17" s="177"/>
+      <c r="AA17" s="177"/>
+      <c r="AB17" s="177"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="6"/>
@@ -4372,33 +4369,33 @@
       <c r="AP17" s="7"/>
     </row>
     <row r="18" spans="1:49" ht="6.75" customHeight="1">
-      <c r="B18" s="173"/>
-      <c r="C18" s="146"/>
-      <c r="D18" s="146"/>
-      <c r="E18" s="146"/>
-      <c r="F18" s="146"/>
-      <c r="G18" s="146"/>
-      <c r="H18" s="146"/>
-      <c r="I18" s="146"/>
-      <c r="J18" s="146"/>
-      <c r="K18" s="146"/>
-      <c r="L18" s="146"/>
-      <c r="M18" s="146"/>
-      <c r="N18" s="146"/>
-      <c r="O18" s="146"/>
-      <c r="P18" s="146"/>
-      <c r="Q18" s="146"/>
-      <c r="R18" s="146"/>
-      <c r="S18" s="146"/>
-      <c r="T18" s="146"/>
-      <c r="U18" s="146"/>
-      <c r="V18" s="146"/>
-      <c r="W18" s="146"/>
-      <c r="X18" s="146"/>
-      <c r="Y18" s="146"/>
-      <c r="Z18" s="146"/>
-      <c r="AA18" s="146"/>
-      <c r="AB18" s="146"/>
+      <c r="B18" s="178"/>
+      <c r="C18" s="177"/>
+      <c r="D18" s="177"/>
+      <c r="E18" s="177"/>
+      <c r="F18" s="177"/>
+      <c r="G18" s="177"/>
+      <c r="H18" s="177"/>
+      <c r="I18" s="177"/>
+      <c r="J18" s="177"/>
+      <c r="K18" s="177"/>
+      <c r="L18" s="177"/>
+      <c r="M18" s="177"/>
+      <c r="N18" s="177"/>
+      <c r="O18" s="177"/>
+      <c r="P18" s="177"/>
+      <c r="Q18" s="177"/>
+      <c r="R18" s="177"/>
+      <c r="S18" s="177"/>
+      <c r="T18" s="177"/>
+      <c r="U18" s="177"/>
+      <c r="V18" s="177"/>
+      <c r="W18" s="177"/>
+      <c r="X18" s="177"/>
+      <c r="Y18" s="177"/>
+      <c r="Z18" s="177"/>
+      <c r="AA18" s="177"/>
+      <c r="AB18" s="177"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
@@ -4416,45 +4413,45 @@
     </row>
     <row r="19" spans="1:49" ht="36.75" customHeight="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="182" t="s">
+      <c r="B19" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="185" t="s">
+      <c r="C19" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="176"/>
-      <c r="E19" s="177"/>
-      <c r="F19" s="186" t="s">
+      <c r="D19" s="181"/>
+      <c r="E19" s="182"/>
+      <c r="F19" s="194" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="175" t="s">
+      <c r="G19" s="180" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176"/>
-      <c r="J19" s="176"/>
-      <c r="K19" s="176"/>
-      <c r="L19" s="176"/>
-      <c r="M19" s="176"/>
-      <c r="N19" s="177"/>
-      <c r="O19" s="175" t="s">
+      <c r="H19" s="181"/>
+      <c r="I19" s="181"/>
+      <c r="J19" s="181"/>
+      <c r="K19" s="181"/>
+      <c r="L19" s="181"/>
+      <c r="M19" s="181"/>
+      <c r="N19" s="182"/>
+      <c r="O19" s="180" t="s">
         <v>52</v>
       </c>
-      <c r="P19" s="176"/>
-      <c r="Q19" s="176"/>
-      <c r="R19" s="176"/>
-      <c r="S19" s="176"/>
-      <c r="T19" s="176"/>
-      <c r="U19" s="176"/>
-      <c r="V19" s="176"/>
-      <c r="W19" s="177"/>
-      <c r="X19" s="178" t="s">
+      <c r="P19" s="181"/>
+      <c r="Q19" s="181"/>
+      <c r="R19" s="181"/>
+      <c r="S19" s="181"/>
+      <c r="T19" s="181"/>
+      <c r="U19" s="181"/>
+      <c r="V19" s="181"/>
+      <c r="W19" s="182"/>
+      <c r="X19" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Y19" s="176"/>
-      <c r="Z19" s="176"/>
-      <c r="AA19" s="177"/>
-      <c r="AB19" s="74" t="s">
+      <c r="Y19" s="181"/>
+      <c r="Z19" s="181"/>
+      <c r="AA19" s="182"/>
+      <c r="AB19" s="73" t="s">
         <v>9</v>
       </c>
       <c r="AC19" s="14"/>
@@ -4480,33 +4477,33 @@
     </row>
     <row r="20" spans="1:49" ht="10.5" customHeight="1">
       <c r="A20" s="14"/>
-      <c r="B20" s="183"/>
-      <c r="C20" s="179"/>
-      <c r="D20" s="146"/>
-      <c r="E20" s="180"/>
-      <c r="F20" s="187"/>
-      <c r="G20" s="157"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="141"/>
-      <c r="K20" s="141"/>
-      <c r="L20" s="141"/>
-      <c r="M20" s="141"/>
-      <c r="N20" s="158"/>
-      <c r="O20" s="179"/>
-      <c r="P20" s="189"/>
-      <c r="Q20" s="189"/>
-      <c r="R20" s="189"/>
-      <c r="S20" s="189"/>
-      <c r="T20" s="189"/>
-      <c r="U20" s="189"/>
-      <c r="V20" s="189"/>
-      <c r="W20" s="180"/>
-      <c r="X20" s="179"/>
-      <c r="Y20" s="146"/>
-      <c r="Z20" s="146"/>
-      <c r="AA20" s="180"/>
-      <c r="AB20" s="75"/>
+      <c r="B20" s="191"/>
+      <c r="C20" s="187"/>
+      <c r="D20" s="177"/>
+      <c r="E20" s="188"/>
+      <c r="F20" s="195"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="184"/>
+      <c r="I20" s="184"/>
+      <c r="J20" s="184"/>
+      <c r="K20" s="184"/>
+      <c r="L20" s="184"/>
+      <c r="M20" s="184"/>
+      <c r="N20" s="185"/>
+      <c r="O20" s="187"/>
+      <c r="P20" s="197"/>
+      <c r="Q20" s="197"/>
+      <c r="R20" s="197"/>
+      <c r="S20" s="197"/>
+      <c r="T20" s="197"/>
+      <c r="U20" s="197"/>
+      <c r="V20" s="197"/>
+      <c r="W20" s="188"/>
+      <c r="X20" s="187"/>
+      <c r="Y20" s="177"/>
+      <c r="Z20" s="177"/>
+      <c r="AA20" s="188"/>
+      <c r="AB20" s="74"/>
       <c r="AC20" s="14"/>
       <c r="AD20" s="14"/>
       <c r="AE20" s="14"/>
@@ -4530,49 +4527,49 @@
     </row>
     <row r="21" spans="1:49" ht="34.5" customHeight="1">
       <c r="A21" s="15"/>
-      <c r="B21" s="183"/>
-      <c r="C21" s="179"/>
-      <c r="D21" s="146"/>
-      <c r="E21" s="180"/>
-      <c r="F21" s="187"/>
-      <c r="G21" s="181" t="s">
+      <c r="B21" s="191"/>
+      <c r="C21" s="187"/>
+      <c r="D21" s="177"/>
+      <c r="E21" s="188"/>
+      <c r="F21" s="195"/>
+      <c r="G21" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="137"/>
-      <c r="I21" s="181" t="s">
+      <c r="H21" s="165"/>
+      <c r="I21" s="189" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="137"/>
-      <c r="K21" s="181" t="s">
+      <c r="J21" s="165"/>
+      <c r="K21" s="189" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="137"/>
-      <c r="M21" s="181" t="s">
+      <c r="L21" s="165"/>
+      <c r="M21" s="189" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="136"/>
-      <c r="O21" s="201" t="s">
+      <c r="N21" s="164"/>
+      <c r="O21" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="P21" s="201"/>
-      <c r="Q21" s="201"/>
-      <c r="R21" s="201"/>
-      <c r="S21" s="200" t="s">
+      <c r="P21" s="156"/>
+      <c r="Q21" s="156"/>
+      <c r="R21" s="156"/>
+      <c r="S21" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="T21" s="201"/>
-      <c r="U21" s="81" t="s">
+      <c r="T21" s="156"/>
+      <c r="U21" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="V21" s="81" t="s">
+      <c r="V21" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="W21" s="78"/>
-      <c r="X21" s="141"/>
-      <c r="Y21" s="141"/>
-      <c r="Z21" s="141"/>
-      <c r="AA21" s="158"/>
-      <c r="AB21" s="75"/>
+      <c r="W21" s="77"/>
+      <c r="X21" s="184"/>
+      <c r="Y21" s="184"/>
+      <c r="Z21" s="184"/>
+      <c r="AA21" s="185"/>
+      <c r="AB21" s="74"/>
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
       <c r="AE21" s="15"/>
@@ -4596,11 +4593,11 @@
     </row>
     <row r="22" spans="1:49" ht="38.25" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="184"/>
-      <c r="C22" s="157"/>
-      <c r="D22" s="141"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="188"/>
+      <c r="B22" s="192"/>
+      <c r="C22" s="183"/>
+      <c r="D22" s="184"/>
+      <c r="E22" s="185"/>
+      <c r="F22" s="196"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
@@ -4618,38 +4615,38 @@
       <c r="M22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="N22" s="73" t="s">
+      <c r="N22" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="O22" s="80" t="s">
+      <c r="O22" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="P22" s="80" t="s">
+      <c r="P22" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="Q22" s="191">
+      <c r="Q22" s="169">
         <v>10</v>
       </c>
-      <c r="R22" s="192"/>
-      <c r="S22" s="79" t="s">
+      <c r="R22" s="170"/>
+      <c r="S22" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="T22" s="77" t="s">
+      <c r="T22" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="U22" s="77" t="s">
+      <c r="U22" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="V22" s="77" t="s">
+      <c r="V22" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="W22" s="77"/>
-      <c r="X22" s="77"/>
-      <c r="Y22" s="190"/>
-      <c r="Z22" s="136"/>
-      <c r="AA22" s="136"/>
-      <c r="AB22" s="137"/>
-      <c r="AC22" s="76"/>
+      <c r="W22" s="76"/>
+      <c r="X22" s="76"/>
+      <c r="Y22" s="163"/>
+      <c r="Z22" s="164"/>
+      <c r="AA22" s="164"/>
+      <c r="AB22" s="165"/>
+      <c r="AC22" s="75"/>
       <c r="AD22" s="14"/>
       <c r="AE22" s="14"/>
       <c r="AF22" s="14"/>
@@ -4676,39 +4673,39 @@
       <c r="B23" s="18">
         <v>1</v>
       </c>
-      <c r="C23" s="151" t="s">
+      <c r="C23" s="166" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="152"/>
-      <c r="E23" s="153"/>
-      <c r="F23" s="67">
+      <c r="D23" s="167"/>
+      <c r="E23" s="168"/>
+      <c r="F23" s="66">
         <v>1</v>
       </c>
       <c r="G23" s="20"/>
-      <c r="H23" s="113"/>
-      <c r="I23" s="114" t="s">
+      <c r="H23" s="112"/>
+      <c r="I23" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="114"/>
-      <c r="K23" s="114"/>
-      <c r="L23" s="114"/>
-      <c r="M23" s="114"/>
-      <c r="N23" s="114"/>
-      <c r="O23" s="115"/>
-      <c r="P23" s="115"/>
-      <c r="Q23" s="193"/>
-      <c r="R23" s="194"/>
-      <c r="S23" s="116"/>
-      <c r="T23" s="116"/>
-      <c r="U23" s="116"/>
-      <c r="V23" s="116"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="113"/>
+      <c r="M23" s="113"/>
+      <c r="N23" s="113"/>
+      <c r="O23" s="114"/>
+      <c r="P23" s="114"/>
+      <c r="Q23" s="171"/>
+      <c r="R23" s="172"/>
+      <c r="S23" s="115"/>
+      <c r="T23" s="115"/>
+      <c r="U23" s="115"/>
+      <c r="V23" s="115"/>
       <c r="W23" s="22"/>
-      <c r="X23" s="142" t="s">
+      <c r="X23" s="143" t="s">
         <v>54</v>
       </c>
-      <c r="Y23" s="136"/>
-      <c r="Z23" s="136"/>
-      <c r="AA23" s="137"/>
+      <c r="Y23" s="164"/>
+      <c r="Z23" s="164"/>
+      <c r="AA23" s="165"/>
       <c r="AB23" s="23" t="s">
         <v>55</v>
       </c>
@@ -4728,42 +4725,42 @@
     </row>
     <row r="24" spans="1:49" ht="239.25" customHeight="1">
       <c r="A24" s="17"/>
-      <c r="B24" s="106">
+      <c r="B24" s="105">
         <v>2</v>
       </c>
-      <c r="C24" s="198" t="s">
+      <c r="C24" s="146" t="s">
         <v>190</v>
       </c>
-      <c r="D24" s="199"/>
-      <c r="E24" s="199"/>
-      <c r="F24" s="107">
+      <c r="D24" s="147"/>
+      <c r="E24" s="147"/>
+      <c r="F24" s="106">
         <v>2</v>
       </c>
-      <c r="G24" s="108"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="119" t="s">
+      <c r="G24" s="107"/>
+      <c r="H24" s="116"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="K24" s="120"/>
-      <c r="L24" s="117"/>
-      <c r="M24" s="117"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="117"/>
-      <c r="P24" s="121"/>
-      <c r="Q24" s="202"/>
-      <c r="R24" s="203"/>
-      <c r="S24" s="122"/>
-      <c r="T24" s="117"/>
-      <c r="U24" s="117"/>
-      <c r="V24" s="117"/>
-      <c r="W24" s="109"/>
-      <c r="X24" s="170" t="s">
+      <c r="K24" s="119"/>
+      <c r="L24" s="116"/>
+      <c r="M24" s="116"/>
+      <c r="N24" s="116"/>
+      <c r="O24" s="116"/>
+      <c r="P24" s="120"/>
+      <c r="Q24" s="138"/>
+      <c r="R24" s="139"/>
+      <c r="S24" s="121"/>
+      <c r="T24" s="116"/>
+      <c r="U24" s="116"/>
+      <c r="V24" s="116"/>
+      <c r="W24" s="108"/>
+      <c r="X24" s="173" t="s">
         <v>191</v>
       </c>
-      <c r="Y24" s="171"/>
-      <c r="Z24" s="171"/>
-      <c r="AA24" s="172"/>
+      <c r="Y24" s="174"/>
+      <c r="Z24" s="174"/>
+      <c r="AA24" s="175"/>
       <c r="AB24" s="23" t="s">
         <v>55</v>
       </c>
@@ -4783,42 +4780,42 @@
     </row>
     <row r="25" spans="1:49" ht="159" customHeight="1">
       <c r="A25" s="17"/>
-      <c r="B25" s="106">
+      <c r="B25" s="105">
         <v>3</v>
       </c>
-      <c r="C25" s="198" t="s">
+      <c r="C25" s="146" t="s">
         <v>192</v>
       </c>
-      <c r="D25" s="199"/>
-      <c r="E25" s="199"/>
-      <c r="F25" s="107">
+      <c r="D25" s="147"/>
+      <c r="E25" s="147"/>
+      <c r="F25" s="106">
         <v>3</v>
       </c>
-      <c r="G25" s="108"/>
-      <c r="H25" s="117"/>
-      <c r="I25" s="121"/>
-      <c r="J25" s="123"/>
-      <c r="K25" s="124"/>
-      <c r="L25" s="125"/>
-      <c r="M25" s="117"/>
-      <c r="N25" s="125"/>
-      <c r="O25" s="126" t="s">
+      <c r="G25" s="107"/>
+      <c r="H25" s="116"/>
+      <c r="I25" s="120"/>
+      <c r="J25" s="122"/>
+      <c r="K25" s="123"/>
+      <c r="L25" s="124"/>
+      <c r="M25" s="116"/>
+      <c r="N25" s="124"/>
+      <c r="O25" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="P25" s="127"/>
-      <c r="Q25" s="202"/>
-      <c r="R25" s="203"/>
-      <c r="S25" s="126"/>
-      <c r="T25" s="125"/>
-      <c r="U25" s="117"/>
-      <c r="V25" s="117"/>
-      <c r="W25" s="109"/>
-      <c r="X25" s="208" t="s">
+      <c r="P25" s="126"/>
+      <c r="Q25" s="138"/>
+      <c r="R25" s="139"/>
+      <c r="S25" s="125"/>
+      <c r="T25" s="124"/>
+      <c r="U25" s="116"/>
+      <c r="V25" s="116"/>
+      <c r="W25" s="108"/>
+      <c r="X25" s="135" t="s">
         <v>193</v>
       </c>
-      <c r="Y25" s="209"/>
-      <c r="Z25" s="209"/>
-      <c r="AA25" s="210"/>
+      <c r="Y25" s="136"/>
+      <c r="Z25" s="136"/>
+      <c r="AA25" s="137"/>
       <c r="AB25" s="23" t="s">
         <v>55</v>
       </c>
@@ -4838,42 +4835,42 @@
     </row>
     <row r="26" spans="1:49" ht="108" customHeight="1">
       <c r="A26" s="17"/>
-      <c r="B26" s="106">
+      <c r="B26" s="105">
         <v>4</v>
       </c>
-      <c r="C26" s="198" t="s">
+      <c r="C26" s="146" t="s">
         <v>194</v>
       </c>
-      <c r="D26" s="199"/>
-      <c r="E26" s="199"/>
-      <c r="F26" s="107">
+      <c r="D26" s="147"/>
+      <c r="E26" s="147"/>
+      <c r="F26" s="106">
         <v>4</v>
       </c>
-      <c r="G26" s="108"/>
-      <c r="H26" s="117"/>
-      <c r="I26" s="121"/>
-      <c r="J26" s="123"/>
-      <c r="K26" s="124"/>
-      <c r="L26" s="111"/>
-      <c r="M26" s="128"/>
-      <c r="N26" s="111"/>
-      <c r="O26" s="121"/>
-      <c r="P26" s="112"/>
-      <c r="Q26" s="215"/>
-      <c r="R26" s="216"/>
-      <c r="S26" s="126"/>
-      <c r="T26" s="125" t="s">
+      <c r="G26" s="107"/>
+      <c r="H26" s="116"/>
+      <c r="I26" s="120"/>
+      <c r="J26" s="122"/>
+      <c r="K26" s="123"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="127"/>
+      <c r="N26" s="110"/>
+      <c r="O26" s="120"/>
+      <c r="P26" s="111"/>
+      <c r="Q26" s="152"/>
+      <c r="R26" s="153"/>
+      <c r="S26" s="125"/>
+      <c r="T26" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="U26" s="128"/>
-      <c r="V26" s="117"/>
-      <c r="W26" s="110"/>
-      <c r="X26" s="211" t="s">
+      <c r="U26" s="127"/>
+      <c r="V26" s="116"/>
+      <c r="W26" s="109"/>
+      <c r="X26" s="148" t="s">
         <v>195</v>
       </c>
-      <c r="Y26" s="211"/>
-      <c r="Z26" s="211"/>
-      <c r="AA26" s="211"/>
+      <c r="Y26" s="148"/>
+      <c r="Z26" s="148"/>
+      <c r="AA26" s="148"/>
       <c r="AB26" s="23" t="s">
         <v>55</v>
       </c>
@@ -4893,42 +4890,42 @@
     </row>
     <row r="27" spans="1:49" ht="157.5" customHeight="1">
       <c r="A27" s="17"/>
-      <c r="B27" s="106">
+      <c r="B27" s="105">
         <v>5</v>
       </c>
-      <c r="C27" s="198" t="s">
+      <c r="C27" s="146" t="s">
         <v>196</v>
       </c>
-      <c r="D27" s="199"/>
-      <c r="E27" s="199"/>
-      <c r="F27" s="107">
+      <c r="D27" s="147"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="106">
         <v>5</v>
       </c>
-      <c r="G27" s="108"/>
-      <c r="H27" s="117"/>
-      <c r="I27" s="121"/>
-      <c r="J27" s="123"/>
-      <c r="K27" s="124"/>
-      <c r="L27" s="129"/>
-      <c r="M27" s="130"/>
-      <c r="N27" s="131"/>
-      <c r="O27" s="117"/>
-      <c r="P27" s="111"/>
-      <c r="Q27" s="217"/>
-      <c r="R27" s="217"/>
-      <c r="S27" s="132"/>
-      <c r="T27" s="129"/>
-      <c r="U27" s="130" t="s">
+      <c r="G27" s="107"/>
+      <c r="H27" s="116"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="122"/>
+      <c r="K27" s="123"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="129"/>
+      <c r="N27" s="130"/>
+      <c r="O27" s="116"/>
+      <c r="P27" s="110"/>
+      <c r="Q27" s="154"/>
+      <c r="R27" s="154"/>
+      <c r="S27" s="131"/>
+      <c r="T27" s="128"/>
+      <c r="U27" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="V27" s="131"/>
-      <c r="W27" s="110"/>
-      <c r="X27" s="211" t="s">
+      <c r="V27" s="130"/>
+      <c r="W27" s="109"/>
+      <c r="X27" s="148" t="s">
         <v>197</v>
       </c>
-      <c r="Y27" s="211"/>
-      <c r="Z27" s="211"/>
-      <c r="AA27" s="211"/>
+      <c r="Y27" s="148"/>
+      <c r="Z27" s="148"/>
+      <c r="AA27" s="148"/>
       <c r="AB27" s="23" t="s">
         <v>55</v>
       </c>
@@ -4948,42 +4945,42 @@
     </row>
     <row r="28" spans="1:49" ht="163.5" customHeight="1">
       <c r="A28" s="17"/>
-      <c r="B28" s="106">
+      <c r="B28" s="105">
         <v>6</v>
       </c>
-      <c r="C28" s="198" t="s">
+      <c r="C28" s="146" t="s">
         <v>198</v>
       </c>
-      <c r="D28" s="199"/>
-      <c r="E28" s="199"/>
-      <c r="F28" s="107">
+      <c r="D28" s="147"/>
+      <c r="E28" s="147"/>
+      <c r="F28" s="106">
         <v>6</v>
       </c>
-      <c r="G28" s="108"/>
-      <c r="H28" s="117"/>
-      <c r="I28" s="121"/>
-      <c r="J28" s="123"/>
-      <c r="K28" s="124"/>
-      <c r="L28" s="129"/>
-      <c r="M28" s="130"/>
-      <c r="N28" s="131"/>
-      <c r="O28" s="117"/>
-      <c r="P28" s="121"/>
-      <c r="Q28" s="217"/>
-      <c r="R28" s="217"/>
-      <c r="S28" s="132"/>
-      <c r="T28" s="125"/>
-      <c r="U28" s="130"/>
-      <c r="V28" s="125" t="s">
+      <c r="G28" s="107"/>
+      <c r="H28" s="116"/>
+      <c r="I28" s="120"/>
+      <c r="J28" s="122"/>
+      <c r="K28" s="123"/>
+      <c r="L28" s="128"/>
+      <c r="M28" s="129"/>
+      <c r="N28" s="130"/>
+      <c r="O28" s="116"/>
+      <c r="P28" s="120"/>
+      <c r="Q28" s="154"/>
+      <c r="R28" s="154"/>
+      <c r="S28" s="131"/>
+      <c r="T28" s="124"/>
+      <c r="U28" s="129"/>
+      <c r="V28" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="W28" s="109"/>
-      <c r="X28" s="212" t="s">
+      <c r="W28" s="108"/>
+      <c r="X28" s="149" t="s">
         <v>199</v>
       </c>
-      <c r="Y28" s="213"/>
-      <c r="Z28" s="213"/>
-      <c r="AA28" s="214"/>
+      <c r="Y28" s="150"/>
+      <c r="Z28" s="150"/>
+      <c r="AA28" s="151"/>
       <c r="AB28" s="23" t="s">
         <v>55</v>
       </c>
@@ -5006,39 +5003,39 @@
       <c r="B29" s="18">
         <v>7</v>
       </c>
-      <c r="C29" s="195" t="s">
+      <c r="C29" s="140" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="196"/>
-      <c r="E29" s="197"/>
-      <c r="F29" s="67">
+      <c r="D29" s="141"/>
+      <c r="E29" s="142"/>
+      <c r="F29" s="66">
         <v>7</v>
       </c>
       <c r="G29" s="21"/>
-      <c r="H29" s="114"/>
-      <c r="I29" s="114"/>
-      <c r="J29" s="133"/>
-      <c r="K29" s="133"/>
-      <c r="L29" s="114"/>
-      <c r="M29" s="114"/>
-      <c r="N29" s="114"/>
-      <c r="O29" s="114"/>
-      <c r="P29" s="114"/>
-      <c r="Q29" s="204"/>
-      <c r="R29" s="205"/>
-      <c r="S29" s="116"/>
-      <c r="T29" s="116"/>
-      <c r="U29" s="116"/>
-      <c r="V29" s="134" t="s">
+      <c r="H29" s="113"/>
+      <c r="I29" s="113"/>
+      <c r="J29" s="132"/>
+      <c r="K29" s="132"/>
+      <c r="L29" s="113"/>
+      <c r="M29" s="113"/>
+      <c r="N29" s="113"/>
+      <c r="O29" s="113"/>
+      <c r="P29" s="113"/>
+      <c r="Q29" s="157"/>
+      <c r="R29" s="158"/>
+      <c r="S29" s="115"/>
+      <c r="T29" s="115"/>
+      <c r="U29" s="115"/>
+      <c r="V29" s="133" t="s">
         <v>20</v>
       </c>
       <c r="W29" s="22"/>
-      <c r="X29" s="142" t="s">
+      <c r="X29" s="143" t="s">
         <v>68</v>
       </c>
-      <c r="Y29" s="143"/>
-      <c r="Z29" s="143"/>
-      <c r="AA29" s="144"/>
+      <c r="Y29" s="144"/>
+      <c r="Z29" s="144"/>
+      <c r="AA29" s="145"/>
       <c r="AB29" s="23" t="s">
         <v>60</v>
       </c>
@@ -5068,39 +5065,39 @@
       <c r="B30" s="18">
         <v>8</v>
       </c>
-      <c r="C30" s="195" t="s">
+      <c r="C30" s="140" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="196"/>
-      <c r="E30" s="197"/>
-      <c r="F30" s="67">
+      <c r="D30" s="141"/>
+      <c r="E30" s="142"/>
+      <c r="F30" s="66">
         <v>8</v>
       </c>
       <c r="G30" s="21"/>
-      <c r="H30" s="114"/>
-      <c r="I30" s="114"/>
-      <c r="J30" s="114"/>
-      <c r="K30" s="133"/>
-      <c r="L30" s="133"/>
-      <c r="M30" s="114"/>
-      <c r="N30" s="114"/>
-      <c r="O30" s="114"/>
-      <c r="P30" s="114"/>
-      <c r="Q30" s="206"/>
-      <c r="R30" s="207"/>
-      <c r="S30" s="116"/>
-      <c r="T30" s="116"/>
-      <c r="U30" s="116"/>
-      <c r="V30" s="134" t="s">
+      <c r="H30" s="113"/>
+      <c r="I30" s="113"/>
+      <c r="J30" s="113"/>
+      <c r="K30" s="132"/>
+      <c r="L30" s="132"/>
+      <c r="M30" s="113"/>
+      <c r="N30" s="113"/>
+      <c r="O30" s="113"/>
+      <c r="P30" s="113"/>
+      <c r="Q30" s="159"/>
+      <c r="R30" s="160"/>
+      <c r="S30" s="115"/>
+      <c r="T30" s="115"/>
+      <c r="U30" s="115"/>
+      <c r="V30" s="133" t="s">
         <v>20</v>
       </c>
       <c r="W30" s="22"/>
-      <c r="X30" s="142" t="s">
+      <c r="X30" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="Y30" s="143"/>
-      <c r="Z30" s="143"/>
-      <c r="AA30" s="144"/>
+      <c r="Y30" s="144"/>
+      <c r="Z30" s="144"/>
+      <c r="AA30" s="145"/>
       <c r="AB30" s="23" t="s">
         <v>55</v>
       </c>
@@ -5130,39 +5127,39 @@
       <c r="B31" s="18">
         <v>9</v>
       </c>
-      <c r="C31" s="195" t="s">
+      <c r="C31" s="140" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="196"/>
-      <c r="E31" s="197"/>
-      <c r="F31" s="71">
+      <c r="D31" s="141"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="70">
         <v>9</v>
       </c>
       <c r="G31" s="21"/>
-      <c r="H31" s="114"/>
-      <c r="I31" s="114"/>
-      <c r="J31" s="114"/>
-      <c r="K31" s="114"/>
-      <c r="L31" s="133"/>
-      <c r="M31" s="133"/>
-      <c r="N31" s="114"/>
-      <c r="O31" s="114"/>
-      <c r="P31" s="114"/>
-      <c r="Q31" s="206"/>
-      <c r="R31" s="207"/>
-      <c r="S31" s="116"/>
-      <c r="T31" s="116"/>
-      <c r="U31" s="116"/>
-      <c r="V31" s="134" t="s">
+      <c r="H31" s="113"/>
+      <c r="I31" s="113"/>
+      <c r="J31" s="113"/>
+      <c r="K31" s="113"/>
+      <c r="L31" s="132"/>
+      <c r="M31" s="132"/>
+      <c r="N31" s="113"/>
+      <c r="O31" s="113"/>
+      <c r="P31" s="113"/>
+      <c r="Q31" s="159"/>
+      <c r="R31" s="160"/>
+      <c r="S31" s="115"/>
+      <c r="T31" s="115"/>
+      <c r="U31" s="115"/>
+      <c r="V31" s="133" t="s">
         <v>20</v>
       </c>
       <c r="W31" s="22"/>
-      <c r="X31" s="142" t="s">
+      <c r="X31" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="Y31" s="143"/>
-      <c r="Z31" s="143"/>
-      <c r="AA31" s="144"/>
+      <c r="Y31" s="144"/>
+      <c r="Z31" s="144"/>
+      <c r="AA31" s="145"/>
       <c r="AB31" s="23" t="s">
         <v>59</v>
       </c>
@@ -5190,10 +5187,10 @@
     <row r="32" spans="1:49" ht="90.75" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
-      <c r="C32" s="195"/>
-      <c r="D32" s="196"/>
-      <c r="E32" s="197"/>
-      <c r="F32" s="72"/>
+      <c r="C32" s="140"/>
+      <c r="D32" s="141"/>
+      <c r="E32" s="142"/>
+      <c r="F32" s="71"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
@@ -5204,19 +5201,19 @@
       <c r="N32" s="21"/>
       <c r="O32" s="21"/>
       <c r="P32" s="21"/>
-      <c r="Q32" s="148"/>
-      <c r="R32" s="149"/>
+      <c r="Q32" s="161"/>
+      <c r="R32" s="162"/>
       <c r="S32" s="22"/>
       <c r="T32" s="22"/>
       <c r="U32" s="22"/>
       <c r="V32" s="22"/>
       <c r="W32" s="22"/>
-      <c r="X32" s="142" t="s">
+      <c r="X32" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="Y32" s="143"/>
-      <c r="Z32" s="143"/>
-      <c r="AA32" s="144"/>
+      <c r="Y32" s="144"/>
+      <c r="Z32" s="144"/>
+      <c r="AA32" s="145"/>
       <c r="AB32" s="23"/>
       <c r="AC32" s="17"/>
       <c r="AD32" s="17"/>
@@ -5242,9 +5239,9 @@
     <row r="33" spans="1:29" ht="14.25" customHeight="1">
       <c r="A33" s="26"/>
       <c r="B33" s="18"/>
-      <c r="C33" s="151"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="153"/>
+      <c r="C33" s="166"/>
+      <c r="D33" s="167"/>
+      <c r="E33" s="168"/>
       <c r="F33" s="19"/>
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
@@ -5256,25 +5253,25 @@
       <c r="N33" s="25"/>
       <c r="O33" s="21"/>
       <c r="P33" s="21"/>
-      <c r="Q33" s="148"/>
-      <c r="R33" s="149"/>
+      <c r="Q33" s="161"/>
+      <c r="R33" s="162"/>
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
       <c r="U33" s="22"/>
       <c r="V33" s="22"/>
       <c r="W33" s="22"/>
-      <c r="X33" s="142"/>
-      <c r="Y33" s="136"/>
-      <c r="Z33" s="136"/>
-      <c r="AA33" s="137"/>
+      <c r="X33" s="143"/>
+      <c r="Y33" s="164"/>
+      <c r="Z33" s="164"/>
+      <c r="AA33" s="165"/>
       <c r="AB33" s="23"/>
     </row>
     <row r="34" spans="1:29" ht="12.75" customHeight="1">
       <c r="A34" s="26"/>
       <c r="B34" s="18"/>
-      <c r="C34" s="151"/>
-      <c r="D34" s="152"/>
-      <c r="E34" s="153"/>
+      <c r="C34" s="166"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="168"/>
       <c r="F34" s="19"/>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
@@ -5286,25 +5283,25 @@
       <c r="N34" s="21"/>
       <c r="O34" s="25"/>
       <c r="P34" s="21"/>
-      <c r="Q34" s="148"/>
-      <c r="R34" s="149"/>
+      <c r="Q34" s="161"/>
+      <c r="R34" s="162"/>
       <c r="S34" s="22"/>
       <c r="T34" s="22"/>
       <c r="U34" s="22"/>
       <c r="V34" s="22"/>
       <c r="W34" s="22"/>
-      <c r="X34" s="142"/>
-      <c r="Y34" s="136"/>
-      <c r="Z34" s="136"/>
-      <c r="AA34" s="137"/>
+      <c r="X34" s="143"/>
+      <c r="Y34" s="164"/>
+      <c r="Z34" s="164"/>
+      <c r="AA34" s="165"/>
       <c r="AB34" s="23"/>
     </row>
     <row r="35" spans="1:29" ht="19.5" customHeight="1">
       <c r="A35" s="26"/>
       <c r="B35" s="18"/>
-      <c r="C35" s="154"/>
-      <c r="D35" s="152"/>
-      <c r="E35" s="153"/>
+      <c r="C35" s="211"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="168"/>
       <c r="F35" s="19"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
@@ -5316,25 +5313,25 @@
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
       <c r="P35" s="21"/>
-      <c r="Q35" s="148"/>
-      <c r="R35" s="149"/>
+      <c r="Q35" s="161"/>
+      <c r="R35" s="162"/>
       <c r="S35" s="22"/>
       <c r="T35" s="22"/>
       <c r="U35" s="22"/>
       <c r="V35" s="22"/>
       <c r="W35" s="22"/>
-      <c r="X35" s="135"/>
-      <c r="Y35" s="136"/>
-      <c r="Z35" s="136"/>
-      <c r="AA35" s="137"/>
+      <c r="X35" s="213"/>
+      <c r="Y35" s="164"/>
+      <c r="Z35" s="164"/>
+      <c r="AA35" s="165"/>
       <c r="AB35" s="23"/>
     </row>
     <row r="36" spans="1:29" ht="18.75" customHeight="1">
       <c r="A36" s="26"/>
       <c r="B36" s="18"/>
-      <c r="C36" s="155"/>
-      <c r="D36" s="136"/>
-      <c r="E36" s="137"/>
+      <c r="C36" s="212"/>
+      <c r="D36" s="164"/>
+      <c r="E36" s="165"/>
       <c r="F36" s="19"/>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
@@ -5346,17 +5343,17 @@
       <c r="N36" s="21"/>
       <c r="O36" s="21"/>
       <c r="P36" s="21"/>
-      <c r="Q36" s="148"/>
-      <c r="R36" s="149"/>
+      <c r="Q36" s="161"/>
+      <c r="R36" s="162"/>
       <c r="S36" s="22"/>
       <c r="T36" s="22"/>
       <c r="U36" s="22"/>
       <c r="V36" s="22"/>
       <c r="W36" s="22"/>
-      <c r="X36" s="135"/>
-      <c r="Y36" s="136"/>
-      <c r="Z36" s="136"/>
-      <c r="AA36" s="137"/>
+      <c r="X36" s="213"/>
+      <c r="Y36" s="164"/>
+      <c r="Z36" s="164"/>
+      <c r="AA36" s="165"/>
       <c r="AB36" s="23"/>
       <c r="AC36" s="41"/>
     </row>
@@ -5384,10 +5381,10 @@
       <c r="U37" s="29"/>
       <c r="V37" s="29"/>
       <c r="W37" s="29"/>
-      <c r="X37" s="147"/>
-      <c r="Y37" s="146"/>
-      <c r="Z37" s="146"/>
-      <c r="AA37" s="146"/>
+      <c r="X37" s="217"/>
+      <c r="Y37" s="177"/>
+      <c r="Z37" s="177"/>
+      <c r="AA37" s="177"/>
       <c r="AB37" s="30"/>
     </row>
     <row r="38" spans="1:29" ht="24.75" customHeight="1">
@@ -5414,10 +5411,10 @@
       <c r="U38" s="29"/>
       <c r="V38" s="29"/>
       <c r="W38" s="29"/>
-      <c r="X38" s="147"/>
-      <c r="Y38" s="146"/>
-      <c r="Z38" s="146"/>
-      <c r="AA38" s="146"/>
+      <c r="X38" s="217"/>
+      <c r="Y38" s="177"/>
+      <c r="Z38" s="177"/>
+      <c r="AA38" s="177"/>
       <c r="AB38" s="30"/>
     </row>
     <row r="39" spans="1:29" ht="24.75" customHeight="1">
@@ -5435,10 +5432,10 @@
       <c r="J39" s="17"/>
       <c r="O39" s="38"/>
       <c r="P39" s="38"/>
-      <c r="X39" s="145"/>
-      <c r="Y39" s="146"/>
-      <c r="Z39" s="146"/>
-      <c r="AA39" s="146"/>
+      <c r="X39" s="216"/>
+      <c r="Y39" s="177"/>
+      <c r="Z39" s="177"/>
+      <c r="AA39" s="177"/>
       <c r="AB39" s="26"/>
     </row>
     <row r="40" spans="1:29" ht="39.75" customHeight="1">
@@ -5546,36 +5543,36 @@
       <c r="AA43" s="44"/>
       <c r="AB43" s="45"/>
     </row>
-    <row r="44" spans="1:29" s="86" customFormat="1" ht="37.15" customHeight="1">
+    <row r="44" spans="1:29" s="85" customFormat="1" ht="37.15" customHeight="1">
       <c r="B44" s="27"/>
-      <c r="C44" s="138" t="s">
+      <c r="C44" s="214" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="138"/>
-      <c r="E44" s="138"/>
-      <c r="F44" s="138"/>
-      <c r="G44" s="138"/>
-      <c r="H44" s="138"/>
-      <c r="I44" s="138"/>
-      <c r="J44" s="138"/>
-      <c r="K44" s="138"/>
-      <c r="L44" s="138"/>
-      <c r="M44" s="138"/>
-      <c r="N44" s="138"/>
-      <c r="O44" s="138"/>
-      <c r="P44" s="138"/>
-      <c r="Q44" s="138"/>
-      <c r="R44" s="138"/>
-      <c r="S44" s="138"/>
-      <c r="T44" s="138"/>
-      <c r="U44" s="138"/>
-      <c r="V44" s="138"/>
-      <c r="W44" s="138"/>
-      <c r="X44" s="138"/>
-      <c r="Y44" s="138"/>
-      <c r="Z44" s="138"/>
-      <c r="AA44" s="138"/>
-      <c r="AB44" s="139"/>
+      <c r="D44" s="214"/>
+      <c r="E44" s="214"/>
+      <c r="F44" s="214"/>
+      <c r="G44" s="214"/>
+      <c r="H44" s="214"/>
+      <c r="I44" s="214"/>
+      <c r="J44" s="214"/>
+      <c r="K44" s="214"/>
+      <c r="L44" s="214"/>
+      <c r="M44" s="214"/>
+      <c r="N44" s="214"/>
+      <c r="O44" s="214"/>
+      <c r="P44" s="214"/>
+      <c r="Q44" s="214"/>
+      <c r="R44" s="214"/>
+      <c r="S44" s="214"/>
+      <c r="T44" s="214"/>
+      <c r="U44" s="214"/>
+      <c r="V44" s="214"/>
+      <c r="W44" s="214"/>
+      <c r="X44" s="214"/>
+      <c r="Y44" s="214"/>
+      <c r="Z44" s="214"/>
+      <c r="AA44" s="214"/>
+      <c r="AB44" s="215"/>
     </row>
     <row r="45" spans="1:29" ht="69.599999999999994" customHeight="1" thickBot="1">
       <c r="B45" s="48"/>
@@ -5652,14 +5649,14 @@
       <c r="C50" s="53"/>
     </row>
     <row r="51" spans="1:17" ht="12" customHeight="1">
-      <c r="B51" s="150" t="s">
+      <c r="B51" s="209" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="150"/>
-      <c r="D51" s="150"/>
-      <c r="E51" s="150"/>
-      <c r="F51" s="150"/>
-      <c r="G51" s="150"/>
+      <c r="C51" s="209"/>
+      <c r="D51" s="209"/>
+      <c r="E51" s="209"/>
+      <c r="F51" s="209"/>
+      <c r="G51" s="209"/>
       <c r="J51" s="17"/>
       <c r="K51" s="55" t="s">
         <v>32</v>
@@ -5680,17 +5677,17 @@
       </c>
       <c r="D54" s="59"/>
       <c r="E54" s="59"/>
-      <c r="F54" s="140"/>
-      <c r="G54" s="141"/>
-      <c r="H54" s="141"/>
+      <c r="F54" s="210"/>
+      <c r="G54" s="184"/>
+      <c r="H54" s="184"/>
       <c r="J54" s="60"/>
       <c r="K54" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="N54" s="140"/>
-      <c r="O54" s="141"/>
-      <c r="P54" s="141"/>
-      <c r="Q54" s="141"/>
+      <c r="N54" s="210"/>
+      <c r="O54" s="184"/>
+      <c r="P54" s="184"/>
+      <c r="Q54" s="184"/>
     </row>
     <row r="55" spans="1:17" ht="12" customHeight="1">
       <c r="A55" s="1"/>
@@ -35859,36 +35856,45 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="X25:AA25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="X29:AA29"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="X26:AA26"/>
-    <mergeCell ref="X27:AA27"/>
-    <mergeCell ref="X28:AA28"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="Y22:AB22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="X23:AA23"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="X36:AA36"/>
+    <mergeCell ref="C44:AB44"/>
+    <mergeCell ref="N54:Q54"/>
+    <mergeCell ref="X30:AA30"/>
+    <mergeCell ref="X31:AA31"/>
+    <mergeCell ref="X39:AA39"/>
+    <mergeCell ref="X32:AA32"/>
+    <mergeCell ref="X34:AA34"/>
+    <mergeCell ref="X35:AA35"/>
+    <mergeCell ref="X37:AA37"/>
+    <mergeCell ref="X38:AA38"/>
+    <mergeCell ref="X33:AA33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="G2:Q2"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="G3:Q3"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="B6:AB6"/>
+    <mergeCell ref="B7:AB7"/>
+    <mergeCell ref="B8:AB8"/>
+    <mergeCell ref="B10:AB10"/>
+    <mergeCell ref="B11:AB11"/>
+    <mergeCell ref="B12:AB12"/>
     <mergeCell ref="X24:AA24"/>
     <mergeCell ref="B13:AB13"/>
     <mergeCell ref="B15:AB15"/>
@@ -35905,45 +35911,36 @@
     <mergeCell ref="C19:E22"/>
     <mergeCell ref="F19:F22"/>
     <mergeCell ref="O19:W20"/>
-    <mergeCell ref="B7:AB7"/>
-    <mergeCell ref="B8:AB8"/>
-    <mergeCell ref="B10:AB10"/>
-    <mergeCell ref="B11:AB11"/>
-    <mergeCell ref="B12:AB12"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="B6:AB6"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="G3:Q3"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="X36:AA36"/>
-    <mergeCell ref="C44:AB44"/>
-    <mergeCell ref="N54:Q54"/>
-    <mergeCell ref="X30:AA30"/>
-    <mergeCell ref="X31:AA31"/>
-    <mergeCell ref="X39:AA39"/>
-    <mergeCell ref="X32:AA32"/>
-    <mergeCell ref="X34:AA34"/>
-    <mergeCell ref="X35:AA35"/>
-    <mergeCell ref="X37:AA37"/>
-    <mergeCell ref="X38:AA38"/>
-    <mergeCell ref="X33:AA33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Y22:AB22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="X23:AA23"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="X25:AA25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="X26:AA26"/>
+    <mergeCell ref="X27:AA27"/>
+    <mergeCell ref="X28:AA28"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
   </mergeCells>
   <conditionalFormatting sqref="F53:G54">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
@@ -35972,8 +35969,8 @@
   </sheetPr>
   <dimension ref="A2:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -35991,52 +35988,52 @@
       <c r="A2" s="218" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
+      <c r="B2" s="181"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="181"/>
       <c r="H2" s="219"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="220"/>
-      <c r="B3" s="146"/>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
       <c r="H3" s="221"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="220"/>
-      <c r="B4" s="146"/>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
       <c r="H4" s="221"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="220"/>
-      <c r="B5" s="146"/>
-      <c r="C5" s="146"/>
-      <c r="D5" s="146"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="146"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="177"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
       <c r="H5" s="221"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="220"/>
-      <c r="B6" s="146"/>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="146"/>
+      <c r="B6" s="177"/>
+      <c r="C6" s="177"/>
+      <c r="D6" s="177"/>
+      <c r="E6" s="177"/>
+      <c r="F6" s="177"/>
+      <c r="G6" s="177"/>
       <c r="H6" s="221"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
@@ -36079,9 +36076,6 @@
       <c r="E10" s="63">
         <v>1</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="225"/>
-      <c r="H10" s="226"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="61"/>
@@ -36093,9 +36087,6 @@
       <c r="E11" s="64">
         <v>45644</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="146"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="61" t="s">
@@ -36105,1574 +36096,1566 @@
       <c r="C12" s="61"/>
       <c r="D12" s="65"/>
       <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="66"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="87"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="89"/>
+      <c r="A13" s="86"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="86"/>
+      <c r="I13" s="88"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="99" t="s">
+      <c r="A14" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="91" t="s">
+      <c r="D14" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="85" t="s">
+      <c r="E14" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="85" t="s">
+      <c r="F14" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="92" t="s">
+      <c r="G14" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="85" t="s">
+      <c r="H14" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="85" t="s">
+      <c r="I14" s="84" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="157.5" customHeight="1">
-      <c r="A15" s="227" t="s">
+      <c r="A15" s="225" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="93">
-        <v>45664</v>
-      </c>
-      <c r="C15" s="94" t="s">
+      <c r="B15" s="92">
+        <v>45665</v>
+      </c>
+      <c r="C15" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="68" t="s">
+      <c r="E15" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="84" t="s">
+      <c r="F15" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="82" t="s">
+      <c r="G15" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="69" t="s">
+      <c r="H15" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="I15" s="96" t="s">
+      <c r="I15" s="95" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="141.75" customHeight="1">
-      <c r="A16" s="228"/>
-      <c r="B16" s="93">
+      <c r="A16" s="226"/>
+      <c r="B16" s="92">
         <v>45665</v>
       </c>
-      <c r="C16" s="94" t="s">
+      <c r="C16" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="95" t="s">
+      <c r="D16" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="68" t="s">
+      <c r="E16" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="84" t="s">
+      <c r="F16" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="82" t="s">
+      <c r="G16" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="70" t="s">
+      <c r="H16" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="95" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="165" customHeight="1">
-      <c r="A17" s="228"/>
-      <c r="B17" s="93">
+      <c r="A17" s="226"/>
+      <c r="B17" s="92">
         <v>45667</v>
       </c>
-      <c r="C17" s="94" t="s">
+      <c r="C17" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="95" t="s">
+      <c r="D17" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="68" t="s">
+      <c r="E17" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="84" t="s">
+      <c r="F17" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="82" t="s">
+      <c r="G17" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="83" t="s">
+      <c r="H17" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="I17" s="96" t="s">
+      <c r="I17" s="95" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="134.25" customHeight="1">
-      <c r="A18" s="228"/>
-      <c r="B18" s="93">
+      <c r="A18" s="226"/>
+      <c r="B18" s="92">
         <v>45667</v>
       </c>
-      <c r="C18" s="94" t="s">
+      <c r="C18" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="97" t="s">
+      <c r="E18" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="F18" s="84" t="s">
+      <c r="F18" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="82" t="s">
+      <c r="G18" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="100" t="s">
+      <c r="H18" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="I18" s="96" t="s">
+      <c r="I18" s="95" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="162" customHeight="1">
-      <c r="A19" s="228"/>
-      <c r="B19" s="103" t="s">
+      <c r="A19" s="226"/>
+      <c r="B19" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="102"/>
-      <c r="D19" s="98" t="s">
+      <c r="C19" s="101"/>
+      <c r="D19" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="97" t="s">
+      <c r="E19" s="96" t="s">
         <v>255</v>
       </c>
-      <c r="F19" s="103" t="s">
+      <c r="F19" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="82" t="s">
+      <c r="G19" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H19" s="101" t="s">
+      <c r="H19" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="I19" s="96" t="s">
+      <c r="I19" s="95" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="165" customHeight="1">
-      <c r="A20" s="228"/>
-      <c r="B20" s="103" t="s">
+      <c r="A20" s="226"/>
+      <c r="B20" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="102"/>
-      <c r="D20" s="98" t="s">
+      <c r="C20" s="101"/>
+      <c r="D20" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="97" t="s">
+      <c r="E20" s="96" t="s">
         <v>202</v>
       </c>
-      <c r="F20" s="103" t="s">
+      <c r="F20" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="82" t="s">
+      <c r="G20" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="103" t="s">
+      <c r="H20" s="102" t="s">
         <v>90</v>
       </c>
-      <c r="I20" s="96" t="s">
+      <c r="I20" s="95" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="112.9" customHeight="1">
-      <c r="A21" s="228"/>
-      <c r="B21" s="103" t="s">
+      <c r="A21" s="226"/>
+      <c r="B21" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="102"/>
-      <c r="D21" s="98" t="s">
+      <c r="C21" s="101"/>
+      <c r="D21" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="97" t="s">
+      <c r="E21" s="96" t="s">
         <v>203</v>
       </c>
-      <c r="F21" s="103" t="s">
+      <c r="F21" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="82" t="s">
+      <c r="G21" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H21" s="103" t="s">
+      <c r="H21" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="I21" s="96" t="s">
+      <c r="I21" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="109.5" customHeight="1">
-      <c r="A22" s="228"/>
-      <c r="B22" s="103" t="s">
+      <c r="A22" s="226"/>
+      <c r="B22" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="98" t="s">
+      <c r="C22" s="101"/>
+      <c r="D22" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="97" t="s">
+      <c r="E22" s="96" t="s">
         <v>204</v>
       </c>
-      <c r="F22" s="103" t="s">
+      <c r="F22" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="82" t="s">
+      <c r="G22" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="101" t="s">
+      <c r="H22" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="96" t="s">
+      <c r="I22" s="95" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="103.5" customHeight="1">
-      <c r="A23" s="228"/>
-      <c r="B23" s="103" t="s">
+      <c r="A23" s="226"/>
+      <c r="B23" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="103" t="s">
+      <c r="C23" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="104" t="s">
+      <c r="E23" s="103" t="s">
         <v>206</v>
       </c>
-      <c r="F23" s="103" t="s">
+      <c r="F23" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G23" s="82" t="s">
+      <c r="G23" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="103" t="s">
+      <c r="H23" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="I23" s="105" t="s">
+      <c r="I23" s="104" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="240" customHeight="1">
-      <c r="A24" s="228"/>
-      <c r="B24" s="103" t="s">
+      <c r="A24" s="226"/>
+      <c r="B24" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="103" t="s">
+      <c r="C24" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="98" t="s">
+      <c r="D24" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="104" t="s">
+      <c r="E24" s="103" t="s">
         <v>207</v>
       </c>
-      <c r="F24" s="103" t="s">
+      <c r="F24" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G24" s="82" t="s">
+      <c r="G24" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="103" t="s">
+      <c r="H24" s="102" t="s">
         <v>94</v>
       </c>
-      <c r="I24" s="105" t="s">
+      <c r="I24" s="104" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="152.25" customHeight="1">
-      <c r="A25" s="228"/>
-      <c r="B25" s="103" t="s">
+      <c r="A25" s="226"/>
+      <c r="B25" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="103" t="s">
+      <c r="C25" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="98" t="s">
+      <c r="D25" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="104" t="s">
+      <c r="E25" s="103" t="s">
         <v>208</v>
       </c>
-      <c r="F25" s="103" t="s">
+      <c r="F25" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="82" t="s">
+      <c r="G25" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H25" s="103" t="s">
+      <c r="H25" s="102" t="s">
         <v>95</v>
       </c>
-      <c r="I25" s="105" t="s">
+      <c r="I25" s="104" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="162.75" customHeight="1">
-      <c r="A26" s="228"/>
-      <c r="B26" s="103" t="s">
+      <c r="A26" s="226"/>
+      <c r="B26" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="103" t="s">
+      <c r="C26" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="98" t="s">
+      <c r="D26" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="104" t="s">
+      <c r="E26" s="103" t="s">
         <v>209</v>
       </c>
-      <c r="F26" s="103" t="s">
+      <c r="F26" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G26" s="82" t="s">
+      <c r="G26" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="103" t="s">
+      <c r="H26" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="I26" s="105" t="s">
+      <c r="I26" s="104" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="168" customHeight="1">
-      <c r="A27" s="228"/>
-      <c r="B27" s="103" t="s">
+      <c r="A27" s="226"/>
+      <c r="B27" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="98" t="s">
+      <c r="D27" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="104" t="s">
+      <c r="E27" s="103" t="s">
         <v>210</v>
       </c>
-      <c r="F27" s="103" t="s">
+      <c r="F27" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="82" t="s">
+      <c r="G27" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H27" s="103" t="s">
+      <c r="H27" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="I27" s="105" t="s">
+      <c r="I27" s="104" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="187.5" customHeight="1">
-      <c r="A28" s="228"/>
-      <c r="B28" s="103" t="s">
+      <c r="A28" s="226"/>
+      <c r="B28" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="103" t="s">
+      <c r="C28" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="98" t="s">
+      <c r="D28" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="104" t="s">
+      <c r="E28" s="103" t="s">
         <v>211</v>
       </c>
-      <c r="F28" s="103" t="s">
+      <c r="F28" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="82" t="s">
+      <c r="G28" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="103" t="s">
+      <c r="H28" s="102" t="s">
         <v>98</v>
       </c>
-      <c r="I28" s="105" t="s">
+      <c r="I28" s="104" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="145.5" customHeight="1">
-      <c r="A29" s="228"/>
-      <c r="B29" s="103" t="s">
+      <c r="A29" s="226"/>
+      <c r="B29" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="103" t="s">
+      <c r="C29" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="98" t="s">
+      <c r="D29" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="104" t="s">
+      <c r="E29" s="103" t="s">
         <v>212</v>
       </c>
-      <c r="F29" s="103" t="s">
+      <c r="F29" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G29" s="82" t="s">
+      <c r="G29" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H29" s="103" t="s">
+      <c r="H29" s="102" t="s">
         <v>99</v>
       </c>
-      <c r="I29" s="105" t="s">
+      <c r="I29" s="104" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="82.9" customHeight="1">
-      <c r="A30" s="228"/>
-      <c r="B30" s="103" t="s">
+      <c r="A30" s="226"/>
+      <c r="B30" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="103" t="s">
+      <c r="C30" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="98" t="s">
+      <c r="D30" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="104" t="s">
+      <c r="E30" s="103" t="s">
         <v>213</v>
       </c>
-      <c r="F30" s="103" t="s">
+      <c r="F30" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="82" t="s">
+      <c r="G30" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H30" s="103" t="s">
+      <c r="H30" s="102" t="s">
         <v>100</v>
       </c>
-      <c r="I30" s="105" t="s">
+      <c r="I30" s="104" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="104.45" customHeight="1">
-      <c r="A31" s="228"/>
-      <c r="B31" s="103" t="s">
+      <c r="A31" s="226"/>
+      <c r="B31" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="103" t="s">
+      <c r="C31" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="98" t="s">
+      <c r="D31" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="104" t="s">
+      <c r="E31" s="103" t="s">
         <v>214</v>
       </c>
-      <c r="F31" s="103" t="s">
+      <c r="F31" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G31" s="82" t="s">
+      <c r="G31" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="103" t="s">
+      <c r="H31" s="102" t="s">
         <v>101</v>
       </c>
-      <c r="I31" s="105" t="s">
+      <c r="I31" s="104" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="96" customHeight="1">
-      <c r="A32" s="228"/>
-      <c r="B32" s="103" t="s">
+      <c r="A32" s="226"/>
+      <c r="B32" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="103" t="s">
+      <c r="C32" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="98" t="s">
+      <c r="D32" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="104" t="s">
+      <c r="E32" s="103" t="s">
         <v>215</v>
       </c>
-      <c r="F32" s="103" t="s">
+      <c r="F32" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G32" s="82" t="s">
+      <c r="G32" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="103" t="s">
+      <c r="H32" s="102" t="s">
         <v>102</v>
       </c>
-      <c r="I32" s="105" t="s">
+      <c r="I32" s="104" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="80.45" customHeight="1">
-      <c r="A33" s="228"/>
-      <c r="B33" s="103" t="s">
+      <c r="A33" s="226"/>
+      <c r="B33" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="103" t="s">
+      <c r="C33" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="98" t="s">
+      <c r="D33" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="104" t="s">
+      <c r="E33" s="103" t="s">
         <v>216</v>
       </c>
-      <c r="F33" s="103" t="s">
+      <c r="F33" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G33" s="82" t="s">
+      <c r="G33" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H33" s="103" t="s">
+      <c r="H33" s="102" t="s">
         <v>103</v>
       </c>
-      <c r="I33" s="105" t="s">
+      <c r="I33" s="104" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="81" customHeight="1">
-      <c r="A34" s="228"/>
-      <c r="B34" s="103" t="s">
+      <c r="A34" s="226"/>
+      <c r="B34" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="103" t="s">
+      <c r="C34" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="104" t="s">
+      <c r="E34" s="103" t="s">
         <v>217</v>
       </c>
-      <c r="F34" s="103" t="s">
+      <c r="F34" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G34" s="82" t="s">
+      <c r="G34" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H34" s="103" t="s">
+      <c r="H34" s="102" t="s">
         <v>104</v>
       </c>
-      <c r="I34" s="105" t="s">
+      <c r="I34" s="104" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="93" customHeight="1">
-      <c r="A35" s="228"/>
-      <c r="B35" s="103" t="s">
+      <c r="A35" s="226"/>
+      <c r="B35" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="103" t="s">
+      <c r="C35" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="98" t="s">
+      <c r="D35" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="104" t="s">
+      <c r="E35" s="103" t="s">
         <v>218</v>
       </c>
-      <c r="F35" s="103" t="s">
+      <c r="F35" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G35" s="82" t="s">
+      <c r="G35" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H35" s="103" t="s">
+      <c r="H35" s="102" t="s">
         <v>105</v>
       </c>
-      <c r="I35" s="105" t="s">
+      <c r="I35" s="104" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="115.9" customHeight="1">
-      <c r="A36" s="228"/>
-      <c r="B36" s="103" t="s">
+      <c r="A36" s="226"/>
+      <c r="B36" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="103" t="s">
+      <c r="C36" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="98" t="s">
+      <c r="D36" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="104" t="s">
+      <c r="E36" s="103" t="s">
         <v>219</v>
       </c>
-      <c r="F36" s="103" t="s">
+      <c r="F36" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G36" s="82" t="s">
+      <c r="G36" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H36" s="103" t="s">
+      <c r="H36" s="102" t="s">
         <v>106</v>
       </c>
-      <c r="I36" s="105" t="s">
+      <c r="I36" s="104" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="122.45" customHeight="1">
-      <c r="A37" s="228"/>
-      <c r="B37" s="103" t="s">
+      <c r="A37" s="226"/>
+      <c r="B37" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="103" t="s">
+      <c r="C37" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="98" t="s">
+      <c r="D37" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="104" t="s">
+      <c r="E37" s="103" t="s">
         <v>220</v>
       </c>
-      <c r="F37" s="103" t="s">
+      <c r="F37" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G37" s="82" t="s">
+      <c r="G37" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H37" s="103" t="s">
+      <c r="H37" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="I37" s="105" t="s">
+      <c r="I37" s="104" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="105.6" customHeight="1">
-      <c r="A38" s="228"/>
-      <c r="B38" s="103" t="s">
+      <c r="A38" s="226"/>
+      <c r="B38" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="103" t="s">
+      <c r="C38" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="98" t="s">
+      <c r="D38" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="104" t="s">
+      <c r="E38" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="F38" s="103" t="s">
+      <c r="F38" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G38" s="82" t="s">
+      <c r="G38" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H38" s="103" t="s">
+      <c r="H38" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="I38" s="105" t="s">
+      <c r="I38" s="104" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="107.45" customHeight="1">
-      <c r="A39" s="228"/>
-      <c r="B39" s="103" t="s">
+      <c r="A39" s="226"/>
+      <c r="B39" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="103" t="s">
+      <c r="C39" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="98" t="s">
+      <c r="D39" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="104" t="s">
+      <c r="E39" s="103" t="s">
         <v>221</v>
       </c>
-      <c r="F39" s="103" t="s">
+      <c r="F39" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G39" s="82" t="s">
+      <c r="G39" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H39" s="103" t="s">
+      <c r="H39" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="I39" s="105" t="s">
+      <c r="I39" s="104" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="85.9" customHeight="1">
-      <c r="A40" s="228"/>
-      <c r="B40" s="103" t="s">
+      <c r="A40" s="226"/>
+      <c r="B40" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="103" t="s">
+      <c r="C40" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="104" t="s">
+      <c r="E40" s="103" t="s">
         <v>222</v>
       </c>
-      <c r="F40" s="103" t="s">
+      <c r="F40" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G40" s="82" t="s">
+      <c r="G40" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H40" s="103" t="s">
+      <c r="H40" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="I40" s="105" t="s">
+      <c r="I40" s="104" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="93" customHeight="1">
-      <c r="A41" s="228"/>
-      <c r="B41" s="103" t="s">
+      <c r="A41" s="226"/>
+      <c r="B41" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="103" t="s">
+      <c r="C41" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="98" t="s">
+      <c r="D41" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="104" t="s">
+      <c r="E41" s="103" t="s">
         <v>223</v>
       </c>
-      <c r="F41" s="103" t="s">
+      <c r="F41" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G41" s="82" t="s">
+      <c r="G41" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H41" s="103" t="s">
+      <c r="H41" s="102" t="s">
         <v>111</v>
       </c>
-      <c r="I41" s="105" t="s">
+      <c r="I41" s="104" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="82.9" customHeight="1">
-      <c r="A42" s="228"/>
-      <c r="B42" s="103" t="s">
+      <c r="A42" s="226"/>
+      <c r="B42" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="103" t="s">
+      <c r="C42" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D42" s="98" t="s">
+      <c r="D42" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="104" t="s">
+      <c r="E42" s="103" t="s">
         <v>224</v>
       </c>
-      <c r="F42" s="103" t="s">
+      <c r="F42" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G42" s="82" t="s">
+      <c r="G42" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H42" s="103" t="s">
+      <c r="H42" s="102" t="s">
         <v>112</v>
       </c>
-      <c r="I42" s="105" t="s">
+      <c r="I42" s="104" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="100.9" customHeight="1">
-      <c r="A43" s="228"/>
-      <c r="B43" s="103" t="s">
+      <c r="A43" s="226"/>
+      <c r="B43" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="103" t="s">
+      <c r="C43" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="98" t="s">
+      <c r="D43" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="104" t="s">
+      <c r="E43" s="103" t="s">
         <v>225</v>
       </c>
-      <c r="F43" s="103" t="s">
+      <c r="F43" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G43" s="82" t="s">
+      <c r="G43" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H43" s="103" t="s">
+      <c r="H43" s="102" t="s">
         <v>113</v>
       </c>
-      <c r="I43" s="105" t="s">
+      <c r="I43" s="104" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="74.45" customHeight="1">
-      <c r="A44" s="228"/>
-      <c r="B44" s="103" t="s">
+      <c r="A44" s="226"/>
+      <c r="B44" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="103" t="s">
+      <c r="C44" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D44" s="98" t="s">
+      <c r="D44" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="104" t="s">
+      <c r="E44" s="103" t="s">
         <v>226</v>
       </c>
-      <c r="F44" s="103" t="s">
+      <c r="F44" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G44" s="82" t="s">
+      <c r="G44" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H44" s="103" t="s">
+      <c r="H44" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="I44" s="105" t="s">
+      <c r="I44" s="104" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="89.45" customHeight="1">
-      <c r="A45" s="228"/>
-      <c r="B45" s="103" t="s">
+      <c r="A45" s="226"/>
+      <c r="B45" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="103" t="s">
+      <c r="C45" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="98" t="s">
+      <c r="D45" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E45" s="104" t="s">
+      <c r="E45" s="103" t="s">
         <v>227</v>
       </c>
-      <c r="F45" s="103" t="s">
+      <c r="F45" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G45" s="82" t="s">
+      <c r="G45" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H45" s="103" t="s">
+      <c r="H45" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="I45" s="105" t="s">
+      <c r="I45" s="104" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="111" customHeight="1">
-      <c r="A46" s="228"/>
-      <c r="B46" s="103" t="s">
+      <c r="A46" s="226"/>
+      <c r="B46" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C46" s="103" t="s">
+      <c r="C46" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D46" s="98" t="s">
+      <c r="D46" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="104" t="s">
+      <c r="E46" s="103" t="s">
         <v>228</v>
       </c>
-      <c r="F46" s="103" t="s">
+      <c r="F46" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G46" s="82" t="s">
+      <c r="G46" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H46" s="103" t="s">
+      <c r="H46" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="I46" s="105" t="s">
+      <c r="I46" s="104" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="82.9" customHeight="1">
-      <c r="A47" s="228"/>
-      <c r="B47" s="103" t="s">
+      <c r="A47" s="226"/>
+      <c r="B47" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="103" t="s">
+      <c r="C47" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D47" s="98" t="s">
+      <c r="D47" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E47" s="104" t="s">
+      <c r="E47" s="103" t="s">
         <v>229</v>
       </c>
-      <c r="F47" s="103" t="s">
+      <c r="F47" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G47" s="82" t="s">
+      <c r="G47" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H47" s="103" t="s">
+      <c r="H47" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="I47" s="105" t="s">
+      <c r="I47" s="104" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="82.15" customHeight="1">
-      <c r="A48" s="228"/>
-      <c r="B48" s="103" t="s">
+      <c r="A48" s="226"/>
+      <c r="B48" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="103" t="s">
+      <c r="C48" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D48" s="98" t="s">
+      <c r="D48" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="104" t="s">
+      <c r="E48" s="103" t="s">
         <v>230</v>
       </c>
-      <c r="F48" s="103" t="s">
+      <c r="F48" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G48" s="82" t="s">
+      <c r="G48" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H48" s="103" t="s">
+      <c r="H48" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="I48" s="105" t="s">
+      <c r="I48" s="104" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="97.15" customHeight="1">
-      <c r="A49" s="228"/>
-      <c r="B49" s="103" t="s">
+      <c r="A49" s="226"/>
+      <c r="B49" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="103" t="s">
+      <c r="C49" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D49" s="98" t="s">
+      <c r="D49" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="104" t="s">
+      <c r="E49" s="103" t="s">
         <v>231</v>
       </c>
-      <c r="F49" s="103" t="s">
+      <c r="F49" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G49" s="82" t="s">
+      <c r="G49" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H49" s="103" t="s">
+      <c r="H49" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="I49" s="105" t="s">
+      <c r="I49" s="104" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="77.45" customHeight="1">
-      <c r="A50" s="228"/>
-      <c r="B50" s="103" t="s">
+      <c r="A50" s="226"/>
+      <c r="B50" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="103" t="s">
+      <c r="C50" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D50" s="98" t="s">
+      <c r="D50" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E50" s="104" t="s">
+      <c r="E50" s="103" t="s">
         <v>248</v>
       </c>
-      <c r="F50" s="103" t="s">
+      <c r="F50" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G50" s="82" t="s">
+      <c r="G50" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H50" s="103" t="s">
+      <c r="H50" s="102" t="s">
         <v>120</v>
       </c>
-      <c r="I50" s="105" t="s">
+      <c r="I50" s="104" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="100.9" customHeight="1">
-      <c r="A51" s="228"/>
-      <c r="B51" s="103" t="s">
+      <c r="A51" s="226"/>
+      <c r="B51" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="103" t="s">
+      <c r="C51" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D51" s="98" t="s">
+      <c r="D51" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E51" s="104" t="s">
+      <c r="E51" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="F51" s="103" t="s">
+      <c r="F51" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G51" s="82" t="s">
+      <c r="G51" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H51" s="103" t="s">
+      <c r="H51" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="I51" s="105" t="s">
+      <c r="I51" s="104" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="92.45" customHeight="1">
-      <c r="A52" s="228"/>
-      <c r="B52" s="103" t="s">
+      <c r="A52" s="226"/>
+      <c r="B52" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C52" s="103" t="s">
+      <c r="C52" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D52" s="98" t="s">
+      <c r="D52" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E52" s="229" t="s">
+      <c r="E52" s="134" t="s">
         <v>250</v>
       </c>
-      <c r="F52" s="103" t="s">
+      <c r="F52" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G52" s="82" t="s">
+      <c r="G52" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H52" s="103" t="s">
+      <c r="H52" s="102" t="s">
         <v>122</v>
       </c>
-      <c r="I52" s="105" t="s">
+      <c r="I52" s="104" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="95.45" customHeight="1">
-      <c r="A53" s="228"/>
-      <c r="B53" s="103" t="s">
+      <c r="A53" s="226"/>
+      <c r="B53" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C53" s="103" t="s">
+      <c r="C53" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D53" s="98" t="s">
+      <c r="D53" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E53" s="104" t="s">
+      <c r="E53" s="103" t="s">
         <v>251</v>
       </c>
-      <c r="F53" s="103" t="s">
+      <c r="F53" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G53" s="82" t="s">
+      <c r="G53" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H53" s="103" t="s">
+      <c r="H53" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="I53" s="105" t="s">
+      <c r="I53" s="104" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="82.15" customHeight="1">
-      <c r="A54" s="228"/>
-      <c r="B54" s="103" t="s">
+      <c r="A54" s="226"/>
+      <c r="B54" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="103" t="s">
+      <c r="C54" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D54" s="98" t="s">
+      <c r="D54" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E54" s="104" t="s">
+      <c r="E54" s="103" t="s">
         <v>232</v>
       </c>
-      <c r="F54" s="103" t="s">
+      <c r="F54" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G54" s="82" t="s">
+      <c r="G54" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H54" s="103" t="s">
+      <c r="H54" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="I54" s="105" t="s">
+      <c r="I54" s="104" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="85.9" customHeight="1">
-      <c r="A55" s="228"/>
-      <c r="B55" s="103" t="s">
+      <c r="A55" s="226"/>
+      <c r="B55" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="103" t="s">
+      <c r="C55" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="98" t="s">
+      <c r="D55" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E55" s="104" t="s">
+      <c r="E55" s="103" t="s">
         <v>233</v>
       </c>
-      <c r="F55" s="103" t="s">
+      <c r="F55" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G55" s="82" t="s">
+      <c r="G55" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H55" s="103" t="s">
+      <c r="H55" s="102" t="s">
         <v>125</v>
       </c>
-      <c r="I55" s="105" t="s">
+      <c r="I55" s="104" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="83.45" customHeight="1">
-      <c r="A56" s="228"/>
-      <c r="B56" s="103" t="s">
+      <c r="A56" s="226"/>
+      <c r="B56" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="103" t="s">
+      <c r="C56" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D56" s="98" t="s">
+      <c r="D56" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E56" s="104" t="s">
+      <c r="E56" s="103" t="s">
         <v>234</v>
       </c>
-      <c r="F56" s="103" t="s">
+      <c r="F56" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G56" s="82" t="s">
+      <c r="G56" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H56" s="103" t="s">
+      <c r="H56" s="102" t="s">
         <v>126</v>
       </c>
-      <c r="I56" s="105" t="s">
+      <c r="I56" s="104" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="108" customHeight="1">
-      <c r="A57" s="228"/>
-      <c r="B57" s="103" t="s">
+      <c r="A57" s="226"/>
+      <c r="B57" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C57" s="103" t="s">
+      <c r="C57" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D57" s="98" t="s">
+      <c r="D57" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E57" s="104" t="s">
+      <c r="E57" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="F57" s="103" t="s">
+      <c r="F57" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G57" s="82" t="s">
+      <c r="G57" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H57" s="103" t="s">
+      <c r="H57" s="102" t="s">
         <v>127</v>
       </c>
-      <c r="I57" s="105" t="s">
+      <c r="I57" s="104" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="74.45" customHeight="1">
-      <c r="A58" s="228"/>
-      <c r="B58" s="103" t="s">
+      <c r="A58" s="226"/>
+      <c r="B58" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C58" s="103" t="s">
+      <c r="C58" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D58" s="98" t="s">
+      <c r="D58" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E58" s="104" t="s">
+      <c r="E58" s="103" t="s">
         <v>236</v>
       </c>
-      <c r="F58" s="103" t="s">
+      <c r="F58" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G58" s="82" t="s">
+      <c r="G58" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H58" s="103" t="s">
+      <c r="H58" s="102" t="s">
         <v>128</v>
       </c>
-      <c r="I58" s="105" t="s">
+      <c r="I58" s="104" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="84.6" customHeight="1">
-      <c r="A59" s="228"/>
-      <c r="B59" s="103" t="s">
+      <c r="A59" s="226"/>
+      <c r="B59" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C59" s="103" t="s">
+      <c r="C59" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="98" t="s">
+      <c r="D59" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E59" s="104" t="s">
+      <c r="E59" s="103" t="s">
         <v>237</v>
       </c>
-      <c r="F59" s="103" t="s">
+      <c r="F59" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G59" s="82" t="s">
+      <c r="G59" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H59" s="103" t="s">
+      <c r="H59" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="I59" s="105" t="s">
+      <c r="I59" s="104" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="103.9" customHeight="1">
-      <c r="A60" s="228"/>
-      <c r="B60" s="103" t="s">
+      <c r="A60" s="226"/>
+      <c r="B60" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C60" s="103" t="s">
+      <c r="C60" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D60" s="98" t="s">
+      <c r="D60" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E60" s="104" t="s">
+      <c r="E60" s="103" t="s">
         <v>238</v>
       </c>
-      <c r="F60" s="103" t="s">
+      <c r="F60" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G60" s="82" t="s">
+      <c r="G60" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H60" s="103" t="s">
+      <c r="H60" s="102" t="s">
         <v>130</v>
       </c>
-      <c r="I60" s="105" t="s">
+      <c r="I60" s="104" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="93.6" customHeight="1">
-      <c r="A61" s="228"/>
-      <c r="B61" s="103" t="s">
+      <c r="A61" s="226"/>
+      <c r="B61" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C61" s="103" t="s">
+      <c r="C61" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D61" s="98" t="s">
+      <c r="D61" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E61" s="104" t="s">
+      <c r="E61" s="103" t="s">
         <v>252</v>
       </c>
-      <c r="F61" s="103" t="s">
+      <c r="F61" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G61" s="82" t="s">
+      <c r="G61" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H61" s="103" t="s">
+      <c r="H61" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="I61" s="105" t="s">
+      <c r="I61" s="104" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="92.45" customHeight="1">
-      <c r="A62" s="228"/>
-      <c r="B62" s="103" t="s">
+      <c r="A62" s="226"/>
+      <c r="B62" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C62" s="103" t="s">
+      <c r="C62" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D62" s="98" t="s">
+      <c r="D62" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E62" s="104" t="s">
+      <c r="E62" s="103" t="s">
         <v>239</v>
       </c>
-      <c r="F62" s="103" t="s">
+      <c r="F62" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G62" s="82" t="s">
+      <c r="G62" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H62" s="103" t="s">
+      <c r="H62" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="I62" s="105" t="s">
+      <c r="I62" s="104" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="85.15" customHeight="1">
-      <c r="A63" s="228"/>
-      <c r="B63" s="103" t="s">
+      <c r="A63" s="226"/>
+      <c r="B63" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="103" t="s">
+      <c r="C63" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D63" s="98" t="s">
+      <c r="D63" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E63" s="104" t="s">
+      <c r="E63" s="103" t="s">
         <v>240</v>
       </c>
-      <c r="F63" s="103" t="s">
+      <c r="F63" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G63" s="82" t="s">
+      <c r="G63" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H63" s="103" t="s">
+      <c r="H63" s="102" t="s">
         <v>133</v>
       </c>
-      <c r="I63" s="105" t="s">
+      <c r="I63" s="104" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="81" customHeight="1">
-      <c r="A64" s="228"/>
-      <c r="B64" s="103" t="s">
+      <c r="A64" s="226"/>
+      <c r="B64" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C64" s="103" t="s">
+      <c r="C64" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D64" s="98" t="s">
+      <c r="D64" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E64" s="104" t="s">
+      <c r="E64" s="103" t="s">
         <v>241</v>
       </c>
-      <c r="F64" s="103" t="s">
+      <c r="F64" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G64" s="82" t="s">
+      <c r="G64" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H64" s="103" t="s">
+      <c r="H64" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="I64" s="105" t="s">
+      <c r="I64" s="104" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="90.6" customHeight="1">
-      <c r="A65" s="228"/>
-      <c r="B65" s="103" t="s">
+      <c r="A65" s="226"/>
+      <c r="B65" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="103" t="s">
+      <c r="C65" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D65" s="98" t="s">
+      <c r="D65" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E65" s="104" t="s">
+      <c r="E65" s="103" t="s">
         <v>242</v>
       </c>
-      <c r="F65" s="103" t="s">
+      <c r="F65" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G65" s="82" t="s">
+      <c r="G65" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H65" s="103" t="s">
+      <c r="H65" s="102" t="s">
         <v>135</v>
       </c>
-      <c r="I65" s="105" t="s">
+      <c r="I65" s="104" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="88.9" customHeight="1">
-      <c r="A66" s="228"/>
-      <c r="B66" s="103" t="s">
+      <c r="A66" s="226"/>
+      <c r="B66" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C66" s="103" t="s">
+      <c r="C66" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="98" t="s">
+      <c r="D66" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E66" s="104" t="s">
+      <c r="E66" s="103" t="s">
         <v>243</v>
       </c>
-      <c r="F66" s="103" t="s">
+      <c r="F66" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G66" s="82" t="s">
+      <c r="G66" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H66" s="103" t="s">
+      <c r="H66" s="102" t="s">
         <v>136</v>
       </c>
-      <c r="I66" s="105" t="s">
+      <c r="I66" s="104" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="86.45" customHeight="1">
-      <c r="A67" s="228"/>
-      <c r="B67" s="103" t="s">
+      <c r="A67" s="226"/>
+      <c r="B67" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C67" s="103" t="s">
+      <c r="C67" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="98" t="s">
+      <c r="D67" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E67" s="104" t="s">
+      <c r="E67" s="103" t="s">
         <v>244</v>
       </c>
-      <c r="F67" s="103" t="s">
+      <c r="F67" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G67" s="82" t="s">
+      <c r="G67" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H67" s="103" t="s">
+      <c r="H67" s="102" t="s">
         <v>137</v>
       </c>
-      <c r="I67" s="105" t="s">
+      <c r="I67" s="104" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="79.150000000000006" customHeight="1">
-      <c r="A68" s="228"/>
-      <c r="B68" s="103" t="s">
+      <c r="A68" s="226"/>
+      <c r="B68" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C68" s="103" t="s">
+      <c r="C68" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D68" s="98" t="s">
+      <c r="D68" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E68" s="104" t="s">
+      <c r="E68" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="F68" s="103" t="s">
+      <c r="F68" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G68" s="82" t="s">
+      <c r="G68" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H68" s="103" t="s">
+      <c r="H68" s="102" t="s">
         <v>138</v>
       </c>
-      <c r="I68" s="105" t="s">
+      <c r="I68" s="104" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="77.45" customHeight="1">
-      <c r="A69" s="228"/>
-      <c r="B69" s="103" t="s">
+      <c r="A69" s="226"/>
+      <c r="B69" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C69" s="103" t="s">
+      <c r="C69" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D69" s="98" t="s">
+      <c r="D69" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E69" s="104" t="s">
+      <c r="E69" s="103" t="s">
         <v>246</v>
       </c>
-      <c r="F69" s="103" t="s">
+      <c r="F69" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G69" s="82" t="s">
+      <c r="G69" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H69" s="103" t="s">
+      <c r="H69" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="I69" s="105" t="s">
+      <c r="I69" s="104" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="76.900000000000006" customHeight="1">
-      <c r="A70" s="228"/>
-      <c r="B70" s="103" t="s">
+      <c r="A70" s="226"/>
+      <c r="B70" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="C70" s="103" t="s">
+      <c r="C70" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D70" s="98" t="s">
+      <c r="D70" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E70" s="104" t="s">
+      <c r="E70" s="103" t="s">
         <v>247</v>
       </c>
-      <c r="F70" s="103" t="s">
+      <c r="F70" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G70" s="82" t="s">
+      <c r="G70" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="H70" s="103" t="s">
+      <c r="H70" s="102" t="s">
         <v>140</v>
       </c>
-      <c r="I70" s="105" t="s">
+      <c r="I70" s="104" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="75" customHeight="1">
-      <c r="A71" s="228"/>
+      <c r="A71" s="226"/>
     </row>
     <row r="72" spans="1:9" ht="84.6" customHeight="1">
-      <c r="A72" s="228"/>
+      <c r="A72" s="226"/>
     </row>
     <row r="73" spans="1:9" ht="74.45" customHeight="1">
-      <c r="A73" s="228"/>
+      <c r="A73" s="226"/>
     </row>
     <row r="74" spans="1:9" ht="78" customHeight="1">
-      <c r="A74" s="228"/>
+      <c r="A74" s="226"/>
     </row>
     <row r="75" spans="1:9" ht="78.599999999999994" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A2:H7"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
     <mergeCell ref="A15:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37689,15 +37672,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EDB39E34F5A9B445B025C05B2A05D030" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c21ef800502b5dc1190a9a0361733939">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f1f31ffb-9912-4459-99c8-b26e82094b51" xmlns:ns4="ce621958-37b1-43fe-a1f1-1aad67996a88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30daf50bb6192471b76b9808b4256f50" ns3:_="" ns4:_="">
     <xsd:import namespace="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
@@ -37892,6 +37866,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
   <ds:schemaRefs>
@@ -37910,14 +37893,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D01A9D5D-1824-48C2-8527-9D8749A8DDDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37934,4 +37909,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adaptación en el header del informe
</commit_message>
<xml_diff>
--- a/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
+++ b/02_Proyecto/09. Programa de Auditoria/G3_ProgramayPlanAuditoria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATIAS\Desktop\ESPE\Septimo_Semestre\Quality Assurance\Repo\2563_G3_ACSW\02_Proyecto\09. Programa de Auditoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EC0227-981D-4A5B-AF7D-DD11F7B5BBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2FF814-C2E5-4921-8648-76728C133310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3078,30 +3078,21 @@
     <xf numFmtId="0" fontId="42" fillId="8" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="10" fontId="19" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3111,50 +3102,10 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="44" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="50" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3162,27 +3113,57 @@
     <xf numFmtId="10" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="48" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="44" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3194,10 +3175,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3208,9 +3185,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3233,63 +3207,89 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="44" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="50" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="48" fillId="0" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="19" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3606,37 +3606,37 @@
     </row>
     <row r="2" spans="1:48" ht="42.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="205"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="206"/>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
-      <c r="L2" s="164"/>
-      <c r="M2" s="164"/>
-      <c r="N2" s="164"/>
-      <c r="O2" s="164"/>
-      <c r="P2" s="164"/>
-      <c r="Q2" s="165"/>
-      <c r="R2" s="203" t="s">
+      <c r="B2" s="156"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="136"/>
+      <c r="O2" s="136"/>
+      <c r="P2" s="136"/>
+      <c r="Q2" s="137"/>
+      <c r="R2" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="207"/>
-      <c r="T2" s="207"/>
-      <c r="U2" s="207"/>
-      <c r="V2" s="207"/>
-      <c r="W2" s="164"/>
-      <c r="X2" s="164"/>
-      <c r="Y2" s="165"/>
-      <c r="Z2" s="203" t="s">
+      <c r="S2" s="161"/>
+      <c r="T2" s="161"/>
+      <c r="U2" s="161"/>
+      <c r="V2" s="161"/>
+      <c r="W2" s="136"/>
+      <c r="X2" s="136"/>
+      <c r="Y2" s="137"/>
+      <c r="Z2" s="160" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="164"/>
-      <c r="AB2" s="165"/>
+      <c r="AA2" s="136"/>
+      <c r="AB2" s="137"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -3660,37 +3660,37 @@
     </row>
     <row r="3" spans="1:48" ht="48.75" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="183"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="208"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="164"/>
-      <c r="J3" s="164"/>
-      <c r="K3" s="164"/>
-      <c r="L3" s="164"/>
-      <c r="M3" s="164"/>
-      <c r="N3" s="164"/>
-      <c r="O3" s="164"/>
-      <c r="P3" s="164"/>
-      <c r="Q3" s="165"/>
-      <c r="R3" s="201" t="s">
+      <c r="B3" s="157"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="136"/>
+      <c r="L3" s="136"/>
+      <c r="M3" s="136"/>
+      <c r="N3" s="136"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="136"/>
+      <c r="Q3" s="137"/>
+      <c r="R3" s="163" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="202"/>
-      <c r="T3" s="202"/>
-      <c r="U3" s="202"/>
-      <c r="V3" s="202"/>
-      <c r="W3" s="164"/>
-      <c r="X3" s="164"/>
-      <c r="Y3" s="165"/>
-      <c r="Z3" s="203" t="s">
+      <c r="S3" s="164"/>
+      <c r="T3" s="164"/>
+      <c r="U3" s="164"/>
+      <c r="V3" s="164"/>
+      <c r="W3" s="136"/>
+      <c r="X3" s="136"/>
+      <c r="Y3" s="137"/>
+      <c r="Z3" s="160" t="s">
         <v>49</v>
       </c>
-      <c r="AA3" s="164"/>
-      <c r="AB3" s="165"/>
+      <c r="AA3" s="136"/>
+      <c r="AB3" s="137"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
@@ -3714,39 +3714,39 @@
     </row>
     <row r="4" spans="1:48" ht="21" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="165" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="164"/>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="200"/>
-      <c r="H4" s="164"/>
-      <c r="I4" s="164"/>
-      <c r="J4" s="164"/>
-      <c r="K4" s="164"/>
-      <c r="L4" s="164"/>
-      <c r="M4" s="164"/>
-      <c r="N4" s="164"/>
-      <c r="O4" s="164"/>
-      <c r="P4" s="164"/>
-      <c r="Q4" s="165"/>
-      <c r="R4" s="201" t="s">
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="136"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="136"/>
+      <c r="Q4" s="137"/>
+      <c r="R4" s="163" t="s">
         <v>75</v>
       </c>
-      <c r="S4" s="202"/>
-      <c r="T4" s="202"/>
-      <c r="U4" s="202"/>
-      <c r="V4" s="202"/>
-      <c r="W4" s="164"/>
-      <c r="X4" s="164"/>
-      <c r="Y4" s="165"/>
-      <c r="Z4" s="203" t="s">
+      <c r="S4" s="164"/>
+      <c r="T4" s="164"/>
+      <c r="U4" s="164"/>
+      <c r="V4" s="164"/>
+      <c r="W4" s="136"/>
+      <c r="X4" s="136"/>
+      <c r="Y4" s="137"/>
+      <c r="Z4" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="164"/>
-      <c r="AB4" s="165"/>
+      <c r="AA4" s="136"/>
+      <c r="AB4" s="137"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
@@ -3819,35 +3819,35 @@
       <c r="AV5" s="2"/>
     </row>
     <row r="6" spans="1:48" ht="81.75" customHeight="1">
-      <c r="B6" s="204" t="s">
+      <c r="B6" s="167" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="177"/>
-      <c r="D6" s="177"/>
-      <c r="E6" s="177"/>
-      <c r="F6" s="177"/>
-      <c r="G6" s="177"/>
-      <c r="H6" s="177"/>
-      <c r="I6" s="177"/>
-      <c r="J6" s="177"/>
-      <c r="K6" s="177"/>
-      <c r="L6" s="177"/>
-      <c r="M6" s="177"/>
-      <c r="N6" s="177"/>
-      <c r="O6" s="177"/>
-      <c r="P6" s="177"/>
-      <c r="Q6" s="177"/>
-      <c r="R6" s="177"/>
-      <c r="S6" s="177"/>
-      <c r="T6" s="177"/>
-      <c r="U6" s="177"/>
-      <c r="V6" s="177"/>
-      <c r="W6" s="177"/>
-      <c r="X6" s="177"/>
-      <c r="Y6" s="177"/>
-      <c r="Z6" s="177"/>
-      <c r="AA6" s="177"/>
-      <c r="AB6" s="177"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="146"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="146"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="146"/>
+      <c r="L6" s="146"/>
+      <c r="M6" s="146"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="146"/>
+      <c r="P6" s="146"/>
+      <c r="Q6" s="146"/>
+      <c r="R6" s="146"/>
+      <c r="S6" s="146"/>
+      <c r="T6" s="146"/>
+      <c r="U6" s="146"/>
+      <c r="V6" s="146"/>
+      <c r="W6" s="146"/>
+      <c r="X6" s="146"/>
+      <c r="Y6" s="146"/>
+      <c r="Z6" s="146"/>
+      <c r="AA6" s="146"/>
+      <c r="AB6" s="146"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="6"/>
@@ -3864,35 +3864,35 @@
       <c r="AP6" s="7"/>
     </row>
     <row r="7" spans="1:48" ht="198" customHeight="1">
-      <c r="B7" s="176" t="s">
+      <c r="B7" s="168" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="177"/>
-      <c r="D7" s="177"/>
-      <c r="E7" s="177"/>
-      <c r="F7" s="177"/>
-      <c r="G7" s="177"/>
-      <c r="H7" s="177"/>
-      <c r="I7" s="177"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="177"/>
-      <c r="L7" s="177"/>
-      <c r="M7" s="177"/>
-      <c r="N7" s="177"/>
-      <c r="O7" s="177"/>
-      <c r="P7" s="177"/>
-      <c r="Q7" s="177"/>
-      <c r="R7" s="177"/>
-      <c r="S7" s="177"/>
-      <c r="T7" s="177"/>
-      <c r="U7" s="177"/>
-      <c r="V7" s="177"/>
-      <c r="W7" s="177"/>
-      <c r="X7" s="177"/>
-      <c r="Y7" s="177"/>
-      <c r="Z7" s="177"/>
-      <c r="AA7" s="177"/>
-      <c r="AB7" s="177"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="146"/>
+      <c r="H7" s="146"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="146"/>
+      <c r="K7" s="146"/>
+      <c r="L7" s="146"/>
+      <c r="M7" s="146"/>
+      <c r="N7" s="146"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="146"/>
+      <c r="R7" s="146"/>
+      <c r="S7" s="146"/>
+      <c r="T7" s="146"/>
+      <c r="U7" s="146"/>
+      <c r="V7" s="146"/>
+      <c r="W7" s="146"/>
+      <c r="X7" s="146"/>
+      <c r="Y7" s="146"/>
+      <c r="Z7" s="146"/>
+      <c r="AA7" s="146"/>
+      <c r="AB7" s="146"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
       <c r="AE7" s="6"/>
@@ -3909,35 +3909,35 @@
       <c r="AP7" s="7"/>
     </row>
     <row r="8" spans="1:48" ht="51" customHeight="1">
-      <c r="B8" s="198" t="s">
+      <c r="B8" s="169" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="177"/>
-      <c r="D8" s="177"/>
-      <c r="E8" s="177"/>
-      <c r="F8" s="177"/>
-      <c r="G8" s="177"/>
-      <c r="H8" s="177"/>
-      <c r="I8" s="177"/>
-      <c r="J8" s="177"/>
-      <c r="K8" s="177"/>
-      <c r="L8" s="177"/>
-      <c r="M8" s="177"/>
-      <c r="N8" s="177"/>
-      <c r="O8" s="177"/>
-      <c r="P8" s="177"/>
-      <c r="Q8" s="177"/>
-      <c r="R8" s="177"/>
-      <c r="S8" s="177"/>
-      <c r="T8" s="177"/>
-      <c r="U8" s="177"/>
-      <c r="V8" s="177"/>
-      <c r="W8" s="177"/>
-      <c r="X8" s="177"/>
-      <c r="Y8" s="177"/>
-      <c r="Z8" s="177"/>
-      <c r="AA8" s="177"/>
-      <c r="AB8" s="177"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="146"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="146"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="146"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="146"/>
+      <c r="M8" s="146"/>
+      <c r="N8" s="146"/>
+      <c r="O8" s="146"/>
+      <c r="P8" s="146"/>
+      <c r="Q8" s="146"/>
+      <c r="R8" s="146"/>
+      <c r="S8" s="146"/>
+      <c r="T8" s="146"/>
+      <c r="U8" s="146"/>
+      <c r="V8" s="146"/>
+      <c r="W8" s="146"/>
+      <c r="X8" s="146"/>
+      <c r="Y8" s="146"/>
+      <c r="Z8" s="146"/>
+      <c r="AA8" s="146"/>
+      <c r="AB8" s="146"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="6"/>
@@ -3997,35 +3997,35 @@
       <c r="AP9" s="7"/>
     </row>
     <row r="10" spans="1:48" ht="20.25" customHeight="1">
-      <c r="B10" s="198" t="s">
+      <c r="B10" s="169" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="177"/>
-      <c r="D10" s="177"/>
-      <c r="E10" s="177"/>
-      <c r="F10" s="177"/>
-      <c r="G10" s="177"/>
-      <c r="H10" s="177"/>
-      <c r="I10" s="177"/>
-      <c r="J10" s="177"/>
-      <c r="K10" s="177"/>
-      <c r="L10" s="177"/>
-      <c r="M10" s="177"/>
-      <c r="N10" s="177"/>
-      <c r="O10" s="177"/>
-      <c r="P10" s="177"/>
-      <c r="Q10" s="177"/>
-      <c r="R10" s="177"/>
-      <c r="S10" s="177"/>
-      <c r="T10" s="177"/>
-      <c r="U10" s="177"/>
-      <c r="V10" s="177"/>
-      <c r="W10" s="177"/>
-      <c r="X10" s="177"/>
-      <c r="Y10" s="177"/>
-      <c r="Z10" s="177"/>
-      <c r="AA10" s="177"/>
-      <c r="AB10" s="177"/>
+      <c r="C10" s="146"/>
+      <c r="D10" s="146"/>
+      <c r="E10" s="146"/>
+      <c r="F10" s="146"/>
+      <c r="G10" s="146"/>
+      <c r="H10" s="146"/>
+      <c r="I10" s="146"/>
+      <c r="J10" s="146"/>
+      <c r="K10" s="146"/>
+      <c r="L10" s="146"/>
+      <c r="M10" s="146"/>
+      <c r="N10" s="146"/>
+      <c r="O10" s="146"/>
+      <c r="P10" s="146"/>
+      <c r="Q10" s="146"/>
+      <c r="R10" s="146"/>
+      <c r="S10" s="146"/>
+      <c r="T10" s="146"/>
+      <c r="U10" s="146"/>
+      <c r="V10" s="146"/>
+      <c r="W10" s="146"/>
+      <c r="X10" s="146"/>
+      <c r="Y10" s="146"/>
+      <c r="Z10" s="146"/>
+      <c r="AA10" s="146"/>
+      <c r="AB10" s="146"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="6"/>
@@ -4043,35 +4043,35 @@
     </row>
     <row r="11" spans="1:48" ht="60" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="176" t="s">
+      <c r="B11" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="177"/>
-      <c r="D11" s="177"/>
-      <c r="E11" s="177"/>
-      <c r="F11" s="177"/>
-      <c r="G11" s="177"/>
-      <c r="H11" s="177"/>
-      <c r="I11" s="177"/>
-      <c r="J11" s="177"/>
-      <c r="K11" s="177"/>
-      <c r="L11" s="177"/>
-      <c r="M11" s="177"/>
-      <c r="N11" s="177"/>
-      <c r="O11" s="177"/>
-      <c r="P11" s="177"/>
-      <c r="Q11" s="177"/>
-      <c r="R11" s="177"/>
-      <c r="S11" s="177"/>
-      <c r="T11" s="177"/>
-      <c r="U11" s="177"/>
-      <c r="V11" s="177"/>
-      <c r="W11" s="177"/>
-      <c r="X11" s="177"/>
-      <c r="Y11" s="177"/>
-      <c r="Z11" s="177"/>
-      <c r="AA11" s="177"/>
-      <c r="AB11" s="177"/>
+      <c r="C11" s="146"/>
+      <c r="D11" s="146"/>
+      <c r="E11" s="146"/>
+      <c r="F11" s="146"/>
+      <c r="G11" s="146"/>
+      <c r="H11" s="146"/>
+      <c r="I11" s="146"/>
+      <c r="J11" s="146"/>
+      <c r="K11" s="146"/>
+      <c r="L11" s="146"/>
+      <c r="M11" s="146"/>
+      <c r="N11" s="146"/>
+      <c r="O11" s="146"/>
+      <c r="P11" s="146"/>
+      <c r="Q11" s="146"/>
+      <c r="R11" s="146"/>
+      <c r="S11" s="146"/>
+      <c r="T11" s="146"/>
+      <c r="U11" s="146"/>
+      <c r="V11" s="146"/>
+      <c r="W11" s="146"/>
+      <c r="X11" s="146"/>
+      <c r="Y11" s="146"/>
+      <c r="Z11" s="146"/>
+      <c r="AA11" s="146"/>
+      <c r="AB11" s="146"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="9"/>
       <c r="AE11" s="9"/>
@@ -4094,35 +4094,35 @@
       <c r="AV11" s="8"/>
     </row>
     <row r="12" spans="1:48" ht="53.25" customHeight="1">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="168" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="177"/>
-      <c r="E12" s="177"/>
-      <c r="F12" s="177"/>
-      <c r="G12" s="177"/>
-      <c r="H12" s="177"/>
-      <c r="I12" s="177"/>
-      <c r="J12" s="177"/>
-      <c r="K12" s="177"/>
-      <c r="L12" s="177"/>
-      <c r="M12" s="177"/>
-      <c r="N12" s="177"/>
-      <c r="O12" s="177"/>
-      <c r="P12" s="177"/>
-      <c r="Q12" s="177"/>
-      <c r="R12" s="177"/>
-      <c r="S12" s="177"/>
-      <c r="T12" s="177"/>
-      <c r="U12" s="177"/>
-      <c r="V12" s="177"/>
-      <c r="W12" s="177"/>
-      <c r="X12" s="177"/>
-      <c r="Y12" s="177"/>
-      <c r="Z12" s="177"/>
-      <c r="AA12" s="177"/>
-      <c r="AB12" s="177"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="146"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="146"/>
+      <c r="H12" s="146"/>
+      <c r="I12" s="146"/>
+      <c r="J12" s="146"/>
+      <c r="K12" s="146"/>
+      <c r="L12" s="146"/>
+      <c r="M12" s="146"/>
+      <c r="N12" s="146"/>
+      <c r="O12" s="146"/>
+      <c r="P12" s="146"/>
+      <c r="Q12" s="146"/>
+      <c r="R12" s="146"/>
+      <c r="S12" s="146"/>
+      <c r="T12" s="146"/>
+      <c r="U12" s="146"/>
+      <c r="V12" s="146"/>
+      <c r="W12" s="146"/>
+      <c r="X12" s="146"/>
+      <c r="Y12" s="146"/>
+      <c r="Z12" s="146"/>
+      <c r="AA12" s="146"/>
+      <c r="AB12" s="146"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
@@ -4139,35 +4139,35 @@
       <c r="AP12" s="7"/>
     </row>
     <row r="13" spans="1:48" ht="39.75" customHeight="1">
-      <c r="B13" s="176" t="s">
+      <c r="B13" s="168" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="177"/>
-      <c r="D13" s="177"/>
-      <c r="E13" s="177"/>
-      <c r="F13" s="177"/>
-      <c r="G13" s="177"/>
-      <c r="H13" s="177"/>
-      <c r="I13" s="177"/>
-      <c r="J13" s="177"/>
-      <c r="K13" s="177"/>
-      <c r="L13" s="177"/>
-      <c r="M13" s="177"/>
-      <c r="N13" s="177"/>
-      <c r="O13" s="177"/>
-      <c r="P13" s="177"/>
-      <c r="Q13" s="177"/>
-      <c r="R13" s="177"/>
-      <c r="S13" s="177"/>
-      <c r="T13" s="177"/>
-      <c r="U13" s="177"/>
-      <c r="V13" s="177"/>
-      <c r="W13" s="177"/>
-      <c r="X13" s="177"/>
-      <c r="Y13" s="177"/>
-      <c r="Z13" s="177"/>
-      <c r="AA13" s="177"/>
-      <c r="AB13" s="177"/>
+      <c r="C13" s="146"/>
+      <c r="D13" s="146"/>
+      <c r="E13" s="146"/>
+      <c r="F13" s="146"/>
+      <c r="G13" s="146"/>
+      <c r="H13" s="146"/>
+      <c r="I13" s="146"/>
+      <c r="J13" s="146"/>
+      <c r="K13" s="146"/>
+      <c r="L13" s="146"/>
+      <c r="M13" s="146"/>
+      <c r="N13" s="146"/>
+      <c r="O13" s="146"/>
+      <c r="P13" s="146"/>
+      <c r="Q13" s="146"/>
+      <c r="R13" s="146"/>
+      <c r="S13" s="146"/>
+      <c r="T13" s="146"/>
+      <c r="U13" s="146"/>
+      <c r="V13" s="146"/>
+      <c r="W13" s="146"/>
+      <c r="X13" s="146"/>
+      <c r="Y13" s="146"/>
+      <c r="Z13" s="146"/>
+      <c r="AA13" s="146"/>
+      <c r="AB13" s="146"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
@@ -4227,35 +4227,35 @@
       <c r="AP14" s="7"/>
     </row>
     <row r="15" spans="1:48" ht="99.75" customHeight="1">
-      <c r="B15" s="178" t="s">
+      <c r="B15" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="177"/>
-      <c r="D15" s="177"/>
-      <c r="E15" s="177"/>
-      <c r="F15" s="177"/>
-      <c r="G15" s="177"/>
-      <c r="H15" s="177"/>
-      <c r="I15" s="177"/>
-      <c r="J15" s="177"/>
-      <c r="K15" s="177"/>
-      <c r="L15" s="177"/>
-      <c r="M15" s="177"/>
-      <c r="N15" s="177"/>
-      <c r="O15" s="177"/>
-      <c r="P15" s="177"/>
-      <c r="Q15" s="177"/>
-      <c r="R15" s="177"/>
-      <c r="S15" s="177"/>
-      <c r="T15" s="177"/>
-      <c r="U15" s="177"/>
-      <c r="V15" s="177"/>
-      <c r="W15" s="177"/>
-      <c r="X15" s="177"/>
-      <c r="Y15" s="177"/>
-      <c r="Z15" s="177"/>
-      <c r="AA15" s="177"/>
-      <c r="AB15" s="177"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="146"/>
+      <c r="E15" s="146"/>
+      <c r="F15" s="146"/>
+      <c r="G15" s="146"/>
+      <c r="H15" s="146"/>
+      <c r="I15" s="146"/>
+      <c r="J15" s="146"/>
+      <c r="K15" s="146"/>
+      <c r="L15" s="146"/>
+      <c r="M15" s="146"/>
+      <c r="N15" s="146"/>
+      <c r="O15" s="146"/>
+      <c r="P15" s="146"/>
+      <c r="Q15" s="146"/>
+      <c r="R15" s="146"/>
+      <c r="S15" s="146"/>
+      <c r="T15" s="146"/>
+      <c r="U15" s="146"/>
+      <c r="V15" s="146"/>
+      <c r="W15" s="146"/>
+      <c r="X15" s="146"/>
+      <c r="Y15" s="146"/>
+      <c r="Z15" s="146"/>
+      <c r="AA15" s="146"/>
+      <c r="AB15" s="146"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="6"/>
@@ -4273,35 +4273,35 @@
     </row>
     <row r="16" spans="1:48" ht="24.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="179" t="s">
+      <c r="B16" s="174" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="177"/>
-      <c r="D16" s="177"/>
-      <c r="E16" s="177"/>
-      <c r="F16" s="177"/>
-      <c r="G16" s="177"/>
-      <c r="H16" s="177"/>
-      <c r="I16" s="177"/>
-      <c r="J16" s="177"/>
-      <c r="K16" s="177"/>
-      <c r="L16" s="177"/>
-      <c r="M16" s="177"/>
-      <c r="N16" s="177"/>
-      <c r="O16" s="177"/>
-      <c r="P16" s="177"/>
-      <c r="Q16" s="177"/>
-      <c r="R16" s="177"/>
-      <c r="S16" s="177"/>
-      <c r="T16" s="177"/>
-      <c r="U16" s="177"/>
-      <c r="V16" s="177"/>
-      <c r="W16" s="177"/>
-      <c r="X16" s="177"/>
-      <c r="Y16" s="177"/>
-      <c r="Z16" s="177"/>
-      <c r="AA16" s="177"/>
-      <c r="AB16" s="177"/>
+      <c r="C16" s="146"/>
+      <c r="D16" s="146"/>
+      <c r="E16" s="146"/>
+      <c r="F16" s="146"/>
+      <c r="G16" s="146"/>
+      <c r="H16" s="146"/>
+      <c r="I16" s="146"/>
+      <c r="J16" s="146"/>
+      <c r="K16" s="146"/>
+      <c r="L16" s="146"/>
+      <c r="M16" s="146"/>
+      <c r="N16" s="146"/>
+      <c r="O16" s="146"/>
+      <c r="P16" s="146"/>
+      <c r="Q16" s="146"/>
+      <c r="R16" s="146"/>
+      <c r="S16" s="146"/>
+      <c r="T16" s="146"/>
+      <c r="U16" s="146"/>
+      <c r="V16" s="146"/>
+      <c r="W16" s="146"/>
+      <c r="X16" s="146"/>
+      <c r="Y16" s="146"/>
+      <c r="Z16" s="146"/>
+      <c r="AA16" s="146"/>
+      <c r="AB16" s="146"/>
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
@@ -4324,35 +4324,35 @@
       <c r="AV16" s="2"/>
     </row>
     <row r="17" spans="1:49" ht="24.75" customHeight="1">
-      <c r="B17" s="178" t="s">
+      <c r="B17" s="173" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="177"/>
-      <c r="D17" s="177"/>
-      <c r="E17" s="177"/>
-      <c r="F17" s="177"/>
-      <c r="G17" s="177"/>
-      <c r="H17" s="177"/>
-      <c r="I17" s="177"/>
-      <c r="J17" s="177"/>
-      <c r="K17" s="177"/>
-      <c r="L17" s="177"/>
-      <c r="M17" s="177"/>
-      <c r="N17" s="177"/>
-      <c r="O17" s="177"/>
-      <c r="P17" s="177"/>
-      <c r="Q17" s="177"/>
-      <c r="R17" s="177"/>
-      <c r="S17" s="177"/>
-      <c r="T17" s="177"/>
-      <c r="U17" s="177"/>
-      <c r="V17" s="177"/>
-      <c r="W17" s="177"/>
-      <c r="X17" s="177"/>
-      <c r="Y17" s="177"/>
-      <c r="Z17" s="177"/>
-      <c r="AA17" s="177"/>
-      <c r="AB17" s="177"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="146"/>
+      <c r="H17" s="146"/>
+      <c r="I17" s="146"/>
+      <c r="J17" s="146"/>
+      <c r="K17" s="146"/>
+      <c r="L17" s="146"/>
+      <c r="M17" s="146"/>
+      <c r="N17" s="146"/>
+      <c r="O17" s="146"/>
+      <c r="P17" s="146"/>
+      <c r="Q17" s="146"/>
+      <c r="R17" s="146"/>
+      <c r="S17" s="146"/>
+      <c r="T17" s="146"/>
+      <c r="U17" s="146"/>
+      <c r="V17" s="146"/>
+      <c r="W17" s="146"/>
+      <c r="X17" s="146"/>
+      <c r="Y17" s="146"/>
+      <c r="Z17" s="146"/>
+      <c r="AA17" s="146"/>
+      <c r="AB17" s="146"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="6"/>
@@ -4369,33 +4369,33 @@
       <c r="AP17" s="7"/>
     </row>
     <row r="18" spans="1:49" ht="6.75" customHeight="1">
-      <c r="B18" s="178"/>
-      <c r="C18" s="177"/>
-      <c r="D18" s="177"/>
-      <c r="E18" s="177"/>
-      <c r="F18" s="177"/>
-      <c r="G18" s="177"/>
-      <c r="H18" s="177"/>
-      <c r="I18" s="177"/>
-      <c r="J18" s="177"/>
-      <c r="K18" s="177"/>
-      <c r="L18" s="177"/>
-      <c r="M18" s="177"/>
-      <c r="N18" s="177"/>
-      <c r="O18" s="177"/>
-      <c r="P18" s="177"/>
-      <c r="Q18" s="177"/>
-      <c r="R18" s="177"/>
-      <c r="S18" s="177"/>
-      <c r="T18" s="177"/>
-      <c r="U18" s="177"/>
-      <c r="V18" s="177"/>
-      <c r="W18" s="177"/>
-      <c r="X18" s="177"/>
-      <c r="Y18" s="177"/>
-      <c r="Z18" s="177"/>
-      <c r="AA18" s="177"/>
-      <c r="AB18" s="177"/>
+      <c r="B18" s="173"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="146"/>
+      <c r="F18" s="146"/>
+      <c r="G18" s="146"/>
+      <c r="H18" s="146"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="146"/>
+      <c r="K18" s="146"/>
+      <c r="L18" s="146"/>
+      <c r="M18" s="146"/>
+      <c r="N18" s="146"/>
+      <c r="O18" s="146"/>
+      <c r="P18" s="146"/>
+      <c r="Q18" s="146"/>
+      <c r="R18" s="146"/>
+      <c r="S18" s="146"/>
+      <c r="T18" s="146"/>
+      <c r="U18" s="146"/>
+      <c r="V18" s="146"/>
+      <c r="W18" s="146"/>
+      <c r="X18" s="146"/>
+      <c r="Y18" s="146"/>
+      <c r="Z18" s="146"/>
+      <c r="AA18" s="146"/>
+      <c r="AB18" s="146"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
@@ -4413,44 +4413,44 @@
     </row>
     <row r="19" spans="1:49" ht="36.75" customHeight="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="190" t="s">
+      <c r="B19" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="193" t="s">
+      <c r="C19" s="185" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="181"/>
-      <c r="E19" s="182"/>
-      <c r="F19" s="194" t="s">
+      <c r="D19" s="176"/>
+      <c r="E19" s="177"/>
+      <c r="F19" s="186" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="180" t="s">
+      <c r="G19" s="175" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="181"/>
-      <c r="I19" s="181"/>
-      <c r="J19" s="181"/>
-      <c r="K19" s="181"/>
-      <c r="L19" s="181"/>
-      <c r="M19" s="181"/>
-      <c r="N19" s="182"/>
-      <c r="O19" s="180" t="s">
+      <c r="H19" s="176"/>
+      <c r="I19" s="176"/>
+      <c r="J19" s="176"/>
+      <c r="K19" s="176"/>
+      <c r="L19" s="176"/>
+      <c r="M19" s="176"/>
+      <c r="N19" s="177"/>
+      <c r="O19" s="175" t="s">
         <v>52</v>
       </c>
-      <c r="P19" s="181"/>
-      <c r="Q19" s="181"/>
-      <c r="R19" s="181"/>
-      <c r="S19" s="181"/>
-      <c r="T19" s="181"/>
-      <c r="U19" s="181"/>
-      <c r="V19" s="181"/>
-      <c r="W19" s="182"/>
-      <c r="X19" s="186" t="s">
+      <c r="P19" s="176"/>
+      <c r="Q19" s="176"/>
+      <c r="R19" s="176"/>
+      <c r="S19" s="176"/>
+      <c r="T19" s="176"/>
+      <c r="U19" s="176"/>
+      <c r="V19" s="176"/>
+      <c r="W19" s="177"/>
+      <c r="X19" s="178" t="s">
         <v>8</v>
       </c>
-      <c r="Y19" s="181"/>
-      <c r="Z19" s="181"/>
-      <c r="AA19" s="182"/>
+      <c r="Y19" s="176"/>
+      <c r="Z19" s="176"/>
+      <c r="AA19" s="177"/>
       <c r="AB19" s="73" t="s">
         <v>9</v>
       </c>
@@ -4477,32 +4477,32 @@
     </row>
     <row r="20" spans="1:49" ht="10.5" customHeight="1">
       <c r="A20" s="14"/>
-      <c r="B20" s="191"/>
-      <c r="C20" s="187"/>
-      <c r="D20" s="177"/>
-      <c r="E20" s="188"/>
-      <c r="F20" s="195"/>
-      <c r="G20" s="183"/>
-      <c r="H20" s="184"/>
-      <c r="I20" s="184"/>
-      <c r="J20" s="184"/>
-      <c r="K20" s="184"/>
-      <c r="L20" s="184"/>
-      <c r="M20" s="184"/>
-      <c r="N20" s="185"/>
-      <c r="O20" s="187"/>
-      <c r="P20" s="197"/>
-      <c r="Q20" s="197"/>
-      <c r="R20" s="197"/>
-      <c r="S20" s="197"/>
-      <c r="T20" s="197"/>
-      <c r="U20" s="197"/>
-      <c r="V20" s="197"/>
-      <c r="W20" s="188"/>
-      <c r="X20" s="187"/>
-      <c r="Y20" s="177"/>
-      <c r="Z20" s="177"/>
-      <c r="AA20" s="188"/>
+      <c r="B20" s="183"/>
+      <c r="C20" s="179"/>
+      <c r="D20" s="146"/>
+      <c r="E20" s="180"/>
+      <c r="F20" s="187"/>
+      <c r="G20" s="157"/>
+      <c r="H20" s="141"/>
+      <c r="I20" s="141"/>
+      <c r="J20" s="141"/>
+      <c r="K20" s="141"/>
+      <c r="L20" s="141"/>
+      <c r="M20" s="141"/>
+      <c r="N20" s="158"/>
+      <c r="O20" s="179"/>
+      <c r="P20" s="189"/>
+      <c r="Q20" s="189"/>
+      <c r="R20" s="189"/>
+      <c r="S20" s="189"/>
+      <c r="T20" s="189"/>
+      <c r="U20" s="189"/>
+      <c r="V20" s="189"/>
+      <c r="W20" s="180"/>
+      <c r="X20" s="179"/>
+      <c r="Y20" s="146"/>
+      <c r="Z20" s="146"/>
+      <c r="AA20" s="180"/>
       <c r="AB20" s="74"/>
       <c r="AC20" s="14"/>
       <c r="AD20" s="14"/>
@@ -4527,37 +4527,37 @@
     </row>
     <row r="21" spans="1:49" ht="34.5" customHeight="1">
       <c r="A21" s="15"/>
-      <c r="B21" s="191"/>
-      <c r="C21" s="187"/>
-      <c r="D21" s="177"/>
-      <c r="E21" s="188"/>
-      <c r="F21" s="195"/>
-      <c r="G21" s="189" t="s">
+      <c r="B21" s="183"/>
+      <c r="C21" s="179"/>
+      <c r="D21" s="146"/>
+      <c r="E21" s="180"/>
+      <c r="F21" s="187"/>
+      <c r="G21" s="181" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="165"/>
-      <c r="I21" s="189" t="s">
+      <c r="H21" s="137"/>
+      <c r="I21" s="181" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="165"/>
-      <c r="K21" s="189" t="s">
+      <c r="J21" s="137"/>
+      <c r="K21" s="181" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="165"/>
-      <c r="M21" s="189" t="s">
+      <c r="L21" s="137"/>
+      <c r="M21" s="181" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="164"/>
-      <c r="O21" s="156" t="s">
+      <c r="N21" s="136"/>
+      <c r="O21" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="P21" s="156"/>
-      <c r="Q21" s="156"/>
-      <c r="R21" s="156"/>
-      <c r="S21" s="155" t="s">
+      <c r="P21" s="201"/>
+      <c r="Q21" s="201"/>
+      <c r="R21" s="201"/>
+      <c r="S21" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="T21" s="156"/>
+      <c r="T21" s="201"/>
       <c r="U21" s="80" t="s">
         <v>12</v>
       </c>
@@ -4565,10 +4565,10 @@
         <v>13</v>
       </c>
       <c r="W21" s="77"/>
-      <c r="X21" s="184"/>
-      <c r="Y21" s="184"/>
-      <c r="Z21" s="184"/>
-      <c r="AA21" s="185"/>
+      <c r="X21" s="141"/>
+      <c r="Y21" s="141"/>
+      <c r="Z21" s="141"/>
+      <c r="AA21" s="158"/>
       <c r="AB21" s="74"/>
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
@@ -4593,11 +4593,11 @@
     </row>
     <row r="22" spans="1:49" ht="38.25" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="192"/>
-      <c r="C22" s="183"/>
-      <c r="D22" s="184"/>
-      <c r="E22" s="185"/>
-      <c r="F22" s="196"/>
+      <c r="B22" s="184"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="141"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="188"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
@@ -4624,10 +4624,10 @@
       <c r="P22" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="Q22" s="169">
+      <c r="Q22" s="191">
         <v>10</v>
       </c>
-      <c r="R22" s="170"/>
+      <c r="R22" s="192"/>
       <c r="S22" s="78" t="s">
         <v>57</v>
       </c>
@@ -4642,10 +4642,10 @@
       </c>
       <c r="W22" s="76"/>
       <c r="X22" s="76"/>
-      <c r="Y22" s="163"/>
-      <c r="Z22" s="164"/>
-      <c r="AA22" s="164"/>
-      <c r="AB22" s="165"/>
+      <c r="Y22" s="190"/>
+      <c r="Z22" s="136"/>
+      <c r="AA22" s="136"/>
+      <c r="AB22" s="137"/>
       <c r="AC22" s="75"/>
       <c r="AD22" s="14"/>
       <c r="AE22" s="14"/>
@@ -4673,11 +4673,11 @@
       <c r="B23" s="18">
         <v>1</v>
       </c>
-      <c r="C23" s="166" t="s">
+      <c r="C23" s="151" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="167"/>
-      <c r="E23" s="168"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="153"/>
       <c r="F23" s="66">
         <v>1</v>
       </c>
@@ -4693,19 +4693,19 @@
       <c r="N23" s="113"/>
       <c r="O23" s="114"/>
       <c r="P23" s="114"/>
-      <c r="Q23" s="171"/>
-      <c r="R23" s="172"/>
+      <c r="Q23" s="193"/>
+      <c r="R23" s="194"/>
       <c r="S23" s="115"/>
       <c r="T23" s="115"/>
       <c r="U23" s="115"/>
       <c r="V23" s="115"/>
       <c r="W23" s="22"/>
-      <c r="X23" s="143" t="s">
+      <c r="X23" s="142" t="s">
         <v>54</v>
       </c>
-      <c r="Y23" s="164"/>
-      <c r="Z23" s="164"/>
-      <c r="AA23" s="165"/>
+      <c r="Y23" s="136"/>
+      <c r="Z23" s="136"/>
+      <c r="AA23" s="137"/>
       <c r="AB23" s="23" t="s">
         <v>55</v>
       </c>
@@ -4728,11 +4728,11 @@
       <c r="B24" s="105">
         <v>2</v>
       </c>
-      <c r="C24" s="146" t="s">
+      <c r="C24" s="198" t="s">
         <v>190</v>
       </c>
-      <c r="D24" s="147"/>
-      <c r="E24" s="147"/>
+      <c r="D24" s="199"/>
+      <c r="E24" s="199"/>
       <c r="F24" s="106">
         <v>2</v>
       </c>
@@ -4748,19 +4748,19 @@
       <c r="N24" s="116"/>
       <c r="O24" s="116"/>
       <c r="P24" s="120"/>
-      <c r="Q24" s="138"/>
-      <c r="R24" s="139"/>
+      <c r="Q24" s="202"/>
+      <c r="R24" s="203"/>
       <c r="S24" s="121"/>
       <c r="T24" s="116"/>
       <c r="U24" s="116"/>
       <c r="V24" s="116"/>
       <c r="W24" s="108"/>
-      <c r="X24" s="173" t="s">
+      <c r="X24" s="170" t="s">
         <v>191</v>
       </c>
-      <c r="Y24" s="174"/>
-      <c r="Z24" s="174"/>
-      <c r="AA24" s="175"/>
+      <c r="Y24" s="171"/>
+      <c r="Z24" s="171"/>
+      <c r="AA24" s="172"/>
       <c r="AB24" s="23" t="s">
         <v>55</v>
       </c>
@@ -4783,11 +4783,11 @@
       <c r="B25" s="105">
         <v>3</v>
       </c>
-      <c r="C25" s="146" t="s">
+      <c r="C25" s="198" t="s">
         <v>192</v>
       </c>
-      <c r="D25" s="147"/>
-      <c r="E25" s="147"/>
+      <c r="D25" s="199"/>
+      <c r="E25" s="199"/>
       <c r="F25" s="106">
         <v>3</v>
       </c>
@@ -4803,19 +4803,19 @@
         <v>20</v>
       </c>
       <c r="P25" s="126"/>
-      <c r="Q25" s="138"/>
-      <c r="R25" s="139"/>
+      <c r="Q25" s="202"/>
+      <c r="R25" s="203"/>
       <c r="S25" s="125"/>
       <c r="T25" s="124"/>
       <c r="U25" s="116"/>
       <c r="V25" s="116"/>
       <c r="W25" s="108"/>
-      <c r="X25" s="135" t="s">
+      <c r="X25" s="208" t="s">
         <v>193</v>
       </c>
-      <c r="Y25" s="136"/>
-      <c r="Z25" s="136"/>
-      <c r="AA25" s="137"/>
+      <c r="Y25" s="209"/>
+      <c r="Z25" s="209"/>
+      <c r="AA25" s="210"/>
       <c r="AB25" s="23" t="s">
         <v>55</v>
       </c>
@@ -4838,11 +4838,11 @@
       <c r="B26" s="105">
         <v>4</v>
       </c>
-      <c r="C26" s="146" t="s">
+      <c r="C26" s="198" t="s">
         <v>194</v>
       </c>
-      <c r="D26" s="147"/>
-      <c r="E26" s="147"/>
+      <c r="D26" s="199"/>
+      <c r="E26" s="199"/>
       <c r="F26" s="106">
         <v>4</v>
       </c>
@@ -4856,8 +4856,8 @@
       <c r="N26" s="110"/>
       <c r="O26" s="120"/>
       <c r="P26" s="111"/>
-      <c r="Q26" s="152"/>
-      <c r="R26" s="153"/>
+      <c r="Q26" s="215"/>
+      <c r="R26" s="216"/>
       <c r="S26" s="125"/>
       <c r="T26" s="124" t="s">
         <v>20</v>
@@ -4865,12 +4865,12 @@
       <c r="U26" s="127"/>
       <c r="V26" s="116"/>
       <c r="W26" s="109"/>
-      <c r="X26" s="148" t="s">
+      <c r="X26" s="211" t="s">
         <v>195</v>
       </c>
-      <c r="Y26" s="148"/>
-      <c r="Z26" s="148"/>
-      <c r="AA26" s="148"/>
+      <c r="Y26" s="211"/>
+      <c r="Z26" s="211"/>
+      <c r="AA26" s="211"/>
       <c r="AB26" s="23" t="s">
         <v>55</v>
       </c>
@@ -4893,11 +4893,11 @@
       <c r="B27" s="105">
         <v>5</v>
       </c>
-      <c r="C27" s="146" t="s">
+      <c r="C27" s="198" t="s">
         <v>196</v>
       </c>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
+      <c r="D27" s="199"/>
+      <c r="E27" s="199"/>
       <c r="F27" s="106">
         <v>5</v>
       </c>
@@ -4911,8 +4911,8 @@
       <c r="N27" s="130"/>
       <c r="O27" s="116"/>
       <c r="P27" s="110"/>
-      <c r="Q27" s="154"/>
-      <c r="R27" s="154"/>
+      <c r="Q27" s="217"/>
+      <c r="R27" s="217"/>
       <c r="S27" s="131"/>
       <c r="T27" s="128"/>
       <c r="U27" s="129" t="s">
@@ -4920,12 +4920,12 @@
       </c>
       <c r="V27" s="130"/>
       <c r="W27" s="109"/>
-      <c r="X27" s="148" t="s">
+      <c r="X27" s="211" t="s">
         <v>197</v>
       </c>
-      <c r="Y27" s="148"/>
-      <c r="Z27" s="148"/>
-      <c r="AA27" s="148"/>
+      <c r="Y27" s="211"/>
+      <c r="Z27" s="211"/>
+      <c r="AA27" s="211"/>
       <c r="AB27" s="23" t="s">
         <v>55</v>
       </c>
@@ -4948,11 +4948,11 @@
       <c r="B28" s="105">
         <v>6</v>
       </c>
-      <c r="C28" s="146" t="s">
+      <c r="C28" s="198" t="s">
         <v>198</v>
       </c>
-      <c r="D28" s="147"/>
-      <c r="E28" s="147"/>
+      <c r="D28" s="199"/>
+      <c r="E28" s="199"/>
       <c r="F28" s="106">
         <v>6</v>
       </c>
@@ -4966,8 +4966,8 @@
       <c r="N28" s="130"/>
       <c r="O28" s="116"/>
       <c r="P28" s="120"/>
-      <c r="Q28" s="154"/>
-      <c r="R28" s="154"/>
+      <c r="Q28" s="217"/>
+      <c r="R28" s="217"/>
       <c r="S28" s="131"/>
       <c r="T28" s="124"/>
       <c r="U28" s="129"/>
@@ -4975,12 +4975,12 @@
         <v>20</v>
       </c>
       <c r="W28" s="108"/>
-      <c r="X28" s="149" t="s">
+      <c r="X28" s="212" t="s">
         <v>199</v>
       </c>
-      <c r="Y28" s="150"/>
-      <c r="Z28" s="150"/>
-      <c r="AA28" s="151"/>
+      <c r="Y28" s="213"/>
+      <c r="Z28" s="213"/>
+      <c r="AA28" s="214"/>
       <c r="AB28" s="23" t="s">
         <v>55</v>
       </c>
@@ -5003,11 +5003,11 @@
       <c r="B29" s="18">
         <v>7</v>
       </c>
-      <c r="C29" s="140" t="s">
+      <c r="C29" s="195" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="141"/>
-      <c r="E29" s="142"/>
+      <c r="D29" s="196"/>
+      <c r="E29" s="197"/>
       <c r="F29" s="66">
         <v>7</v>
       </c>
@@ -5021,8 +5021,8 @@
       <c r="N29" s="113"/>
       <c r="O29" s="113"/>
       <c r="P29" s="113"/>
-      <c r="Q29" s="157"/>
-      <c r="R29" s="158"/>
+      <c r="Q29" s="204"/>
+      <c r="R29" s="205"/>
       <c r="S29" s="115"/>
       <c r="T29" s="115"/>
       <c r="U29" s="115"/>
@@ -5030,12 +5030,12 @@
         <v>20</v>
       </c>
       <c r="W29" s="22"/>
-      <c r="X29" s="143" t="s">
+      <c r="X29" s="142" t="s">
         <v>68</v>
       </c>
-      <c r="Y29" s="144"/>
-      <c r="Z29" s="144"/>
-      <c r="AA29" s="145"/>
+      <c r="Y29" s="143"/>
+      <c r="Z29" s="143"/>
+      <c r="AA29" s="144"/>
       <c r="AB29" s="23" t="s">
         <v>60</v>
       </c>
@@ -5065,11 +5065,11 @@
       <c r="B30" s="18">
         <v>8</v>
       </c>
-      <c r="C30" s="140" t="s">
+      <c r="C30" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="141"/>
-      <c r="E30" s="142"/>
+      <c r="D30" s="196"/>
+      <c r="E30" s="197"/>
       <c r="F30" s="66">
         <v>8</v>
       </c>
@@ -5083,8 +5083,8 @@
       <c r="N30" s="113"/>
       <c r="O30" s="113"/>
       <c r="P30" s="113"/>
-      <c r="Q30" s="159"/>
-      <c r="R30" s="160"/>
+      <c r="Q30" s="206"/>
+      <c r="R30" s="207"/>
       <c r="S30" s="115"/>
       <c r="T30" s="115"/>
       <c r="U30" s="115"/>
@@ -5092,12 +5092,12 @@
         <v>20</v>
       </c>
       <c r="W30" s="22"/>
-      <c r="X30" s="143" t="s">
+      <c r="X30" s="142" t="s">
         <v>23</v>
       </c>
-      <c r="Y30" s="144"/>
-      <c r="Z30" s="144"/>
-      <c r="AA30" s="145"/>
+      <c r="Y30" s="143"/>
+      <c r="Z30" s="143"/>
+      <c r="AA30" s="144"/>
       <c r="AB30" s="23" t="s">
         <v>55</v>
       </c>
@@ -5127,11 +5127,11 @@
       <c r="B31" s="18">
         <v>9</v>
       </c>
-      <c r="C31" s="140" t="s">
+      <c r="C31" s="195" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="141"/>
-      <c r="E31" s="142"/>
+      <c r="D31" s="196"/>
+      <c r="E31" s="197"/>
       <c r="F31" s="70">
         <v>9</v>
       </c>
@@ -5145,8 +5145,8 @@
       <c r="N31" s="113"/>
       <c r="O31" s="113"/>
       <c r="P31" s="113"/>
-      <c r="Q31" s="159"/>
-      <c r="R31" s="160"/>
+      <c r="Q31" s="206"/>
+      <c r="R31" s="207"/>
       <c r="S31" s="115"/>
       <c r="T31" s="115"/>
       <c r="U31" s="115"/>
@@ -5154,12 +5154,12 @@
         <v>20</v>
       </c>
       <c r="W31" s="22"/>
-      <c r="X31" s="143" t="s">
+      <c r="X31" s="142" t="s">
         <v>25</v>
       </c>
-      <c r="Y31" s="144"/>
-      <c r="Z31" s="144"/>
-      <c r="AA31" s="145"/>
+      <c r="Y31" s="143"/>
+      <c r="Z31" s="143"/>
+      <c r="AA31" s="144"/>
       <c r="AB31" s="23" t="s">
         <v>59</v>
       </c>
@@ -5187,9 +5187,9 @@
     <row r="32" spans="1:49" ht="90.75" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
-      <c r="C32" s="140"/>
-      <c r="D32" s="141"/>
-      <c r="E32" s="142"/>
+      <c r="C32" s="195"/>
+      <c r="D32" s="196"/>
+      <c r="E32" s="197"/>
       <c r="F32" s="71"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
@@ -5201,19 +5201,19 @@
       <c r="N32" s="21"/>
       <c r="O32" s="21"/>
       <c r="P32" s="21"/>
-      <c r="Q32" s="161"/>
-      <c r="R32" s="162"/>
+      <c r="Q32" s="148"/>
+      <c r="R32" s="149"/>
       <c r="S32" s="22"/>
       <c r="T32" s="22"/>
       <c r="U32" s="22"/>
       <c r="V32" s="22"/>
       <c r="W32" s="22"/>
-      <c r="X32" s="143" t="s">
+      <c r="X32" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="Y32" s="144"/>
-      <c r="Z32" s="144"/>
-      <c r="AA32" s="145"/>
+      <c r="Y32" s="143"/>
+      <c r="Z32" s="143"/>
+      <c r="AA32" s="144"/>
       <c r="AB32" s="23"/>
       <c r="AC32" s="17"/>
       <c r="AD32" s="17"/>
@@ -5239,9 +5239,9 @@
     <row r="33" spans="1:29" ht="14.25" customHeight="1">
       <c r="A33" s="26"/>
       <c r="B33" s="18"/>
-      <c r="C33" s="166"/>
-      <c r="D33" s="167"/>
-      <c r="E33" s="168"/>
+      <c r="C33" s="151"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="153"/>
       <c r="F33" s="19"/>
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
@@ -5253,25 +5253,25 @@
       <c r="N33" s="25"/>
       <c r="O33" s="21"/>
       <c r="P33" s="21"/>
-      <c r="Q33" s="161"/>
-      <c r="R33" s="162"/>
+      <c r="Q33" s="148"/>
+      <c r="R33" s="149"/>
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
       <c r="U33" s="22"/>
       <c r="V33" s="22"/>
       <c r="W33" s="22"/>
-      <c r="X33" s="143"/>
-      <c r="Y33" s="164"/>
-      <c r="Z33" s="164"/>
-      <c r="AA33" s="165"/>
+      <c r="X33" s="142"/>
+      <c r="Y33" s="136"/>
+      <c r="Z33" s="136"/>
+      <c r="AA33" s="137"/>
       <c r="AB33" s="23"/>
     </row>
     <row r="34" spans="1:29" ht="12.75" customHeight="1">
       <c r="A34" s="26"/>
       <c r="B34" s="18"/>
-      <c r="C34" s="166"/>
-      <c r="D34" s="167"/>
-      <c r="E34" s="168"/>
+      <c r="C34" s="151"/>
+      <c r="D34" s="152"/>
+      <c r="E34" s="153"/>
       <c r="F34" s="19"/>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
@@ -5283,25 +5283,25 @@
       <c r="N34" s="21"/>
       <c r="O34" s="25"/>
       <c r="P34" s="21"/>
-      <c r="Q34" s="161"/>
-      <c r="R34" s="162"/>
+      <c r="Q34" s="148"/>
+      <c r="R34" s="149"/>
       <c r="S34" s="22"/>
       <c r="T34" s="22"/>
       <c r="U34" s="22"/>
       <c r="V34" s="22"/>
       <c r="W34" s="22"/>
-      <c r="X34" s="143"/>
-      <c r="Y34" s="164"/>
-      <c r="Z34" s="164"/>
-      <c r="AA34" s="165"/>
+      <c r="X34" s="142"/>
+      <c r="Y34" s="136"/>
+      <c r="Z34" s="136"/>
+      <c r="AA34" s="137"/>
       <c r="AB34" s="23"/>
     </row>
     <row r="35" spans="1:29" ht="19.5" customHeight="1">
       <c r="A35" s="26"/>
       <c r="B35" s="18"/>
-      <c r="C35" s="211"/>
-      <c r="D35" s="167"/>
-      <c r="E35" s="168"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="153"/>
       <c r="F35" s="19"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
@@ -5313,25 +5313,25 @@
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
       <c r="P35" s="21"/>
-      <c r="Q35" s="161"/>
-      <c r="R35" s="162"/>
+      <c r="Q35" s="148"/>
+      <c r="R35" s="149"/>
       <c r="S35" s="22"/>
       <c r="T35" s="22"/>
       <c r="U35" s="22"/>
       <c r="V35" s="22"/>
       <c r="W35" s="22"/>
-      <c r="X35" s="213"/>
-      <c r="Y35" s="164"/>
-      <c r="Z35" s="164"/>
-      <c r="AA35" s="165"/>
+      <c r="X35" s="135"/>
+      <c r="Y35" s="136"/>
+      <c r="Z35" s="136"/>
+      <c r="AA35" s="137"/>
       <c r="AB35" s="23"/>
     </row>
     <row r="36" spans="1:29" ht="18.75" customHeight="1">
       <c r="A36" s="26"/>
       <c r="B36" s="18"/>
-      <c r="C36" s="212"/>
-      <c r="D36" s="164"/>
-      <c r="E36" s="165"/>
+      <c r="C36" s="155"/>
+      <c r="D36" s="136"/>
+      <c r="E36" s="137"/>
       <c r="F36" s="19"/>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
@@ -5343,17 +5343,17 @@
       <c r="N36" s="21"/>
       <c r="O36" s="21"/>
       <c r="P36" s="21"/>
-      <c r="Q36" s="161"/>
-      <c r="R36" s="162"/>
+      <c r="Q36" s="148"/>
+      <c r="R36" s="149"/>
       <c r="S36" s="22"/>
       <c r="T36" s="22"/>
       <c r="U36" s="22"/>
       <c r="V36" s="22"/>
       <c r="W36" s="22"/>
-      <c r="X36" s="213"/>
-      <c r="Y36" s="164"/>
-      <c r="Z36" s="164"/>
-      <c r="AA36" s="165"/>
+      <c r="X36" s="135"/>
+      <c r="Y36" s="136"/>
+      <c r="Z36" s="136"/>
+      <c r="AA36" s="137"/>
       <c r="AB36" s="23"/>
       <c r="AC36" s="41"/>
     </row>
@@ -5381,10 +5381,10 @@
       <c r="U37" s="29"/>
       <c r="V37" s="29"/>
       <c r="W37" s="29"/>
-      <c r="X37" s="217"/>
-      <c r="Y37" s="177"/>
-      <c r="Z37" s="177"/>
-      <c r="AA37" s="177"/>
+      <c r="X37" s="147"/>
+      <c r="Y37" s="146"/>
+      <c r="Z37" s="146"/>
+      <c r="AA37" s="146"/>
       <c r="AB37" s="30"/>
     </row>
     <row r="38" spans="1:29" ht="24.75" customHeight="1">
@@ -5411,10 +5411,10 @@
       <c r="U38" s="29"/>
       <c r="V38" s="29"/>
       <c r="W38" s="29"/>
-      <c r="X38" s="217"/>
-      <c r="Y38" s="177"/>
-      <c r="Z38" s="177"/>
-      <c r="AA38" s="177"/>
+      <c r="X38" s="147"/>
+      <c r="Y38" s="146"/>
+      <c r="Z38" s="146"/>
+      <c r="AA38" s="146"/>
       <c r="AB38" s="30"/>
     </row>
     <row r="39" spans="1:29" ht="24.75" customHeight="1">
@@ -5432,10 +5432,10 @@
       <c r="J39" s="17"/>
       <c r="O39" s="38"/>
       <c r="P39" s="38"/>
-      <c r="X39" s="216"/>
-      <c r="Y39" s="177"/>
-      <c r="Z39" s="177"/>
-      <c r="AA39" s="177"/>
+      <c r="X39" s="145"/>
+      <c r="Y39" s="146"/>
+      <c r="Z39" s="146"/>
+      <c r="AA39" s="146"/>
       <c r="AB39" s="26"/>
     </row>
     <row r="40" spans="1:29" ht="39.75" customHeight="1">
@@ -5545,34 +5545,34 @@
     </row>
     <row r="44" spans="1:29" s="85" customFormat="1" ht="37.15" customHeight="1">
       <c r="B44" s="27"/>
-      <c r="C44" s="214" t="s">
+      <c r="C44" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="214"/>
-      <c r="E44" s="214"/>
-      <c r="F44" s="214"/>
-      <c r="G44" s="214"/>
-      <c r="H44" s="214"/>
-      <c r="I44" s="214"/>
-      <c r="J44" s="214"/>
-      <c r="K44" s="214"/>
-      <c r="L44" s="214"/>
-      <c r="M44" s="214"/>
-      <c r="N44" s="214"/>
-      <c r="O44" s="214"/>
-      <c r="P44" s="214"/>
-      <c r="Q44" s="214"/>
-      <c r="R44" s="214"/>
-      <c r="S44" s="214"/>
-      <c r="T44" s="214"/>
-      <c r="U44" s="214"/>
-      <c r="V44" s="214"/>
-      <c r="W44" s="214"/>
-      <c r="X44" s="214"/>
-      <c r="Y44" s="214"/>
-      <c r="Z44" s="214"/>
-      <c r="AA44" s="214"/>
-      <c r="AB44" s="215"/>
+      <c r="D44" s="138"/>
+      <c r="E44" s="138"/>
+      <c r="F44" s="138"/>
+      <c r="G44" s="138"/>
+      <c r="H44" s="138"/>
+      <c r="I44" s="138"/>
+      <c r="J44" s="138"/>
+      <c r="K44" s="138"/>
+      <c r="L44" s="138"/>
+      <c r="M44" s="138"/>
+      <c r="N44" s="138"/>
+      <c r="O44" s="138"/>
+      <c r="P44" s="138"/>
+      <c r="Q44" s="138"/>
+      <c r="R44" s="138"/>
+      <c r="S44" s="138"/>
+      <c r="T44" s="138"/>
+      <c r="U44" s="138"/>
+      <c r="V44" s="138"/>
+      <c r="W44" s="138"/>
+      <c r="X44" s="138"/>
+      <c r="Y44" s="138"/>
+      <c r="Z44" s="138"/>
+      <c r="AA44" s="138"/>
+      <c r="AB44" s="139"/>
     </row>
     <row r="45" spans="1:29" ht="69.599999999999994" customHeight="1" thickBot="1">
       <c r="B45" s="48"/>
@@ -5649,14 +5649,14 @@
       <c r="C50" s="53"/>
     </row>
     <row r="51" spans="1:17" ht="12" customHeight="1">
-      <c r="B51" s="209" t="s">
+      <c r="B51" s="150" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="209"/>
-      <c r="D51" s="209"/>
-      <c r="E51" s="209"/>
-      <c r="F51" s="209"/>
-      <c r="G51" s="209"/>
+      <c r="C51" s="150"/>
+      <c r="D51" s="150"/>
+      <c r="E51" s="150"/>
+      <c r="F51" s="150"/>
+      <c r="G51" s="150"/>
       <c r="J51" s="17"/>
       <c r="K51" s="55" t="s">
         <v>32</v>
@@ -5677,17 +5677,17 @@
       </c>
       <c r="D54" s="59"/>
       <c r="E54" s="59"/>
-      <c r="F54" s="210"/>
-      <c r="G54" s="184"/>
-      <c r="H54" s="184"/>
+      <c r="F54" s="140"/>
+      <c r="G54" s="141"/>
+      <c r="H54" s="141"/>
       <c r="J54" s="60"/>
       <c r="K54" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="N54" s="210"/>
-      <c r="O54" s="184"/>
-      <c r="P54" s="184"/>
-      <c r="Q54" s="184"/>
+      <c r="N54" s="140"/>
+      <c r="O54" s="141"/>
+      <c r="P54" s="141"/>
+      <c r="Q54" s="141"/>
     </row>
     <row r="55" spans="1:17" ht="12" customHeight="1">
       <c r="A55" s="1"/>
@@ -35856,6 +35856,75 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="X25:AA25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="X26:AA26"/>
+    <mergeCell ref="X27:AA27"/>
+    <mergeCell ref="X28:AA28"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="Y22:AB22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="X23:AA23"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="X24:AA24"/>
+    <mergeCell ref="B13:AB13"/>
+    <mergeCell ref="B15:AB15"/>
+    <mergeCell ref="B16:AB16"/>
+    <mergeCell ref="B17:AB17"/>
+    <mergeCell ref="G19:N20"/>
+    <mergeCell ref="X19:AA21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="B18:AB18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="O19:W20"/>
+    <mergeCell ref="B7:AB7"/>
+    <mergeCell ref="B8:AB8"/>
+    <mergeCell ref="B10:AB10"/>
+    <mergeCell ref="B11:AB11"/>
+    <mergeCell ref="B12:AB12"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="B6:AB6"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="G2:Q2"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="G3:Q3"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
     <mergeCell ref="X36:AA36"/>
     <mergeCell ref="C44:AB44"/>
     <mergeCell ref="N54:Q54"/>
@@ -35872,75 +35941,6 @@
     <mergeCell ref="Q34:R34"/>
     <mergeCell ref="Q35:R35"/>
     <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="G3:Q3"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="B6:AB6"/>
-    <mergeCell ref="B7:AB7"/>
-    <mergeCell ref="B8:AB8"/>
-    <mergeCell ref="B10:AB10"/>
-    <mergeCell ref="B11:AB11"/>
-    <mergeCell ref="B12:AB12"/>
-    <mergeCell ref="X24:AA24"/>
-    <mergeCell ref="B13:AB13"/>
-    <mergeCell ref="B15:AB15"/>
-    <mergeCell ref="B16:AB16"/>
-    <mergeCell ref="B17:AB17"/>
-    <mergeCell ref="G19:N20"/>
-    <mergeCell ref="X19:AA21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="B18:AB18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="O19:W20"/>
-    <mergeCell ref="Y22:AB22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="X23:AA23"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="X25:AA25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="X29:AA29"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="X26:AA26"/>
-    <mergeCell ref="X27:AA27"/>
-    <mergeCell ref="X28:AA28"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
   </mergeCells>
   <conditionalFormatting sqref="F53:G54">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
@@ -35969,8 +35969,8 @@
   </sheetPr>
   <dimension ref="A2:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -35988,52 +35988,52 @@
       <c r="A2" s="218" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="181"/>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="181"/>
-      <c r="F2" s="181"/>
-      <c r="G2" s="181"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
       <c r="H2" s="219"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="220"/>
-      <c r="B3" s="177"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="177"/>
-      <c r="F3" s="177"/>
-      <c r="G3" s="177"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="146"/>
+      <c r="F3" s="146"/>
+      <c r="G3" s="146"/>
       <c r="H3" s="221"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="220"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
       <c r="H4" s="221"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="220"/>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="177"/>
-      <c r="E5" s="177"/>
-      <c r="F5" s="177"/>
-      <c r="G5" s="177"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
       <c r="H5" s="221"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="220"/>
-      <c r="B6" s="177"/>
-      <c r="C6" s="177"/>
-      <c r="D6" s="177"/>
-      <c r="E6" s="177"/>
-      <c r="F6" s="177"/>
-      <c r="G6" s="177"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="146"/>
       <c r="H6" s="221"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
@@ -37664,14 +37664,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EDB39E34F5A9B445B025C05B2A05D030" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c21ef800502b5dc1190a9a0361733939">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f1f31ffb-9912-4459-99c8-b26e82094b51" xmlns:ns4="ce621958-37b1-43fe-a1f1-1aad67996a88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30daf50bb6192471b76b9808b4256f50" ns3:_="" ns4:_="">
     <xsd:import namespace="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
@@ -37866,6 +37858,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -37876,23 +37876,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D01A9D5D-1824-48C2-8527-9D8749A8DDDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37911,6 +37894,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0679DBA9-5627-44A3-91B7-DABD2A2D7C98}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96490F3C-DFF7-4107-BF06-5DD550949EBD}">
   <ds:schemaRefs>

</xml_diff>